<commit_message>
completed KTKT BOW 1,1 and 1,2
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5217C8A-4B75-4432-9654-A34FBA2175FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995722AE-EF03-45A8-9244-8D69F76AB3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="308">
   <si>
     <t>TRAINING</t>
   </si>
@@ -96,6 +96,867 @@
   </si>
   <si>
     <t>one seed only</t>
+  </si>
+  <si>
+    <t>0.7336±0.0021</t>
+  </si>
+  <si>
+    <t>0.6925±0.0074</t>
+  </si>
+  <si>
+    <t>0.5753±0.0073</t>
+  </si>
+  <si>
+    <t>0.4504±0.0055</t>
+  </si>
+  <si>
+    <t>0.8094±0.0024</t>
+  </si>
+  <si>
+    <t>0.6284±0.0035</t>
+  </si>
+  <si>
+    <t>0.7309±0.0025</t>
+  </si>
+  <si>
+    <t>0.6766±0.0047</t>
+  </si>
+  <si>
+    <t>0.5895±0.0038</t>
+  </si>
+  <si>
+    <t>0.4513±0.0054</t>
+  </si>
+  <si>
+    <t>0.806±0.002</t>
+  </si>
+  <si>
+    <t>0.6301±0.0037</t>
+  </si>
+  <si>
+    <t>0.7149±0.0026</t>
+  </si>
+  <si>
+    <t>0.6514±0.0046</t>
+  </si>
+  <si>
+    <t>0.5582±0.0046</t>
+  </si>
+  <si>
+    <t>0.4117±0.0062</t>
+  </si>
+  <si>
+    <t>0.8037±0.0036</t>
+  </si>
+  <si>
+    <t>0.6012±0.0043</t>
+  </si>
+  <si>
+    <t>0.7102±0.0024</t>
+  </si>
+  <si>
+    <t>0.6371±0.0051</t>
+  </si>
+  <si>
+    <t>0.569±0.0031</t>
+  </si>
+  <si>
+    <t>0.4107±0.0048</t>
+  </si>
+  <si>
+    <t>0.7968±0.0029</t>
+  </si>
+  <si>
+    <t>0.6011±0.0036</t>
+  </si>
+  <si>
+    <t>0.7105±0.0026</t>
+  </si>
+  <si>
+    <t>0.7116±0.0081</t>
+  </si>
+  <si>
+    <t>0.5025±0.0043</t>
+  </si>
+  <si>
+    <t>0.3826±0.0072</t>
+  </si>
+  <si>
+    <t>0.8066±0.0021</t>
+  </si>
+  <si>
+    <t>0.5891±0.0051</t>
+  </si>
+  <si>
+    <t>0.7411±0.0028</t>
+  </si>
+  <si>
+    <t>0.7118±0.0052</t>
+  </si>
+  <si>
+    <t>0.5859±0.0049</t>
+  </si>
+  <si>
+    <t>0.4667±0.0067</t>
+  </si>
+  <si>
+    <t>0.8401±0.0023</t>
+  </si>
+  <si>
+    <t>0.6427±0.0045</t>
+  </si>
+  <si>
+    <t>0.7101±0.003</t>
+  </si>
+  <si>
+    <t>0.6329±0.0049</t>
+  </si>
+  <si>
+    <t>0.6101±0.0066</t>
+  </si>
+  <si>
+    <t>0.4373±0.0063</t>
+  </si>
+  <si>
+    <t>0.8058±0.0037</t>
+  </si>
+  <si>
+    <t>0.6213±0.0044</t>
+  </si>
+  <si>
+    <t>0.7169±0.0033</t>
+  </si>
+  <si>
+    <t>0.6455±0.0049</t>
+  </si>
+  <si>
+    <t>0.6017±0.0057</t>
+  </si>
+  <si>
+    <t>0.4385±0.0074</t>
+  </si>
+  <si>
+    <t>0.8138±0.0023</t>
+  </si>
+  <si>
+    <t>0.6228±0.0052</t>
+  </si>
+  <si>
+    <t>0.6093±0.0078</t>
+  </si>
+  <si>
+    <t>0.4883±0.0093</t>
+  </si>
+  <si>
+    <t>0.4761±0.0067</t>
+  </si>
+  <si>
+    <t>0.2374±0.0103</t>
+  </si>
+  <si>
+    <t>0.607±0.005</t>
+  </si>
+  <si>
+    <t>0.4821±0.0077</t>
+  </si>
+  <si>
+    <t>0.6317±0.005</t>
+  </si>
+  <si>
+    <t>0.5329±0.006</t>
+  </si>
+  <si>
+    <t>0.5296±0.0081</t>
+  </si>
+  <si>
+    <t>0.3021±0.011</t>
+  </si>
+  <si>
+    <t>0.6562±0.0052</t>
+  </si>
+  <si>
+    <t>0.5313±0.007</t>
+  </si>
+  <si>
+    <t>0.7345±0.0032</t>
+  </si>
+  <si>
+    <t>0.683±0.0053</t>
+  </si>
+  <si>
+    <t>0.5946±0.0042</t>
+  </si>
+  <si>
+    <t>0.4591±0.0067</t>
+  </si>
+  <si>
+    <t>0.8265±0.0022</t>
+  </si>
+  <si>
+    <t>0.6357±0.0044</t>
+  </si>
+  <si>
+    <t>0.7042±0.0042</t>
+  </si>
+  <si>
+    <t>0.6993±0.0061</t>
+  </si>
+  <si>
+    <t>0.4947±0.0079</t>
+  </si>
+  <si>
+    <t>0.3653±0.0118</t>
+  </si>
+  <si>
+    <t>0.8219±0.0018</t>
+  </si>
+  <si>
+    <t>0.5795±0.007</t>
+  </si>
+  <si>
+    <t>0.7385±0.0027</t>
+  </si>
+  <si>
+    <t>0.7021±0.0052</t>
+  </si>
+  <si>
+    <t>0.5812±0.0098</t>
+  </si>
+  <si>
+    <t>0.4612±0.0076</t>
+  </si>
+  <si>
+    <t>0.8177±0.0025</t>
+  </si>
+  <si>
+    <t>0.6359±0.0055</t>
+  </si>
+  <si>
+    <t>0.7296±0.0022</t>
+  </si>
+  <si>
+    <t>0.6655±0.0038</t>
+  </si>
+  <si>
+    <t>0.6067±0.0029</t>
+  </si>
+  <si>
+    <t>0.4587±0.0041</t>
+  </si>
+  <si>
+    <t>0.7978±0.0024</t>
+  </si>
+  <si>
+    <t>0.6347±0.0028</t>
+  </si>
+  <si>
+    <t>0.7222±0.0031</t>
+  </si>
+  <si>
+    <t>0.6665±0.0059</t>
+  </si>
+  <si>
+    <t>0.5673±0.005</t>
+  </si>
+  <si>
+    <t>0.4275±0.0071</t>
+  </si>
+  <si>
+    <t>0.8093±0.0033</t>
+  </si>
+  <si>
+    <t>0.6129±0.0049</t>
+  </si>
+  <si>
+    <t>0.7158±0.0034</t>
+  </si>
+  <si>
+    <t>0.647±0.0054</t>
+  </si>
+  <si>
+    <t>0.5759±0.0044</t>
+  </si>
+  <si>
+    <t>0.4224±0.0072</t>
+  </si>
+  <si>
+    <t>0.8056±0.0033</t>
+  </si>
+  <si>
+    <t>0.6094±0.0043</t>
+  </si>
+  <si>
+    <t>0.7109±0.0016</t>
+  </si>
+  <si>
+    <t>0.719±0.0056</t>
+  </si>
+  <si>
+    <t>0.5012±0.0037</t>
+  </si>
+  <si>
+    <t>0.3838±0.0044</t>
+  </si>
+  <si>
+    <t>0.8091±0.0029</t>
+  </si>
+  <si>
+    <t>0.5906±0.0037</t>
+  </si>
+  <si>
+    <t>0.7419±0.0024</t>
+  </si>
+  <si>
+    <t>0.7156±0.0048</t>
+  </si>
+  <si>
+    <t>0.5837±0.0033</t>
+  </si>
+  <si>
+    <t>0.4679±0.0055</t>
+  </si>
+  <si>
+    <t>0.8444±0.0022</t>
+  </si>
+  <si>
+    <t>0.6429±0.0032</t>
+  </si>
+  <si>
+    <t>0.7203±0.0056</t>
+  </si>
+  <si>
+    <t>0.6481±0.008</t>
+  </si>
+  <si>
+    <t>0.6201±0.0051</t>
+  </si>
+  <si>
+    <t>0.4549±0.0086</t>
+  </si>
+  <si>
+    <t>0.8158±0.0029</t>
+  </si>
+  <si>
+    <t>0.6338±0.0057</t>
+  </si>
+  <si>
+    <t>0.7227±0.0028</t>
+  </si>
+  <si>
+    <t>0.655±0.0045</t>
+  </si>
+  <si>
+    <t>0.6077±0.0031</t>
+  </si>
+  <si>
+    <t>0.4493±0.0051</t>
+  </si>
+  <si>
+    <t>0.8181±0.0038</t>
+  </si>
+  <si>
+    <t>0.6304±0.0035</t>
+  </si>
+  <si>
+    <t>0.6164±0.0057</t>
+  </si>
+  <si>
+    <t>0.4958±0.0057</t>
+  </si>
+  <si>
+    <t>0.4812±0.0045</t>
+  </si>
+  <si>
+    <t>0.2478±0.0079</t>
+  </si>
+  <si>
+    <t>0.6109±0.0034</t>
+  </si>
+  <si>
+    <t>0.4884±0.0047</t>
+  </si>
+  <si>
+    <t>0.6378±0.0028</t>
+  </si>
+  <si>
+    <t>0.5392±0.0026</t>
+  </si>
+  <si>
+    <t>0.5349±0.0041</t>
+  </si>
+  <si>
+    <t>0.3121±0.0058</t>
+  </si>
+  <si>
+    <t>0.6601±0.0027</t>
+  </si>
+  <si>
+    <t>0.5371±0.0032</t>
+  </si>
+  <si>
+    <t>0.7381±0.0021</t>
+  </si>
+  <si>
+    <t>0.6899±0.0038</t>
+  </si>
+  <si>
+    <t>0.5968±0.0035</t>
+  </si>
+  <si>
+    <t>0.4661±0.0047</t>
+  </si>
+  <si>
+    <t>0.834±0.0035</t>
+  </si>
+  <si>
+    <t>0.64±0.0032</t>
+  </si>
+  <si>
+    <t>0.7049±0.0022</t>
+  </si>
+  <si>
+    <t>0.7073±0.0065</t>
+  </si>
+  <si>
+    <t>0.4929±0.003</t>
+  </si>
+  <si>
+    <t>0.367±0.0062</t>
+  </si>
+  <si>
+    <t>0.8243±0.0032</t>
+  </si>
+  <si>
+    <t>0.581±0.004</t>
+  </si>
+  <si>
+    <t>0.7304±0.0026</t>
+  </si>
+  <si>
+    <t>0.688±0.0085</t>
+  </si>
+  <si>
+    <t>0.5652±0.0068</t>
+  </si>
+  <si>
+    <t>0.4412±0.0063</t>
+  </si>
+  <si>
+    <t>0.8048±0.0018</t>
+  </si>
+  <si>
+    <t>0.6205±0.0045</t>
+  </si>
+  <si>
+    <t>0.7271±0.003</t>
+  </si>
+  <si>
+    <t>0.6756±0.0059</t>
+  </si>
+  <si>
+    <t>0.5733±0.0095</t>
+  </si>
+  <si>
+    <t>0.4383±0.0074</t>
+  </si>
+  <si>
+    <t>0.7971±0.0041</t>
+  </si>
+  <si>
+    <t>0.6202±0.0052</t>
+  </si>
+  <si>
+    <t>0.713±0.0032</t>
+  </si>
+  <si>
+    <t>0.6489±0.0061</t>
+  </si>
+  <si>
+    <t>0.5535±0.0058</t>
+  </si>
+  <si>
+    <t>0.4061±0.0077</t>
+  </si>
+  <si>
+    <t>0.8009±0.0038</t>
+  </si>
+  <si>
+    <t>0.5974±0.0057</t>
+  </si>
+  <si>
+    <t>0.7085±0.0032</t>
+  </si>
+  <si>
+    <t>0.6357±0.0062</t>
+  </si>
+  <si>
+    <t>0.5639±0.0035</t>
+  </si>
+  <si>
+    <t>0.4053±0.0063</t>
+  </si>
+  <si>
+    <t>0.7941±0.0038</t>
+  </si>
+  <si>
+    <t>0.5976±0.0044</t>
+  </si>
+  <si>
+    <t>0.7095±0.0021</t>
+  </si>
+  <si>
+    <t>0.7088±0.0072</t>
+  </si>
+  <si>
+    <t>0.5006±0.0032</t>
+  </si>
+  <si>
+    <t>0.3799±0.0058</t>
+  </si>
+  <si>
+    <t>0.8045±0.0024</t>
+  </si>
+  <si>
+    <t>0.5868±0.0041</t>
+  </si>
+  <si>
+    <t>0.7381±0.0028</t>
+  </si>
+  <si>
+    <t>0.705±0.0033</t>
+  </si>
+  <si>
+    <t>0.5807±0.0053</t>
+  </si>
+  <si>
+    <t>0.4597±0.007</t>
+  </si>
+  <si>
+    <t>0.8364±0.0021</t>
+  </si>
+  <si>
+    <t>0.6369±0.0042</t>
+  </si>
+  <si>
+    <t>0.7148±0.005</t>
+  </si>
+  <si>
+    <t>0.6404±0.0079</t>
+  </si>
+  <si>
+    <t>0.6046±0.0054</t>
+  </si>
+  <si>
+    <t>0.4389±0.0083</t>
+  </si>
+  <si>
+    <t>0.8017±0.0047</t>
+  </si>
+  <si>
+    <t>0.6219±0.0051</t>
+  </si>
+  <si>
+    <t>0.7134±0.003</t>
+  </si>
+  <si>
+    <t>0.654±0.0051</t>
+  </si>
+  <si>
+    <t>0.5564±0.0053</t>
+  </si>
+  <si>
+    <t>0.4072±0.0073</t>
+  </si>
+  <si>
+    <t>0.8028±0.0025</t>
+  </si>
+  <si>
+    <t>0.6013±0.0051</t>
+  </si>
+  <si>
+    <t>0.6061±0.0053</t>
+  </si>
+  <si>
+    <t>0.4827±0.0052</t>
+  </si>
+  <si>
+    <t>0.4707±0.0037</t>
+  </si>
+  <si>
+    <t>0.2302±0.007</t>
+  </si>
+  <si>
+    <t>0.603±0.0028</t>
+  </si>
+  <si>
+    <t>0.4766±0.0043</t>
+  </si>
+  <si>
+    <t>0.6292±0.0032</t>
+  </si>
+  <si>
+    <t>0.5289±0.0043</t>
+  </si>
+  <si>
+    <t>0.5268±0.0052</t>
+  </si>
+  <si>
+    <t>0.2987±0.0065</t>
+  </si>
+  <si>
+    <t>0.6537±0.0029</t>
+  </si>
+  <si>
+    <t>0.5278±0.0047</t>
+  </si>
+  <si>
+    <t>0.7282±0.0033</t>
+  </si>
+  <si>
+    <t>0.6768±0.0052</t>
+  </si>
+  <si>
+    <t>0.5761±0.008</t>
+  </si>
+  <si>
+    <t>0.4411±0.0084</t>
+  </si>
+  <si>
+    <t>0.8213±0.0024</t>
+  </si>
+  <si>
+    <t>0.6224±0.0053</t>
+  </si>
+  <si>
+    <t>0.7133±0.0033</t>
+  </si>
+  <si>
+    <t>0.6964±0.0036</t>
+  </si>
+  <si>
+    <t>0.5157±0.0063</t>
+  </si>
+  <si>
+    <t>0.3912±0.0089</t>
+  </si>
+  <si>
+    <t>0.8185±0.0016</t>
+  </si>
+  <si>
+    <t>0.5926±0.005</t>
+  </si>
+  <si>
+    <t>0.7347±0.0026</t>
+  </si>
+  <si>
+    <t>0.6975±0.0092</t>
+  </si>
+  <si>
+    <t>0.572±0.006</t>
+  </si>
+  <si>
+    <t>0.4515±0.0054</t>
+  </si>
+  <si>
+    <t>0.8124±0.004</t>
+  </si>
+  <si>
+    <t>0.6285±0.0033</t>
+  </si>
+  <si>
+    <t>0.7293±0.0022</t>
+  </si>
+  <si>
+    <t>0.6749±0.0036</t>
+  </si>
+  <si>
+    <t>0.5802±0.0035</t>
+  </si>
+  <si>
+    <t>0.4451±0.005</t>
+  </si>
+  <si>
+    <t>0.7917±0.0025</t>
+  </si>
+  <si>
+    <t>0.624±0.0032</t>
+  </si>
+  <si>
+    <t>0.7198±0.0035</t>
+  </si>
+  <si>
+    <t>0.6627±0.007</t>
+  </si>
+  <si>
+    <t>0.5618±0.005</t>
+  </si>
+  <si>
+    <t>0.4209±0.0079</t>
+  </si>
+  <si>
+    <t>0.8064±0.003</t>
+  </si>
+  <si>
+    <t>0.6081±0.0054</t>
+  </si>
+  <si>
+    <t>0.7153±0.0037</t>
+  </si>
+  <si>
+    <t>0.6471±0.0066</t>
+  </si>
+  <si>
+    <t>0.5717±0.005</t>
+  </si>
+  <si>
+    <t>0.4194±0.008</t>
+  </si>
+  <si>
+    <t>0.8031±0.0028</t>
+  </si>
+  <si>
+    <t>0.607±0.0054</t>
+  </si>
+  <si>
+    <t>0.7095±0.0012</t>
+  </si>
+  <si>
+    <t>0.7141±0.0065</t>
+  </si>
+  <si>
+    <t>0.4988±0.0019</t>
+  </si>
+  <si>
+    <t>0.3798±0.0035</t>
+  </si>
+  <si>
+    <t>0.807±0.0034</t>
+  </si>
+  <si>
+    <t>0.5874±0.0027</t>
+  </si>
+  <si>
+    <t>0.7388±0.0023</t>
+  </si>
+  <si>
+    <t>0.7101±0.0049</t>
+  </si>
+  <si>
+    <t>0.5786±0.0035</t>
+  </si>
+  <si>
+    <t>0.4605±0.0053</t>
+  </si>
+  <si>
+    <t>0.8404±0.0025</t>
+  </si>
+  <si>
+    <t>0.6376±0.0036</t>
+  </si>
+  <si>
+    <t>0.7201±0.0036</t>
+  </si>
+  <si>
+    <t>0.6479±0.0057</t>
+  </si>
+  <si>
+    <t>0.6127±0.0062</t>
+  </si>
+  <si>
+    <t>0.45±0.0064</t>
+  </si>
+  <si>
+    <t>0.8099±0.005</t>
+  </si>
+  <si>
+    <t>0.6298±0.004</t>
+  </si>
+  <si>
+    <t>0.7182±0.002</t>
+  </si>
+  <si>
+    <t>0.6649±0.0047</t>
+  </si>
+  <si>
+    <t>0.5609±0.0032</t>
+  </si>
+  <si>
+    <t>0.4171±0.0048</t>
+  </si>
+  <si>
+    <t>0.8053±0.0033</t>
+  </si>
+  <si>
+    <t>0.6085±0.0032</t>
+  </si>
+  <si>
+    <t>0.6131±0.0062</t>
+  </si>
+  <si>
+    <t>0.4906±0.0074</t>
+  </si>
+  <si>
+    <t>0.476±0.0057</t>
+  </si>
+  <si>
+    <t>0.2403±0.0103</t>
+  </si>
+  <si>
+    <t>0.607±0.0043</t>
+  </si>
+  <si>
+    <t>0.4832±0.0064</t>
+  </si>
+  <si>
+    <t>0.6369±0.0024</t>
+  </si>
+  <si>
+    <t>0.538±0.0024</t>
+  </si>
+  <si>
+    <t>0.5349±0.0025</t>
+  </si>
+  <si>
+    <t>0.3123±0.0025</t>
+  </si>
+  <si>
+    <t>0.6598±0.0019</t>
+  </si>
+  <si>
+    <t>0.5365±0.002</t>
+  </si>
+  <si>
+    <t>0.7298±0.002</t>
+  </si>
+  <si>
+    <t>0.6821±0.0051</t>
+  </si>
+  <si>
+    <t>0.5751±0.0039</t>
+  </si>
+  <si>
+    <t>0.4435±0.0044</t>
+  </si>
+  <si>
+    <t>0.8269±0.0036</t>
+  </si>
+  <si>
+    <t>0.7142±0.0018</t>
+  </si>
+  <si>
+    <t>0.7035±0.0052</t>
+  </si>
+  <si>
+    <t>0.5141±0.0026</t>
+  </si>
+  <si>
+    <t>0.3931±0.0047</t>
+  </si>
+  <si>
+    <t>0.8207±0.003</t>
+  </si>
+  <si>
+    <t>0.594±0.0029</t>
   </si>
 </sst>
 </file>
@@ -500,7 +1361,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,9 +1373,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -524,9 +1383,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -576,504 +1433,504 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.727113848202396</v>
-      </c>
-      <c r="C3">
-        <v>0.66807702137932801</v>
-      </c>
-      <c r="D3">
-        <v>0.57062133360081502</v>
-      </c>
-      <c r="E3">
-        <v>0.43830173248870402</v>
-      </c>
-      <c r="F3">
-        <v>0.81674690025732399</v>
-      </c>
-      <c r="G3">
-        <v>0.615515471308822</v>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" t="s">
+        <v>170</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.730548389781143</v>
-      </c>
-      <c r="J3">
-        <v>0.68133907685610795</v>
-      </c>
-      <c r="K3">
-        <v>0.57885114650644998</v>
-      </c>
-      <c r="L3">
-        <v>0.44623303160826799</v>
-      </c>
-      <c r="M3">
-        <v>0.82027199874463197</v>
-      </c>
-      <c r="N3">
-        <v>0.625927575831283</v>
+      <c r="I3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>240</v>
+      </c>
+      <c r="M3" t="s">
+        <v>241</v>
+      </c>
+      <c r="N3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.72669773635153101</v>
-      </c>
-      <c r="C4">
-        <v>0.68007281428656297</v>
-      </c>
-      <c r="D4">
-        <v>0.55868794410126699</v>
-      </c>
-      <c r="E4">
-        <v>0.43212931232212198</v>
-      </c>
-      <c r="F4">
-        <v>0.81907047203292005</v>
-      </c>
-      <c r="G4">
-        <v>0.61343319100195204</v>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>176</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.73229591412166095</v>
-      </c>
-      <c r="J4">
-        <v>0.68148735013522499</v>
-      </c>
-      <c r="K4">
-        <v>0.58577657184556398</v>
-      </c>
-      <c r="L4">
-        <v>0.45208837287285802</v>
-      </c>
-      <c r="M4">
-        <v>0.81584783427344199</v>
-      </c>
-      <c r="N4">
-        <v>0.63001765740219895</v>
+      <c r="I4" t="s">
+        <v>243</v>
+      </c>
+      <c r="J4" t="s">
+        <v>244</v>
+      </c>
+      <c r="K4" t="s">
+        <v>245</v>
+      </c>
+      <c r="L4" t="s">
+        <v>246</v>
+      </c>
+      <c r="M4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.71488015978694996</v>
-      </c>
-      <c r="C5">
-        <v>0.65093403663756999</v>
-      </c>
-      <c r="D5">
-        <v>0.55384457870643</v>
-      </c>
-      <c r="E5">
-        <v>0.40973708499704498</v>
-      </c>
-      <c r="F5">
-        <v>0.80140812754858004</v>
-      </c>
-      <c r="G5">
-        <v>0.598477235063261</v>
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" t="s">
+        <v>182</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.71690105683614802</v>
-      </c>
-      <c r="J5">
-        <v>0.65414430943475799</v>
-      </c>
-      <c r="K5">
-        <v>0.55897344518638203</v>
-      </c>
-      <c r="L5">
-        <v>0.41550559246402902</v>
-      </c>
-      <c r="M5">
-        <v>0.80684043176165399</v>
-      </c>
-      <c r="N5">
-        <v>0.60282573047990096</v>
+      <c r="I5" t="s">
+        <v>249</v>
+      </c>
+      <c r="J5" t="s">
+        <v>250</v>
+      </c>
+      <c r="K5" t="s">
+        <v>251</v>
+      </c>
+      <c r="L5" t="s">
+        <v>252</v>
+      </c>
+      <c r="M5" t="s">
+        <v>253</v>
+      </c>
+      <c r="N5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.70872170439414095</v>
-      </c>
-      <c r="C6">
-        <v>0.63646829758841805</v>
-      </c>
-      <c r="D6">
-        <v>0.56228501373211504</v>
-      </c>
-      <c r="E6">
-        <v>0.40450458857523502</v>
-      </c>
-      <c r="F6">
-        <v>0.794828718759927</v>
-      </c>
-      <c r="G6">
-        <v>0.59708128781780201</v>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" t="s">
+        <v>188</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.71049346758758403</v>
-      </c>
-      <c r="J6">
-        <v>0.63674134522484505</v>
-      </c>
-      <c r="K6">
-        <v>0.56463848519002402</v>
-      </c>
-      <c r="L6">
-        <v>0.409231841104024</v>
-      </c>
-      <c r="M6">
-        <v>0.80173477290939399</v>
-      </c>
-      <c r="N6">
-        <v>0.59852622713244596</v>
+      <c r="I6" t="s">
+        <v>255</v>
+      </c>
+      <c r="J6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L6" t="s">
+        <v>258</v>
+      </c>
+      <c r="M6" t="s">
+        <v>259</v>
+      </c>
+      <c r="N6" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.70947070572569904</v>
-      </c>
-      <c r="C7">
-        <v>0.70333882929118696</v>
-      </c>
-      <c r="D7">
-        <v>0.50122495628931596</v>
-      </c>
-      <c r="E7">
-        <v>0.37972758999832801</v>
-      </c>
-      <c r="F7">
-        <v>0.80727547850570802</v>
-      </c>
-      <c r="G7">
-        <v>0.58532553973165002</v>
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" t="s">
+        <v>194</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.71024382125322405</v>
-      </c>
-      <c r="J7">
-        <v>0.72187294316489303</v>
-      </c>
-      <c r="K7">
-        <v>0.50068020831661197</v>
-      </c>
-      <c r="L7">
-        <v>0.38207811552668403</v>
-      </c>
-      <c r="M7">
-        <v>0.80623665209518103</v>
-      </c>
-      <c r="N7">
-        <v>0.59126671936339503</v>
+      <c r="I7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J7" t="s">
+        <v>262</v>
+      </c>
+      <c r="K7" t="s">
+        <v>263</v>
+      </c>
+      <c r="L7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M7" t="s">
+        <v>265</v>
+      </c>
+      <c r="N7" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.73851531291611106</v>
-      </c>
-      <c r="C8">
-        <v>0.70287367794824696</v>
-      </c>
-      <c r="D8">
-        <v>0.57794653013372499</v>
-      </c>
-      <c r="E8">
-        <v>0.46026609310432698</v>
-      </c>
-      <c r="F8">
-        <v>0.837366427786153</v>
-      </c>
-      <c r="G8">
-        <v>0.63431760481174504</v>
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" t="s">
+        <v>200</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.74203212116168704</v>
-      </c>
-      <c r="J8">
-        <v>0.71578994629525905</v>
-      </c>
-      <c r="K8">
-        <v>0.58396919226601596</v>
-      </c>
-      <c r="L8">
-        <v>0.468311113937392</v>
-      </c>
-      <c r="M8">
-        <v>0.83899206321743403</v>
-      </c>
-      <c r="N8">
-        <v>0.64319498031438005</v>
+      <c r="I8" t="s">
+        <v>267</v>
+      </c>
+      <c r="J8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K8" t="s">
+        <v>269</v>
+      </c>
+      <c r="L8" t="s">
+        <v>270</v>
+      </c>
+      <c r="M8" t="s">
+        <v>271</v>
+      </c>
+      <c r="N8" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.72078894806924099</v>
-      </c>
-      <c r="C9">
-        <v>0.65053129069621096</v>
-      </c>
-      <c r="D9">
-        <v>0.60068555621297604</v>
-      </c>
-      <c r="E9">
-        <v>0.443409558634492</v>
-      </c>
-      <c r="F9">
-        <v>0.80128186955383995</v>
-      </c>
-      <c r="G9">
-        <v>0.62461555109505396</v>
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" t="s">
+        <v>206</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.72264292252642004</v>
-      </c>
-      <c r="J9">
-        <v>0.65396888975869405</v>
-      </c>
-      <c r="K9">
-        <v>0.60360375608468897</v>
-      </c>
-      <c r="L9">
-        <v>0.44725220321862302</v>
-      </c>
-      <c r="M9">
-        <v>0.81073947915866396</v>
-      </c>
-      <c r="N9">
-        <v>0.62777777415181102</v>
+      <c r="I9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J9" t="s">
+        <v>274</v>
+      </c>
+      <c r="K9" t="s">
+        <v>275</v>
+      </c>
+      <c r="L9" t="s">
+        <v>276</v>
+      </c>
+      <c r="M9" t="s">
+        <v>277</v>
+      </c>
+      <c r="N9" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.70938748335552504</v>
-      </c>
-      <c r="C10">
-        <v>0.64500639734873</v>
-      </c>
-      <c r="D10">
-        <v>0.545721535445998</v>
-      </c>
-      <c r="E10">
-        <v>0.396170715122031</v>
-      </c>
-      <c r="F10">
-        <v>0.80027920097839</v>
-      </c>
-      <c r="G10">
-        <v>0.59122469850435799</v>
+      <c r="B10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" t="s">
+        <v>212</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.72014645918282405</v>
-      </c>
-      <c r="J10">
-        <v>0.66706674563470003</v>
-      </c>
-      <c r="K10">
-        <v>0.56464542290927699</v>
-      </c>
-      <c r="L10">
-        <v>0.42216859316302902</v>
-      </c>
-      <c r="M10">
-        <v>0.80329910170468499</v>
-      </c>
-      <c r="N10">
-        <v>0.61159773251711902</v>
+      <c r="I10" t="s">
+        <v>279</v>
+      </c>
+      <c r="J10" t="s">
+        <v>280</v>
+      </c>
+      <c r="K10" t="s">
+        <v>281</v>
+      </c>
+      <c r="L10" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" t="s">
+        <v>283</v>
+      </c>
+      <c r="N10" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.60793941411451402</v>
-      </c>
-      <c r="C11">
-        <v>0.48167047597607598</v>
-      </c>
-      <c r="D11">
-        <v>0.46700300195078598</v>
-      </c>
-      <c r="E11">
-        <v>0.227441716474344</v>
-      </c>
-      <c r="F11">
-        <v>0.60025225146308903</v>
-      </c>
-      <c r="G11">
-        <v>0.47422335179740999</v>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" t="s">
+        <v>218</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.60922027128235001</v>
-      </c>
-      <c r="J11">
-        <v>0.48639588610330198</v>
-      </c>
-      <c r="K11">
-        <v>0.46963356440182102</v>
-      </c>
-      <c r="L11">
-        <v>0.22868498522509101</v>
-      </c>
-      <c r="M11">
-        <v>0.60222517330136605</v>
-      </c>
-      <c r="N11">
-        <v>0.47786777610330899</v>
+      <c r="I11" t="s">
+        <v>285</v>
+      </c>
+      <c r="J11" t="s">
+        <v>286</v>
+      </c>
+      <c r="K11" t="s">
+        <v>287</v>
+      </c>
+      <c r="L11" t="s">
+        <v>288</v>
+      </c>
+      <c r="M11" t="s">
+        <v>289</v>
+      </c>
+      <c r="N11" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.63132490013315501</v>
-      </c>
-      <c r="C12">
-        <v>0.52920349715511905</v>
-      </c>
-      <c r="D12">
-        <v>0.52600090350909601</v>
-      </c>
-      <c r="E12">
-        <v>0.299938552476404</v>
-      </c>
-      <c r="F12">
-        <v>0.651842392894876</v>
-      </c>
-      <c r="G12">
-        <v>0.52759734032296901</v>
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" t="s">
+        <v>224</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.63526670550053999</v>
-      </c>
-      <c r="J12">
-        <v>0.53572921882659497</v>
-      </c>
-      <c r="K12">
-        <v>0.53251227150882197</v>
-      </c>
-      <c r="L12">
-        <v>0.30876196736889699</v>
-      </c>
-      <c r="M12">
-        <v>0.65820951288701601</v>
-      </c>
-      <c r="N12">
-        <v>0.53411590134253495</v>
+      <c r="I12" t="s">
+        <v>291</v>
+      </c>
+      <c r="J12" t="s">
+        <v>292</v>
+      </c>
+      <c r="K12" t="s">
+        <v>293</v>
+      </c>
+      <c r="L12" t="s">
+        <v>294</v>
+      </c>
+      <c r="M12" t="s">
+        <v>295</v>
+      </c>
+      <c r="N12" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.72752996005326198</v>
-      </c>
-      <c r="C13">
-        <v>0.67795847202926296</v>
-      </c>
-      <c r="D13">
-        <v>0.57049858210146498</v>
-      </c>
-      <c r="E13">
-        <v>0.43763072453311502</v>
-      </c>
-      <c r="F13">
-        <v>0.82285210866873404</v>
-      </c>
-      <c r="G13">
-        <v>0.61960376728484601</v>
+      <c r="B13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>230</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.731380544229008</v>
-      </c>
-      <c r="J13">
-        <v>0.68651595210741601</v>
-      </c>
-      <c r="K13">
-        <v>0.57906943426992297</v>
-      </c>
-      <c r="L13">
-        <v>0.44735119964616399</v>
-      </c>
-      <c r="M13">
-        <v>0.82560518941280603</v>
-      </c>
-      <c r="N13">
-        <v>0.62823165988357998</v>
+      <c r="I13" t="s">
+        <v>297</v>
+      </c>
+      <c r="J13" t="s">
+        <v>298</v>
+      </c>
+      <c r="K13" t="s">
+        <v>299</v>
+      </c>
+      <c r="L13" t="s">
+        <v>300</v>
+      </c>
+      <c r="M13" t="s">
+        <v>301</v>
+      </c>
+      <c r="N13" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.71254993342210304</v>
-      </c>
-      <c r="C14">
-        <v>0.69284577312440099</v>
-      </c>
-      <c r="D14">
-        <v>0.50929244029059495</v>
-      </c>
-      <c r="E14">
-        <v>0.388504426912263</v>
-      </c>
-      <c r="F14">
-        <v>0.82096107982044297</v>
-      </c>
-      <c r="G14">
-        <v>0.58705581538274798</v>
+      <c r="B14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" t="s">
+        <v>236</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.71640176416742896</v>
-      </c>
-      <c r="J14">
-        <v>0.70871748036303905</v>
-      </c>
-      <c r="K14">
-        <v>0.51880210496518797</v>
-      </c>
-      <c r="L14">
-        <v>0.399162808682684</v>
-      </c>
-      <c r="M14">
-        <v>0.81946820494492201</v>
-      </c>
-      <c r="N14">
-        <v>0.59906843855310699</v>
+      <c r="I14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J14" t="s">
+        <v>303</v>
+      </c>
+      <c r="K14" t="s">
+        <v>304</v>
+      </c>
+      <c r="L14" t="s">
+        <v>305</v>
+      </c>
+      <c r="M14" t="s">
+        <v>306</v>
+      </c>
+      <c r="N14" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3699,7 +4556,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,9 +4568,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3723,9 +4578,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -3775,504 +4628,504 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.73402130492676398</v>
-      </c>
-      <c r="C3">
-        <v>0.68623368723733602</v>
-      </c>
-      <c r="D3">
-        <v>0.57889767097545097</v>
-      </c>
-      <c r="E3">
-        <v>0.45273960573426902</v>
-      </c>
-      <c r="F3">
-        <v>0.82128050095385796</v>
-      </c>
-      <c r="G3">
-        <v>0.62801238892344902</v>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.74095032037946196</v>
-      </c>
-      <c r="J3">
-        <v>0.70019661485164797</v>
-      </c>
-      <c r="K3">
-        <v>0.590567512661057</v>
-      </c>
-      <c r="L3">
-        <v>0.46887822464175899</v>
-      </c>
-      <c r="M3">
-        <v>0.82635183950008395</v>
-      </c>
-      <c r="N3">
-        <v>0.64072647262589799</v>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.73285619174434002</v>
-      </c>
-      <c r="C4">
-        <v>0.67651390355486196</v>
-      </c>
-      <c r="D4">
-        <v>0.58655201688303604</v>
-      </c>
-      <c r="E4">
-        <v>0.45420711760099303</v>
-      </c>
-      <c r="F4">
-        <v>0.82154397891478603</v>
-      </c>
-      <c r="G4">
-        <v>0.62832919194264703</v>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.72721977198968102</v>
-      </c>
-      <c r="J4">
-        <v>0.66050601615613203</v>
-      </c>
-      <c r="K4">
-        <v>0.60873024615466798</v>
-      </c>
-      <c r="L4">
-        <v>0.45664726220578</v>
-      </c>
-      <c r="M4">
-        <v>0.81579556256789099</v>
-      </c>
-      <c r="N4">
-        <v>0.633562090432783</v>
+      <c r="I4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.71646138482023902</v>
-      </c>
-      <c r="C5">
-        <v>0.65264924797733903</v>
-      </c>
-      <c r="D5">
-        <v>0.55807914553245297</v>
-      </c>
-      <c r="E5">
-        <v>0.41442634911035697</v>
-      </c>
-      <c r="F5">
-        <v>0.803614395297652</v>
-      </c>
-      <c r="G5">
-        <v>0.60167075720050101</v>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.71606890238828302</v>
-      </c>
-      <c r="J5">
-        <v>0.65299779785691803</v>
-      </c>
-      <c r="K5">
-        <v>0.55798273829433398</v>
-      </c>
-      <c r="L5">
-        <v>0.41362107530846398</v>
-      </c>
-      <c r="M5">
-        <v>0.80952080939624604</v>
-      </c>
-      <c r="N5">
-        <v>0.60176276739573298</v>
+      <c r="I5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.71205059920106495</v>
-      </c>
-      <c r="C6">
-        <v>0.63743239315373401</v>
-      </c>
-      <c r="D6">
-        <v>0.56994058425375604</v>
-      </c>
-      <c r="E6">
-        <v>0.41451705952673901</v>
-      </c>
-      <c r="F6">
-        <v>0.79740147305965203</v>
-      </c>
-      <c r="G6">
-        <v>0.60180010216295499</v>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.71423816260297901</v>
-      </c>
-      <c r="J6">
-        <v>0.64068952041587801</v>
-      </c>
-      <c r="K6">
-        <v>0.57278378162492105</v>
-      </c>
-      <c r="L6">
-        <v>0.419570490127679</v>
-      </c>
-      <c r="M6">
-        <v>0.80383274624665102</v>
-      </c>
-      <c r="N6">
-        <v>0.60483665480581805</v>
+      <c r="I6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" t="s">
+        <v>114</v>
+      </c>
+      <c r="M6" t="s">
+        <v>115</v>
+      </c>
+      <c r="N6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.70897137150466005</v>
-      </c>
-      <c r="C7">
-        <v>0.70361085165300397</v>
-      </c>
-      <c r="D7">
-        <v>0.50003001239425604</v>
-      </c>
-      <c r="E7">
-        <v>0.37832006888925002</v>
-      </c>
-      <c r="F7">
-        <v>0.808177672826354</v>
-      </c>
-      <c r="G7">
-        <v>0.58460385216527599</v>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.71365565448947299</v>
-      </c>
-      <c r="J7">
-        <v>0.73106689341585795</v>
-      </c>
-      <c r="K7">
-        <v>0.50593751221596905</v>
-      </c>
-      <c r="L7">
-        <v>0.391468305246638</v>
-      </c>
-      <c r="M7">
-        <v>0.80815477853156303</v>
-      </c>
-      <c r="N7">
-        <v>0.59801592239173196</v>
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.74059587217043898</v>
-      </c>
-      <c r="C8">
-        <v>0.70726563299467804</v>
-      </c>
-      <c r="D8">
-        <v>0.58186690706030897</v>
-      </c>
-      <c r="E8">
-        <v>0.46524271699201197</v>
-      </c>
-      <c r="F8">
-        <v>0.84174555138430196</v>
-      </c>
-      <c r="G8">
-        <v>0.63846726935170095</v>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.74377964550220499</v>
-      </c>
-      <c r="J8">
-        <v>0.71819210804806699</v>
-      </c>
-      <c r="K8">
-        <v>0.58605576989558095</v>
-      </c>
-      <c r="L8">
-        <v>0.47235487294994599</v>
-      </c>
-      <c r="M8">
-        <v>0.84328743091692604</v>
-      </c>
-      <c r="N8">
-        <v>0.64543042152179897</v>
+      <c r="I8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8" t="s">
+        <v>126</v>
+      </c>
+      <c r="M8" t="s">
+        <v>127</v>
+      </c>
+      <c r="N8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.70897137150466005</v>
-      </c>
-      <c r="C9">
-        <v>0.63256455344266704</v>
-      </c>
-      <c r="D9">
-        <v>0.60473847687642102</v>
-      </c>
-      <c r="E9">
-        <v>0.43198425893214198</v>
-      </c>
-      <c r="F9">
-        <v>0.80300431599488797</v>
-      </c>
-      <c r="G9">
-        <v>0.61833862069549705</v>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.71723391861529495</v>
-      </c>
-      <c r="J9">
-        <v>0.64246487006185204</v>
-      </c>
-      <c r="K9">
-        <v>0.61564063477498499</v>
-      </c>
-      <c r="L9">
-        <v>0.44883922677016003</v>
-      </c>
-      <c r="M9">
-        <v>0.81899466602244497</v>
-      </c>
-      <c r="N9">
-        <v>0.62876679086910503</v>
+      <c r="I9" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L9" t="s">
+        <v>132</v>
+      </c>
+      <c r="M9" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.71304926764314203</v>
-      </c>
-      <c r="C10">
-        <v>0.63795708721224897</v>
-      </c>
-      <c r="D10">
-        <v>0.59377418278984195</v>
-      </c>
-      <c r="E10">
-        <v>0.42977380882142502</v>
-      </c>
-      <c r="F10">
-        <v>0.81201132722805403</v>
-      </c>
-      <c r="G10">
-        <v>0.61507320198796001</v>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.72247649163684702</v>
-      </c>
-      <c r="J10">
-        <v>0.65442525833974596</v>
-      </c>
-      <c r="K10">
-        <v>0.60972397425568703</v>
-      </c>
-      <c r="L10">
-        <v>0.45018473761639999</v>
-      </c>
-      <c r="M10">
-        <v>0.81679039476390403</v>
-      </c>
-      <c r="N10">
-        <v>0.63128428049429997</v>
+      <c r="I10" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L10" t="s">
+        <v>138</v>
+      </c>
+      <c r="M10" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.61259986684420698</v>
-      </c>
-      <c r="C11">
-        <v>0.49241528922774702</v>
-      </c>
-      <c r="D11">
-        <v>0.47622537906606199</v>
-      </c>
-      <c r="E11">
-        <v>0.23790992181679299</v>
-      </c>
-      <c r="F11">
-        <v>0.60716903429954605</v>
-      </c>
-      <c r="G11">
-        <v>0.48418503464956603</v>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.61745860031621802</v>
-      </c>
-      <c r="J11">
-        <v>0.49616208817590002</v>
-      </c>
-      <c r="K11">
-        <v>0.47714400759926501</v>
-      </c>
-      <c r="L11">
-        <v>0.242713657969061</v>
-      </c>
-      <c r="M11">
-        <v>0.60785800569944903</v>
-      </c>
-      <c r="N11">
-        <v>0.48646724437192101</v>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" t="s">
+        <v>143</v>
+      </c>
+      <c r="L11" t="s">
+        <v>144</v>
+      </c>
+      <c r="M11" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.641561251664447</v>
-      </c>
-      <c r="C12">
-        <v>0.54233510886773895</v>
-      </c>
-      <c r="D12">
-        <v>0.53811519252844298</v>
-      </c>
-      <c r="E12">
-        <v>0.31833334084805598</v>
-      </c>
-      <c r="F12">
-        <v>0.66205072708525903</v>
-      </c>
-      <c r="G12">
-        <v>0.54021690983134896</v>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.636681368061912</v>
-      </c>
-      <c r="J12">
-        <v>0.53725443455633004</v>
-      </c>
-      <c r="K12">
-        <v>0.53209817923255098</v>
-      </c>
-      <c r="L12">
-        <v>0.30824149874137502</v>
-      </c>
-      <c r="M12">
-        <v>0.65759900814795003</v>
-      </c>
-      <c r="N12">
-        <v>0.53466387555578698</v>
+      <c r="I12" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" t="s">
+        <v>148</v>
+      </c>
+      <c r="K12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L12" t="s">
+        <v>150</v>
+      </c>
+      <c r="M12" t="s">
+        <v>151</v>
+      </c>
+      <c r="N12" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.73543608521970705</v>
-      </c>
-      <c r="C13">
-        <v>0.68197836368920794</v>
-      </c>
-      <c r="D13">
-        <v>0.59048850989229895</v>
-      </c>
-      <c r="E13">
-        <v>0.45982802192901101</v>
-      </c>
-      <c r="F13">
-        <v>0.82803048236071797</v>
-      </c>
-      <c r="G13">
-        <v>0.63294439503981903</v>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.73812099525671904</v>
-      </c>
-      <c r="J13">
-        <v>0.69059501204297202</v>
-      </c>
-      <c r="K13">
-        <v>0.59894957855032005</v>
-      </c>
-      <c r="L13">
-        <v>0.46678860141621598</v>
-      </c>
-      <c r="M13">
-        <v>0.83450936244673402</v>
-      </c>
-      <c r="N13">
-        <v>0.64151576367248897</v>
+      <c r="I13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" t="s">
+        <v>154</v>
+      </c>
+      <c r="K13" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" t="s">
+        <v>156</v>
+      </c>
+      <c r="M13" t="s">
+        <v>157</v>
+      </c>
+      <c r="N13" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.70297936085219703</v>
-      </c>
-      <c r="C14">
-        <v>0.69816596984790602</v>
-      </c>
-      <c r="D14">
-        <v>0.48908435124008798</v>
-      </c>
-      <c r="E14">
-        <v>0.36142671144127497</v>
-      </c>
-      <c r="F14">
-        <v>0.82387318535785503</v>
-      </c>
-      <c r="G14">
-        <v>0.575214922002387</v>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" t="s">
+        <v>92</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.70408587833901903</v>
-      </c>
-      <c r="J14">
-        <v>0.70270643628944995</v>
-      </c>
-      <c r="K14">
-        <v>0.49175019570582901</v>
-      </c>
-      <c r="L14">
-        <v>0.364884530110137</v>
-      </c>
-      <c r="M14">
-        <v>0.82368804672206597</v>
-      </c>
-      <c r="N14">
-        <v>0.57859953775274198</v>
+      <c r="I14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" t="s">
+        <v>161</v>
+      </c>
+      <c r="L14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M14" t="s">
+        <v>163</v>
+      </c>
+      <c r="N14" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added TFIDF (1,1) for KT.
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995722AE-EF03-45A8-9244-8D69F76AB3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E38818-DEE5-44EF-9329-6406E66F7EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="451">
   <si>
     <t>TRAINING</t>
   </si>
@@ -957,6 +957,435 @@
   </si>
   <si>
     <t>0.594±0.0029</t>
+  </si>
+  <si>
+    <t>0.7443±0.0027</t>
+  </si>
+  <si>
+    <t>0.7035±0.0056</t>
+  </si>
+  <si>
+    <t>0.5984±0.0046</t>
+  </si>
+  <si>
+    <t>0.4775±0.0062</t>
+  </si>
+  <si>
+    <t>0.8217±0.0017</t>
+  </si>
+  <si>
+    <t>0.6467±0.0044</t>
+  </si>
+  <si>
+    <t>0.7355±0.0027</t>
+  </si>
+  <si>
+    <t>0.6846±0.006</t>
+  </si>
+  <si>
+    <t>0.5875±0.0062</t>
+  </si>
+  <si>
+    <t>0.4589±0.0061</t>
+  </si>
+  <si>
+    <t>0.8055±0.0033</t>
+  </si>
+  <si>
+    <t>0.6323±0.0036</t>
+  </si>
+  <si>
+    <t>0.6774±0.0083</t>
+  </si>
+  <si>
+    <t>0.5302±0.005</t>
+  </si>
+  <si>
+    <t>0.401±0.0083</t>
+  </si>
+  <si>
+    <t>0.8058±0.0038</t>
+  </si>
+  <si>
+    <t>0.5948±0.0059</t>
+  </si>
+  <si>
+    <t>0.7237±0.0028</t>
+  </si>
+  <si>
+    <t>0.6884±0.0075</t>
+  </si>
+  <si>
+    <t>0.5469±0.0037</t>
+  </si>
+  <si>
+    <t>0.422±0.0065</t>
+  </si>
+  <si>
+    <t>0.8115±0.0047</t>
+  </si>
+  <si>
+    <t>0.6096±0.0049</t>
+  </si>
+  <si>
+    <t>0.7087±0.0026</t>
+  </si>
+  <si>
+    <t>0.7038±0.0075</t>
+  </si>
+  <si>
+    <t>0.4994±0.0042</t>
+  </si>
+  <si>
+    <t>0.3777±0.007</t>
+  </si>
+  <si>
+    <t>0.8036±0.0027</t>
+  </si>
+  <si>
+    <t>0.5843±0.005</t>
+  </si>
+  <si>
+    <t>0.7386±0.0021</t>
+  </si>
+  <si>
+    <t>0.6986±0.003</t>
+  </si>
+  <si>
+    <t>0.5856±0.0037</t>
+  </si>
+  <si>
+    <t>0.4627±0.0052</t>
+  </si>
+  <si>
+    <t>0.8342±0.0025</t>
+  </si>
+  <si>
+    <t>0.6371±0.0032</t>
+  </si>
+  <si>
+    <t>0.7226±0.0104</t>
+  </si>
+  <si>
+    <t>0.6538±0.0203</t>
+  </si>
+  <si>
+    <t>0.6142±0.0089</t>
+  </si>
+  <si>
+    <t>0.4546±0.0138</t>
+  </si>
+  <si>
+    <t>0.8198±0.0058</t>
+  </si>
+  <si>
+    <t>0.6332±0.0083</t>
+  </si>
+  <si>
+    <t>0.722±0.0056</t>
+  </si>
+  <si>
+    <t>0.6884±0.0068</t>
+  </si>
+  <si>
+    <t>0.5462±0.017</t>
+  </si>
+  <si>
+    <t>0.4183±0.0169</t>
+  </si>
+  <si>
+    <t>0.8137±0.0047</t>
+  </si>
+  <si>
+    <t>0.6089±0.0097</t>
+  </si>
+  <si>
+    <t>0.6467±0.0228</t>
+  </si>
+  <si>
+    <t>0.5379±0.0461</t>
+  </si>
+  <si>
+    <t>0.4782±0.0158</t>
+  </si>
+  <si>
+    <t>0.2656±0.0433</t>
+  </si>
+  <si>
+    <t>0.6254±0.0641</t>
+  </si>
+  <si>
+    <t>0.506±0.0284</t>
+  </si>
+  <si>
+    <t>0.6436±0.027</t>
+  </si>
+  <si>
+    <t>0.544±0.0476</t>
+  </si>
+  <si>
+    <t>0.5201±0.0082</t>
+  </si>
+  <si>
+    <t>0.307±0.0377</t>
+  </si>
+  <si>
+    <t>0.658±0.0525</t>
+  </si>
+  <si>
+    <t>0.5312±0.0253</t>
+  </si>
+  <si>
+    <t>0.7322±0.0083</t>
+  </si>
+  <si>
+    <t>0.6833±0.0091</t>
+  </si>
+  <si>
+    <t>0.5826±0.029</t>
+  </si>
+  <si>
+    <t>0.4512±0.0256</t>
+  </si>
+  <si>
+    <t>0.8286±0.0081</t>
+  </si>
+  <si>
+    <t>0.6284±0.0151</t>
+  </si>
+  <si>
+    <t>0.7277±0.005</t>
+  </si>
+  <si>
+    <t>0.6824±0.0077</t>
+  </si>
+  <si>
+    <t>0.5614±0.0104</t>
+  </si>
+  <si>
+    <t>0.435±0.0126</t>
+  </si>
+  <si>
+    <t>0.8217±0.0056</t>
+  </si>
+  <si>
+    <t>0.616±0.0093</t>
+  </si>
+  <si>
+    <t>0.7494±0.0017</t>
+  </si>
+  <si>
+    <t>0.7139±0.0031</t>
+  </si>
+  <si>
+    <t>0.6035±0.003</t>
+  </si>
+  <si>
+    <t>0.4882±0.0041</t>
+  </si>
+  <si>
+    <t>0.8285±0.0018</t>
+  </si>
+  <si>
+    <t>0.6541±0.0025</t>
+  </si>
+  <si>
+    <t>0.7348±0.0025</t>
+  </si>
+  <si>
+    <t>0.6757±0.0038</t>
+  </si>
+  <si>
+    <t>0.5972±0.004</t>
+  </si>
+  <si>
+    <t>0.4623±0.0056</t>
+  </si>
+  <si>
+    <t>0.7972±0.0016</t>
+  </si>
+  <si>
+    <t>0.634±0.0037</t>
+  </si>
+  <si>
+    <t>0.7194±0.003</t>
+  </si>
+  <si>
+    <t>0.6787±0.0071</t>
+  </si>
+  <si>
+    <t>0.5415±0.0033</t>
+  </si>
+  <si>
+    <t>0.412±0.0067</t>
+  </si>
+  <si>
+    <t>0.8102±0.0041</t>
+  </si>
+  <si>
+    <t>0.6024±0.0042</t>
+  </si>
+  <si>
+    <t>0.7265±0.002</t>
+  </si>
+  <si>
+    <t>0.6937±0.0047</t>
+  </si>
+  <si>
+    <t>0.5513±0.0045</t>
+  </si>
+  <si>
+    <t>0.4288±0.0052</t>
+  </si>
+  <si>
+    <t>0.8183±0.0021</t>
+  </si>
+  <si>
+    <t>0.6143±0.0036</t>
+  </si>
+  <si>
+    <t>0.7117±0.0021</t>
+  </si>
+  <si>
+    <t>0.7152±0.0073</t>
+  </si>
+  <si>
+    <t>0.5018±0.0038</t>
+  </si>
+  <si>
+    <t>0.3859±0.0058</t>
+  </si>
+  <si>
+    <t>0.8068±0.0033</t>
+  </si>
+  <si>
+    <t>0.5897±0.0045</t>
+  </si>
+  <si>
+    <t>0.7404±0.002</t>
+  </si>
+  <si>
+    <t>0.7061±0.0048</t>
+  </si>
+  <si>
+    <t>0.585±0.0036</t>
+  </si>
+  <si>
+    <t>0.4658±0.0046</t>
+  </si>
+  <si>
+    <t>0.8397±0.0029</t>
+  </si>
+  <si>
+    <t>0.6398±0.0036</t>
+  </si>
+  <si>
+    <t>0.7297±0.0083</t>
+  </si>
+  <si>
+    <t>0.6666±0.0196</t>
+  </si>
+  <si>
+    <t>0.6169±0.0061</t>
+  </si>
+  <si>
+    <t>0.4645±0.0109</t>
+  </si>
+  <si>
+    <t>0.8265±0.0047</t>
+  </si>
+  <si>
+    <t>0.6406±0.0071</t>
+  </si>
+  <si>
+    <t>0.7251±0.0053</t>
+  </si>
+  <si>
+    <t>0.6939±0.0064</t>
+  </si>
+  <si>
+    <t>0.5505±0.0182</t>
+  </si>
+  <si>
+    <t>0.4259±0.0165</t>
+  </si>
+  <si>
+    <t>0.8153±0.0063</t>
+  </si>
+  <si>
+    <t>0.6138±0.0098</t>
+  </si>
+  <si>
+    <t>0.6516±0.0243</t>
+  </si>
+  <si>
+    <t>0.5467±0.0481</t>
+  </si>
+  <si>
+    <t>0.489±0.0183</t>
+  </si>
+  <si>
+    <t>0.2806±0.0471</t>
+  </si>
+  <si>
+    <t>0.6328±0.064</t>
+  </si>
+  <si>
+    <t>0.516±0.0308</t>
+  </si>
+  <si>
+    <t>0.6498±0.0267</t>
+  </si>
+  <si>
+    <t>0.5526±0.0498</t>
+  </si>
+  <si>
+    <t>0.5262±0.0097</t>
+  </si>
+  <si>
+    <t>0.3171±0.039</t>
+  </si>
+  <si>
+    <t>0.6622±0.0539</t>
+  </si>
+  <si>
+    <t>0.5385±0.0271</t>
+  </si>
+  <si>
+    <t>0.7345±0.0089</t>
+  </si>
+  <si>
+    <t>0.6874±0.0082</t>
+  </si>
+  <si>
+    <t>0.5837±0.0295</t>
+  </si>
+  <si>
+    <t>0.4556±0.0268</t>
+  </si>
+  <si>
+    <t>0.8334±0.0083</t>
+  </si>
+  <si>
+    <t>0.6308±0.0157</t>
+  </si>
+  <si>
+    <t>0.729±0.005</t>
+  </si>
+  <si>
+    <t>0.6877±0.0085</t>
+  </si>
+  <si>
+    <t>0.5602±0.0103</t>
+  </si>
+  <si>
+    <t>0.4371±0.0124</t>
+  </si>
+  <si>
+    <t>0.824±0.0071</t>
+  </si>
+  <si>
+    <t>0.6174±0.0095</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1789,7 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -3849,8 +4278,8 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3867,9 +4296,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3879,9 +4306,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -3931,504 +4356,504 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.746837549933422</v>
-      </c>
-      <c r="C3">
-        <v>0.706932242646645</v>
-      </c>
-      <c r="D3">
-        <v>0.60074629024475601</v>
-      </c>
-      <c r="E3">
-        <v>0.48296157621664498</v>
-      </c>
-      <c r="F3">
-        <v>0.833116213388852</v>
-      </c>
-      <c r="G3">
-        <v>0.64952801708131502</v>
+      <c r="B3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G3" t="s">
+        <v>313</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.74769077140717299</v>
-      </c>
-      <c r="J3">
-        <v>0.70953815031399203</v>
-      </c>
-      <c r="K3">
-        <v>0.60128379454265901</v>
-      </c>
-      <c r="L3">
-        <v>0.48453598112115698</v>
-      </c>
-      <c r="M3">
-        <v>0.84145513739541999</v>
-      </c>
-      <c r="N3">
-        <v>0.65094087426226699</v>
+      <c r="I3" t="s">
+        <v>379</v>
+      </c>
+      <c r="J3" t="s">
+        <v>380</v>
+      </c>
+      <c r="K3" t="s">
+        <v>381</v>
+      </c>
+      <c r="L3" t="s">
+        <v>382</v>
+      </c>
+      <c r="M3" t="s">
+        <v>383</v>
+      </c>
+      <c r="N3" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.73202396804260905</v>
-      </c>
-      <c r="C4">
-        <v>0.671847969297234</v>
-      </c>
-      <c r="D4">
-        <v>0.59654640629718303</v>
-      </c>
-      <c r="E4">
-        <v>0.457295775371029</v>
-      </c>
-      <c r="F4">
-        <v>0.82131351501653505</v>
-      </c>
-      <c r="G4">
-        <v>0.63196195027985802</v>
+      <c r="B4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" t="s">
+        <v>319</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.73579096280269596</v>
-      </c>
-      <c r="J4">
-        <v>0.67474336886591202</v>
-      </c>
-      <c r="K4">
-        <v>0.60051880160445403</v>
-      </c>
-      <c r="L4">
-        <v>0.46569095813732397</v>
-      </c>
-      <c r="M4">
-        <v>0.82117786387560299</v>
-      </c>
-      <c r="N4">
-        <v>0.63547102493043806</v>
+      <c r="I4" t="s">
+        <v>385</v>
+      </c>
+      <c r="J4" t="s">
+        <v>386</v>
+      </c>
+      <c r="K4" t="s">
+        <v>387</v>
+      </c>
+      <c r="L4" t="s">
+        <v>388</v>
+      </c>
+      <c r="M4" t="s">
+        <v>389</v>
+      </c>
+      <c r="N4" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.71521304926764295</v>
-      </c>
-      <c r="C5">
-        <v>0.67388147802522802</v>
-      </c>
-      <c r="D5">
-        <v>0.53198542594676501</v>
-      </c>
-      <c r="E5">
-        <v>0.40028099730320799</v>
-      </c>
-      <c r="F5">
-        <v>0.80559180019825505</v>
-      </c>
-      <c r="G5">
-        <v>0.59458489812439996</v>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F5" t="s">
+        <v>323</v>
+      </c>
+      <c r="G5" t="s">
+        <v>324</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.71873179662145203</v>
-      </c>
-      <c r="J5">
-        <v>0.68338244512953406</v>
-      </c>
-      <c r="K5">
-        <v>0.53448047760569695</v>
-      </c>
-      <c r="L5">
-        <v>0.40833618108486702</v>
-      </c>
-      <c r="M5">
-        <v>0.81077544978773497</v>
-      </c>
-      <c r="N5">
-        <v>0.59982871444981201</v>
+      <c r="I5" t="s">
+        <v>391</v>
+      </c>
+      <c r="J5" t="s">
+        <v>392</v>
+      </c>
+      <c r="K5" t="s">
+        <v>393</v>
+      </c>
+      <c r="L5" t="s">
+        <v>394</v>
+      </c>
+      <c r="M5" t="s">
+        <v>395</v>
+      </c>
+      <c r="N5" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.72644806924101202</v>
-      </c>
-      <c r="C6">
-        <v>0.69496967791601805</v>
-      </c>
-      <c r="D6">
-        <v>0.54909738313452106</v>
-      </c>
-      <c r="E6">
-        <v>0.42821957167796698</v>
-      </c>
-      <c r="F6">
-        <v>0.81292289818641505</v>
-      </c>
-      <c r="G6">
-        <v>0.61348144878827204</v>
+      <c r="B6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F6" t="s">
+        <v>329</v>
+      </c>
+      <c r="G6" t="s">
+        <v>330</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.72389115419821903</v>
-      </c>
-      <c r="J6">
-        <v>0.68827544580644995</v>
-      </c>
-      <c r="K6">
-        <v>0.54618717203220402</v>
-      </c>
-      <c r="L6">
-        <v>0.42222516814224897</v>
-      </c>
-      <c r="M6">
-        <v>0.81933453434522896</v>
-      </c>
-      <c r="N6">
-        <v>0.60905403515971601</v>
+      <c r="I6" t="s">
+        <v>397</v>
+      </c>
+      <c r="J6" t="s">
+        <v>398</v>
+      </c>
+      <c r="K6" t="s">
+        <v>399</v>
+      </c>
+      <c r="L6" t="s">
+        <v>400</v>
+      </c>
+      <c r="M6" t="s">
+        <v>401</v>
+      </c>
+      <c r="N6" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.70689081225033201</v>
-      </c>
-      <c r="C7">
-        <v>0.70300833172065202</v>
-      </c>
-      <c r="D7">
-        <v>0.49582380625149503</v>
-      </c>
-      <c r="E7">
-        <v>0.37257975234331497</v>
-      </c>
-      <c r="F7">
-        <v>0.80398247016575097</v>
-      </c>
-      <c r="G7">
-        <v>0.58151305060916803</v>
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F7" t="s">
+        <v>335</v>
+      </c>
+      <c r="G7" t="s">
+        <v>336</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.70999417491886496</v>
-      </c>
-      <c r="J7">
-        <v>0.70995633120881196</v>
-      </c>
-      <c r="K7">
-        <v>0.49815107745014803</v>
-      </c>
-      <c r="L7">
-        <v>0.38105440247096101</v>
-      </c>
-      <c r="M7">
-        <v>0.80325062692516103</v>
-      </c>
-      <c r="N7">
-        <v>0.58548686780557802</v>
+      <c r="I7" t="s">
+        <v>403</v>
+      </c>
+      <c r="J7" t="s">
+        <v>404</v>
+      </c>
+      <c r="K7" t="s">
+        <v>405</v>
+      </c>
+      <c r="L7" t="s">
+        <v>406</v>
+      </c>
+      <c r="M7" t="s">
+        <v>407</v>
+      </c>
+      <c r="N7" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.73826564580559195</v>
-      </c>
-      <c r="C8">
-        <v>0.69887585884139403</v>
-      </c>
-      <c r="D8">
-        <v>0.58376191423597101</v>
-      </c>
-      <c r="E8">
-        <v>0.46162843537369103</v>
-      </c>
-      <c r="F8">
-        <v>0.83186737150176204</v>
-      </c>
-      <c r="G8">
-        <v>0.636153273720799</v>
+      <c r="B8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E8" t="s">
+        <v>340</v>
+      </c>
+      <c r="F8" t="s">
+        <v>341</v>
+      </c>
+      <c r="G8" t="s">
+        <v>342</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.74153282849296798</v>
-      </c>
-      <c r="J8">
-        <v>0.70857962368607497</v>
-      </c>
-      <c r="K8">
-        <v>0.58816350511414195</v>
-      </c>
-      <c r="L8">
-        <v>0.46858516048604798</v>
-      </c>
-      <c r="M8">
-        <v>0.83482342182175395</v>
-      </c>
-      <c r="N8">
-        <v>0.64278061840244405</v>
+      <c r="I8" t="s">
+        <v>409</v>
+      </c>
+      <c r="J8" t="s">
+        <v>410</v>
+      </c>
+      <c r="K8" t="s">
+        <v>411</v>
+      </c>
+      <c r="L8" t="s">
+        <v>412</v>
+      </c>
+      <c r="M8" t="s">
+        <v>413</v>
+      </c>
+      <c r="N8" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.71837549933422096</v>
-      </c>
-      <c r="C9">
-        <v>0.646147075401584</v>
-      </c>
-      <c r="D9">
-        <v>0.61884263734885503</v>
-      </c>
-      <c r="E9">
-        <v>0.45100436703079699</v>
-      </c>
-      <c r="F9">
-        <v>0.82265728934349702</v>
-      </c>
-      <c r="G9">
-        <v>0.63220017716563304</v>
+      <c r="B9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" t="s">
+        <v>344</v>
+      </c>
+      <c r="D9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" t="s">
+        <v>346</v>
+      </c>
+      <c r="F9" t="s">
+        <v>347</v>
+      </c>
+      <c r="G9" t="s">
+        <v>348</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.73021552800199696</v>
-      </c>
-      <c r="J9">
-        <v>0.66161790189829495</v>
-      </c>
-      <c r="K9">
-        <v>0.62218314537957597</v>
-      </c>
-      <c r="L9">
-        <v>0.46843747618492798</v>
-      </c>
-      <c r="M9">
-        <v>0.82590621565274902</v>
-      </c>
-      <c r="N9">
-        <v>0.64129486124872803</v>
+      <c r="I9" t="s">
+        <v>415</v>
+      </c>
+      <c r="J9" t="s">
+        <v>416</v>
+      </c>
+      <c r="K9" t="s">
+        <v>417</v>
+      </c>
+      <c r="L9" t="s">
+        <v>418</v>
+      </c>
+      <c r="M9" t="s">
+        <v>419</v>
+      </c>
+      <c r="N9" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.71820905459387396</v>
-      </c>
-      <c r="C10">
-        <v>0.68663190372538996</v>
-      </c>
-      <c r="D10">
-        <v>0.53467951298889504</v>
-      </c>
-      <c r="E10">
-        <v>0.40702330853270102</v>
-      </c>
-      <c r="F10">
-        <v>0.812325192244432</v>
-      </c>
-      <c r="G10">
-        <v>0.60120294768752802</v>
+      <c r="B10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10" t="s">
+        <v>352</v>
+      </c>
+      <c r="F10" t="s">
+        <v>353</v>
+      </c>
+      <c r="G10" t="s">
+        <v>354</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.72364150786385895</v>
-      </c>
-      <c r="J10">
-        <v>0.69102024144268603</v>
-      </c>
-      <c r="K10">
-        <v>0.54523177310790005</v>
-      </c>
-      <c r="L10">
-        <v>0.42149758297309198</v>
-      </c>
-      <c r="M10">
-        <v>0.81643395514555195</v>
-      </c>
-      <c r="N10">
-        <v>0.60952975131403198</v>
+      <c r="I10" t="s">
+        <v>421</v>
+      </c>
+      <c r="J10" t="s">
+        <v>422</v>
+      </c>
+      <c r="K10" t="s">
+        <v>423</v>
+      </c>
+      <c r="L10" t="s">
+        <v>424</v>
+      </c>
+      <c r="M10" t="s">
+        <v>425</v>
+      </c>
+      <c r="N10" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.63948069241011896</v>
-      </c>
-      <c r="C11">
-        <v>0.52077197126734998</v>
-      </c>
-      <c r="D11">
-        <v>0.474664291352971</v>
-      </c>
-      <c r="E11">
-        <v>0.25483734206751002</v>
-      </c>
-      <c r="F11">
-        <v>0.60599821851472802</v>
-      </c>
-      <c r="G11">
-        <v>0.49665029893006901</v>
+      <c r="B11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" t="s">
+        <v>357</v>
+      </c>
+      <c r="E11" t="s">
+        <v>358</v>
+      </c>
+      <c r="F11" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" t="s">
+        <v>360</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.64283931097611702</v>
-      </c>
-      <c r="J11">
-        <v>0.52481830931828399</v>
-      </c>
-      <c r="K11">
-        <v>0.479331360201182</v>
-      </c>
-      <c r="L11">
-        <v>0.26320817530643698</v>
-      </c>
-      <c r="M11">
-        <v>0.60949852015088701</v>
-      </c>
-      <c r="N11">
-        <v>0.50104457871186103</v>
+      <c r="I11" t="s">
+        <v>427</v>
+      </c>
+      <c r="J11" t="s">
+        <v>428</v>
+      </c>
+      <c r="K11" t="s">
+        <v>429</v>
+      </c>
+      <c r="L11" t="s">
+        <v>430</v>
+      </c>
+      <c r="M11" t="s">
+        <v>431</v>
+      </c>
+      <c r="N11" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.63215712383488598</v>
-      </c>
-      <c r="C12">
-        <v>0.52462001131888802</v>
-      </c>
-      <c r="D12">
-        <v>0.51221705787635796</v>
-      </c>
-      <c r="E12">
-        <v>0.28748961038497101</v>
-      </c>
-      <c r="F12">
-        <v>0.63930686798518099</v>
-      </c>
-      <c r="G12">
-        <v>0.51834435068837204</v>
+      <c r="B12" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" t="s">
+        <v>363</v>
+      </c>
+      <c r="E12" t="s">
+        <v>364</v>
+      </c>
+      <c r="F12" t="s">
+        <v>365</v>
+      </c>
+      <c r="G12" t="s">
+        <v>366</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.63934426229508201</v>
-      </c>
-      <c r="J12">
-        <v>0.53556592877613995</v>
-      </c>
-      <c r="K12">
-        <v>0.521432885543894</v>
-      </c>
-      <c r="L12">
-        <v>0.30025433131546603</v>
-      </c>
-      <c r="M12">
-        <v>0.64319331036065996</v>
-      </c>
-      <c r="N12">
-        <v>0.52840492128723404</v>
+      <c r="I12" t="s">
+        <v>433</v>
+      </c>
+      <c r="J12" t="s">
+        <v>434</v>
+      </c>
+      <c r="K12" t="s">
+        <v>435</v>
+      </c>
+      <c r="L12" t="s">
+        <v>436</v>
+      </c>
+      <c r="M12" t="s">
+        <v>437</v>
+      </c>
+      <c r="N12" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.73377163781624499</v>
-      </c>
-      <c r="C13">
-        <v>0.67853376020725398</v>
-      </c>
-      <c r="D13">
-        <v>0.588443759686199</v>
-      </c>
-      <c r="E13">
-        <v>0.45648295155384999</v>
-      </c>
-      <c r="F13">
-        <v>0.82995479355361002</v>
-      </c>
-      <c r="G13">
-        <v>0.63028577959922805</v>
+      <c r="B13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E13" t="s">
+        <v>370</v>
+      </c>
+      <c r="F13" t="s">
+        <v>371</v>
+      </c>
+      <c r="G13" t="s">
+        <v>372</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.73712240991928102</v>
-      </c>
-      <c r="J13">
-        <v>0.68044612355608403</v>
-      </c>
-      <c r="K13">
-        <v>0.59535680323035001</v>
-      </c>
-      <c r="L13">
-        <v>0.46531645037555602</v>
-      </c>
-      <c r="M13">
-        <v>0.83255729297623005</v>
-      </c>
-      <c r="N13">
-        <v>0.63506395915118996</v>
+      <c r="I13" t="s">
+        <v>439</v>
+      </c>
+      <c r="J13" t="s">
+        <v>440</v>
+      </c>
+      <c r="K13" t="s">
+        <v>441</v>
+      </c>
+      <c r="L13" t="s">
+        <v>442</v>
+      </c>
+      <c r="M13" t="s">
+        <v>443</v>
+      </c>
+      <c r="N13" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.72453395472702997</v>
-      </c>
-      <c r="C14">
-        <v>0.67892102177834301</v>
-      </c>
-      <c r="D14">
-        <v>0.55355290664132195</v>
-      </c>
-      <c r="E14">
-        <v>0.426463920364334</v>
-      </c>
-      <c r="F14">
-        <v>0.81884678711266101</v>
-      </c>
-      <c r="G14">
-        <v>0.60986069777101104</v>
+      <c r="B14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D14" t="s">
+        <v>375</v>
+      </c>
+      <c r="E14" t="s">
+        <v>376</v>
+      </c>
+      <c r="F14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G14" t="s">
+        <v>378</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.72697012565532104</v>
-      </c>
-      <c r="J14">
-        <v>0.68103748875175796</v>
-      </c>
-      <c r="K14">
-        <v>0.55613770932933204</v>
-      </c>
-      <c r="L14">
-        <v>0.43228419834558801</v>
-      </c>
-      <c r="M14">
-        <v>0.81914946772822905</v>
-      </c>
-      <c r="N14">
-        <v>0.61228293219789898</v>
+      <c r="I14" t="s">
+        <v>445</v>
+      </c>
+      <c r="J14" t="s">
+        <v>446</v>
+      </c>
+      <c r="K14" t="s">
+        <v>447</v>
+      </c>
+      <c r="L14" t="s">
+        <v>448</v>
+      </c>
+      <c r="M14" t="s">
+        <v>449</v>
+      </c>
+      <c r="N14" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added TFIDF 1,2 KT
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E38818-DEE5-44EF-9329-6406E66F7EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB714F-A1A4-46CF-9050-6C7FC4BFD33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="595">
   <si>
     <t>TRAINING</t>
   </si>
@@ -1386,6 +1386,438 @@
   </si>
   <si>
     <t>0.6174±0.0095</t>
+  </si>
+  <si>
+    <t>0.7416±0.0022</t>
+  </si>
+  <si>
+    <t>0.6984±0.0059</t>
+  </si>
+  <si>
+    <t>0.5981±0.0056</t>
+  </si>
+  <si>
+    <t>0.4725±0.0048</t>
+  </si>
+  <si>
+    <t>0.8207±0.002</t>
+  </si>
+  <si>
+    <t>0.6444±0.0037</t>
+  </si>
+  <si>
+    <t>0.7387±0.002</t>
+  </si>
+  <si>
+    <t>0.6871±0.0049</t>
+  </si>
+  <si>
+    <t>0.6018±0.0038</t>
+  </si>
+  <si>
+    <t>0.4695±0.0043</t>
+  </si>
+  <si>
+    <t>0.8147±0.0015</t>
+  </si>
+  <si>
+    <t>0.6417±0.0038</t>
+  </si>
+  <si>
+    <t>0.7165±0.0022</t>
+  </si>
+  <si>
+    <t>0.6776±0.0054</t>
+  </si>
+  <si>
+    <t>0.5327±0.0041</t>
+  </si>
+  <si>
+    <t>0.4033±0.0057</t>
+  </si>
+  <si>
+    <t>0.8087±0.0018</t>
+  </si>
+  <si>
+    <t>0.5965±0.0041</t>
+  </si>
+  <si>
+    <t>0.7237±0.0022</t>
+  </si>
+  <si>
+    <t>0.6861±0.0048</t>
+  </si>
+  <si>
+    <t>0.5505±0.0039</t>
+  </si>
+  <si>
+    <t>0.4231±0.0054</t>
+  </si>
+  <si>
+    <t>0.8143±0.0029</t>
+  </si>
+  <si>
+    <t>0.6109±0.0038</t>
+  </si>
+  <si>
+    <t>0.7107±0.003</t>
+  </si>
+  <si>
+    <t>0.706±0.0068</t>
+  </si>
+  <si>
+    <t>0.5029±0.0048</t>
+  </si>
+  <si>
+    <t>0.383±0.0083</t>
+  </si>
+  <si>
+    <t>0.8053±0.0024</t>
+  </si>
+  <si>
+    <t>0.5874±0.0052</t>
+  </si>
+  <si>
+    <t>0.7408±0.0019</t>
+  </si>
+  <si>
+    <t>0.7037±0.0041</t>
+  </si>
+  <si>
+    <t>0.5898±0.0028</t>
+  </si>
+  <si>
+    <t>0.468±0.0042</t>
+  </si>
+  <si>
+    <t>0.838±0.002</t>
+  </si>
+  <si>
+    <t>0.6417±0.0027</t>
+  </si>
+  <si>
+    <t>0.7199±0.0037</t>
+  </si>
+  <si>
+    <t>0.6478±0.006</t>
+  </si>
+  <si>
+    <t>0.619±0.0059</t>
+  </si>
+  <si>
+    <t>0.4533±0.0075</t>
+  </si>
+  <si>
+    <t>0.82±0.004</t>
+  </si>
+  <si>
+    <t>0.633±0.0055</t>
+  </si>
+  <si>
+    <t>0.725±0.0025</t>
+  </si>
+  <si>
+    <t>0.6687±0.0043</t>
+  </si>
+  <si>
+    <t>0.5822±0.0047</t>
+  </si>
+  <si>
+    <t>0.4383±0.006</t>
+  </si>
+  <si>
+    <t>0.8212±0.0016</t>
+  </si>
+  <si>
+    <t>0.6225±0.0042</t>
+  </si>
+  <si>
+    <t>0.6305±0.0046</t>
+  </si>
+  <si>
+    <t>0.5103±0.0064</t>
+  </si>
+  <si>
+    <t>0.4672±0.0045</t>
+  </si>
+  <si>
+    <t>0.237±0.009</t>
+  </si>
+  <si>
+    <t>0.6004±0.0034</t>
+  </si>
+  <si>
+    <t>0.4878±0.0051</t>
+  </si>
+  <si>
+    <t>0.6346±0.0028</t>
+  </si>
+  <si>
+    <t>0.529±0.0037</t>
+  </si>
+  <si>
+    <t>0.5177±0.0053</t>
+  </si>
+  <si>
+    <t>0.2941±0.0072</t>
+  </si>
+  <si>
+    <t>0.6416±0.0043</t>
+  </si>
+  <si>
+    <t>0.5233±0.0044</t>
+  </si>
+  <si>
+    <t>0.7395±0.0025</t>
+  </si>
+  <si>
+    <t>0.6871±0.0035</t>
+  </si>
+  <si>
+    <t>0.6048±0.0038</t>
+  </si>
+  <si>
+    <t>0.4721±0.0056</t>
+  </si>
+  <si>
+    <t>0.8377±0.0015</t>
+  </si>
+  <si>
+    <t>0.6433±0.0033</t>
+  </si>
+  <si>
+    <t>0.7237±0.0035</t>
+  </si>
+  <si>
+    <t>0.6925±0.0055</t>
+  </si>
+  <si>
+    <t>0.5452±0.0074</t>
+  </si>
+  <si>
+    <t>0.4213±0.0093</t>
+  </si>
+  <si>
+    <t>0.8244±0.0017</t>
+  </si>
+  <si>
+    <t>0.6101±0.0056</t>
+  </si>
+  <si>
+    <t>0.7474±0.0023</t>
+  </si>
+  <si>
+    <t>0.7087±0.0061</t>
+  </si>
+  <si>
+    <t>0.6045±0.0039</t>
+  </si>
+  <si>
+    <t>0.4849±0.0047</t>
+  </si>
+  <si>
+    <t>0.8276±0.002</t>
+  </si>
+  <si>
+    <t>0.6524±0.0035</t>
+  </si>
+  <si>
+    <t>0.7299±0.0026</t>
+  </si>
+  <si>
+    <t>0.6621±0.0044</t>
+  </si>
+  <si>
+    <t>0.6157±0.0024</t>
+  </si>
+  <si>
+    <t>0.4647±0.0045</t>
+  </si>
+  <si>
+    <t>0.7983±0.0023</t>
+  </si>
+  <si>
+    <t>0.6381±0.003</t>
+  </si>
+  <si>
+    <t>0.7211±0.0018</t>
+  </si>
+  <si>
+    <t>0.6833±0.0056</t>
+  </si>
+  <si>
+    <t>0.5441±0.0018</t>
+  </si>
+  <si>
+    <t>0.416±0.0037</t>
+  </si>
+  <si>
+    <t>0.8132±0.0034</t>
+  </si>
+  <si>
+    <t>0.6058±0.0024</t>
+  </si>
+  <si>
+    <t>0.7264±0.0026</t>
+  </si>
+  <si>
+    <t>0.691±0.0062</t>
+  </si>
+  <si>
+    <t>0.5543±0.0036</t>
+  </si>
+  <si>
+    <t>0.4295±0.0062</t>
+  </si>
+  <si>
+    <t>0.8214±0.0036</t>
+  </si>
+  <si>
+    <t>0.6151±0.0038</t>
+  </si>
+  <si>
+    <t>0.7135±0.0015</t>
+  </si>
+  <si>
+    <t>0.7179±0.0057</t>
+  </si>
+  <si>
+    <t>0.5048±0.0031</t>
+  </si>
+  <si>
+    <t>0.3908±0.0042</t>
+  </si>
+  <si>
+    <t>0.8091±0.0031</t>
+  </si>
+  <si>
+    <t>0.5928±0.0034</t>
+  </si>
+  <si>
+    <t>0.7426±0.0021</t>
+  </si>
+  <si>
+    <t>0.7095±0.0042</t>
+  </si>
+  <si>
+    <t>0.5883±0.004</t>
+  </si>
+  <si>
+    <t>0.4708±0.0051</t>
+  </si>
+  <si>
+    <t>0.8433±0.0026</t>
+  </si>
+  <si>
+    <t>0.6433±0.0034</t>
+  </si>
+  <si>
+    <t>0.7273±0.004</t>
+  </si>
+  <si>
+    <t>0.6596±0.0067</t>
+  </si>
+  <si>
+    <t>0.6242±0.0043</t>
+  </si>
+  <si>
+    <t>0.465±0.006</t>
+  </si>
+  <si>
+    <t>0.8286±0.0026</t>
+  </si>
+  <si>
+    <t>0.6414±0.0039</t>
+  </si>
+  <si>
+    <t>0.7285±0.0025</t>
+  </si>
+  <si>
+    <t>0.6744±0.0042</t>
+  </si>
+  <si>
+    <t>0.5879±0.0042</t>
+  </si>
+  <si>
+    <t>0.4465±0.0058</t>
+  </si>
+  <si>
+    <t>0.8247±0.0027</t>
+  </si>
+  <si>
+    <t>0.6282±0.0039</t>
+  </si>
+  <si>
+    <t>0.6341±0.0051</t>
+  </si>
+  <si>
+    <t>0.5178±0.0094</t>
+  </si>
+  <si>
+    <t>0.4749±0.006</t>
+  </si>
+  <si>
+    <t>0.2477±0.0098</t>
+  </si>
+  <si>
+    <t>0.6062±0.0045</t>
+  </si>
+  <si>
+    <t>0.4954±0.0075</t>
+  </si>
+  <si>
+    <t>0.6402±0.0037</t>
+  </si>
+  <si>
+    <t>0.5357±0.0047</t>
+  </si>
+  <si>
+    <t>0.5228±0.0038</t>
+  </si>
+  <si>
+    <t>0.3034±0.0066</t>
+  </si>
+  <si>
+    <t>0.6448±0.0032</t>
+  </si>
+  <si>
+    <t>0.5292±0.0041</t>
+  </si>
+  <si>
+    <t>0.7439±0.002</t>
+  </si>
+  <si>
+    <t>0.6944±0.0043</t>
+  </si>
+  <si>
+    <t>0.6093±0.0038</t>
+  </si>
+  <si>
+    <t>0.4811±0.0046</t>
+  </si>
+  <si>
+    <t>0.8444±0.0026</t>
+  </si>
+  <si>
+    <t>0.6491±0.0034</t>
+  </si>
+  <si>
+    <t>0.7254±0.002</t>
+  </si>
+  <si>
+    <t>0.7012±0.0042</t>
+  </si>
+  <si>
+    <t>0.5441±0.0032</t>
+  </si>
+  <si>
+    <t>0.4247±0.0049</t>
+  </si>
+  <si>
+    <t>0.827±0.0028</t>
+  </si>
+  <si>
+    <t>0.6128±0.0029</t>
   </si>
 </sst>
 </file>
@@ -4278,7 +4710,7 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -5566,7 +5998,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5578,9 +6010,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -5590,9 +6020,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -5642,504 +6070,504 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.73959720372836202</v>
-      </c>
-      <c r="C3">
-        <v>0.69232692953058805</v>
-      </c>
-      <c r="D3">
-        <v>0.59020397280179804</v>
-      </c>
-      <c r="E3">
-        <v>0.466826344214191</v>
-      </c>
-      <c r="F3">
-        <v>0.83328120225746405</v>
-      </c>
-      <c r="G3">
-        <v>0.63719962387421003</v>
+      <c r="B3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F3" t="s">
+        <v>455</v>
+      </c>
+      <c r="G3" t="s">
+        <v>456</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.750353665640342</v>
-      </c>
-      <c r="J3">
-        <v>0.71398913780090101</v>
-      </c>
-      <c r="K3">
-        <v>0.60698449403732202</v>
-      </c>
-      <c r="L3">
-        <v>0.49100902792849599</v>
-      </c>
-      <c r="M3">
-        <v>0.83878672121217401</v>
-      </c>
-      <c r="N3">
-        <v>0.65615289376086305</v>
+      <c r="I3" t="s">
+        <v>523</v>
+      </c>
+      <c r="J3" t="s">
+        <v>524</v>
+      </c>
+      <c r="K3" t="s">
+        <v>525</v>
+      </c>
+      <c r="L3" t="s">
+        <v>526</v>
+      </c>
+      <c r="M3" t="s">
+        <v>527</v>
+      </c>
+      <c r="N3" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.73593541944074503</v>
-      </c>
-      <c r="C4">
-        <v>0.67797990884271497</v>
-      </c>
-      <c r="D4">
-        <v>0.59640018905084202</v>
-      </c>
-      <c r="E4">
-        <v>0.46365733139265197</v>
-      </c>
-      <c r="F4">
-        <v>0.83201131913390103</v>
-      </c>
-      <c r="G4">
-        <v>0.63457887717301897</v>
+      <c r="B4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C4" t="s">
+        <v>458</v>
+      </c>
+      <c r="D4" t="s">
+        <v>459</v>
+      </c>
+      <c r="E4" t="s">
+        <v>460</v>
+      </c>
+      <c r="F4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G4" t="s">
+        <v>462</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.73013231255721001</v>
-      </c>
-      <c r="J4">
-        <v>0.661857714496349</v>
-      </c>
-      <c r="K4">
-        <v>0.61882109324763501</v>
-      </c>
-      <c r="L4">
-        <v>0.46697441768806902</v>
-      </c>
-      <c r="M4">
-        <v>0.82737320723204699</v>
-      </c>
-      <c r="N4">
-        <v>0.63961629095823602</v>
+      <c r="I4" t="s">
+        <v>529</v>
+      </c>
+      <c r="J4" t="s">
+        <v>530</v>
+      </c>
+      <c r="K4" t="s">
+        <v>531</v>
+      </c>
+      <c r="L4" t="s">
+        <v>532</v>
+      </c>
+      <c r="M4" t="s">
+        <v>533</v>
+      </c>
+      <c r="N4" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.71596205059920104</v>
-      </c>
-      <c r="C5">
-        <v>0.67651080860300705</v>
-      </c>
-      <c r="D5">
-        <v>0.53017291156459601</v>
-      </c>
-      <c r="E5">
-        <v>0.40131516769206399</v>
-      </c>
-      <c r="F5">
-        <v>0.80699939932425702</v>
-      </c>
-      <c r="G5">
-        <v>0.59446845781951596</v>
+      <c r="B5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C5" t="s">
+        <v>464</v>
+      </c>
+      <c r="D5" t="s">
+        <v>465</v>
+      </c>
+      <c r="E5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F5" t="s">
+        <v>467</v>
+      </c>
+      <c r="G5" t="s">
+        <v>468</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.71881501206623899</v>
-      </c>
-      <c r="J5">
-        <v>0.68213679564700402</v>
-      </c>
-      <c r="K5">
-        <v>0.53545388717750397</v>
-      </c>
-      <c r="L5">
-        <v>0.40884851832158497</v>
-      </c>
-      <c r="M5">
-        <v>0.81640547550417897</v>
-      </c>
-      <c r="N5">
-        <v>0.599959910942648</v>
+      <c r="I5" t="s">
+        <v>535</v>
+      </c>
+      <c r="J5" t="s">
+        <v>536</v>
+      </c>
+      <c r="K5" t="s">
+        <v>537</v>
+      </c>
+      <c r="L5" t="s">
+        <v>538</v>
+      </c>
+      <c r="M5" t="s">
+        <v>539</v>
+      </c>
+      <c r="N5" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.72395139813581799</v>
-      </c>
-      <c r="C6">
-        <v>0.68574432390523399</v>
-      </c>
-      <c r="D6">
-        <v>0.54873728481028095</v>
-      </c>
-      <c r="E6">
-        <v>0.42308515819391002</v>
-      </c>
-      <c r="F6">
-        <v>0.81220420299547103</v>
-      </c>
-      <c r="G6">
-        <v>0.60963804679983102</v>
+      <c r="B6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C6" t="s">
+        <v>470</v>
+      </c>
+      <c r="D6" t="s">
+        <v>471</v>
+      </c>
+      <c r="E6" t="s">
+        <v>472</v>
+      </c>
+      <c r="F6" t="s">
+        <v>473</v>
+      </c>
+      <c r="G6" t="s">
+        <v>474</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.72513938587001703</v>
-      </c>
-      <c r="J6">
-        <v>0.68391314123509095</v>
-      </c>
-      <c r="K6">
-        <v>0.55207740068394695</v>
-      </c>
-      <c r="L6">
-        <v>0.42688259452331301</v>
-      </c>
-      <c r="M6">
-        <v>0.82026677445624896</v>
-      </c>
-      <c r="N6">
-        <v>0.61096420482381797</v>
+      <c r="I6" t="s">
+        <v>541</v>
+      </c>
+      <c r="J6" t="s">
+        <v>542</v>
+      </c>
+      <c r="K6" t="s">
+        <v>543</v>
+      </c>
+      <c r="L6" t="s">
+        <v>544</v>
+      </c>
+      <c r="M6" t="s">
+        <v>545</v>
+      </c>
+      <c r="N6" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.70614181091877404</v>
-      </c>
-      <c r="C7">
-        <v>0.69561383424578305</v>
-      </c>
-      <c r="D7">
-        <v>0.49725357434678602</v>
-      </c>
-      <c r="E7">
-        <v>0.37058021298592098</v>
-      </c>
-      <c r="F7">
-        <v>0.80812046223432599</v>
-      </c>
-      <c r="G7">
-        <v>0.579941178629236</v>
+      <c r="B7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C7" t="s">
+        <v>476</v>
+      </c>
+      <c r="D7" t="s">
+        <v>477</v>
+      </c>
+      <c r="E7" t="s">
+        <v>478</v>
+      </c>
+      <c r="F7" t="s">
+        <v>479</v>
+      </c>
+      <c r="G7" t="s">
+        <v>480</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.71556960971956396</v>
-      </c>
-      <c r="J7">
-        <v>0.72169000380206605</v>
-      </c>
-      <c r="K7">
-        <v>0.50918871329123505</v>
-      </c>
-      <c r="L7">
-        <v>0.39651003250322198</v>
-      </c>
-      <c r="M7">
-        <v>0.806894298628689</v>
-      </c>
-      <c r="N7">
-        <v>0.59709604094692603</v>
+      <c r="I7" t="s">
+        <v>547</v>
+      </c>
+      <c r="J7" t="s">
+        <v>548</v>
+      </c>
+      <c r="K7" t="s">
+        <v>549</v>
+      </c>
+      <c r="L7" t="s">
+        <v>550</v>
+      </c>
+      <c r="M7" t="s">
+        <v>551</v>
+      </c>
+      <c r="N7" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.73934753661784203</v>
-      </c>
-      <c r="C8">
-        <v>0.69956541416257201</v>
-      </c>
-      <c r="D8">
-        <v>0.58673686128147495</v>
-      </c>
-      <c r="E8">
-        <v>0.464508138584665</v>
-      </c>
-      <c r="F8">
-        <v>0.83919237825047499</v>
-      </c>
-      <c r="G8">
-        <v>0.638202735395344</v>
+      <c r="B8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8" t="s">
+        <v>482</v>
+      </c>
+      <c r="D8" t="s">
+        <v>483</v>
+      </c>
+      <c r="E8" t="s">
+        <v>484</v>
+      </c>
+      <c r="F8" t="s">
+        <v>485</v>
+      </c>
+      <c r="G8" t="s">
+        <v>486</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.74361321461263197</v>
-      </c>
-      <c r="J8">
-        <v>0.709555896698988</v>
-      </c>
-      <c r="K8">
-        <v>0.59065694531759805</v>
-      </c>
-      <c r="L8">
-        <v>0.47362624639377299</v>
-      </c>
-      <c r="M8">
-        <v>0.84039842315680002</v>
-      </c>
-      <c r="N8">
-        <v>0.64467001852757699</v>
+      <c r="I8" t="s">
+        <v>553</v>
+      </c>
+      <c r="J8" t="s">
+        <v>554</v>
+      </c>
+      <c r="K8" t="s">
+        <v>555</v>
+      </c>
+      <c r="L8" t="s">
+        <v>556</v>
+      </c>
+      <c r="M8" t="s">
+        <v>557</v>
+      </c>
+      <c r="N8" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.71488015978694996</v>
-      </c>
-      <c r="C9">
-        <v>0.64074550144779896</v>
-      </c>
-      <c r="D9">
-        <v>0.60929042996776805</v>
-      </c>
-      <c r="E9">
-        <v>0.44138019588636701</v>
-      </c>
-      <c r="F9">
-        <v>0.81681717366282403</v>
-      </c>
-      <c r="G9">
-        <v>0.62462220847515204</v>
+      <c r="B9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C9" t="s">
+        <v>488</v>
+      </c>
+      <c r="D9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E9" t="s">
+        <v>490</v>
+      </c>
+      <c r="F9" t="s">
+        <v>491</v>
+      </c>
+      <c r="G9" t="s">
+        <v>492</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.726221186652242</v>
-      </c>
-      <c r="J9">
-        <v>0.65797694347134095</v>
-      </c>
-      <c r="K9">
-        <v>0.62110036346888897</v>
-      </c>
-      <c r="L9">
-        <v>0.46178609518201702</v>
-      </c>
-      <c r="M9">
-        <v>0.82894477601042804</v>
-      </c>
-      <c r="N9">
-        <v>0.63900706630751802</v>
+      <c r="I9" t="s">
+        <v>559</v>
+      </c>
+      <c r="J9" t="s">
+        <v>560</v>
+      </c>
+      <c r="K9" t="s">
+        <v>561</v>
+      </c>
+      <c r="L9" t="s">
+        <v>562</v>
+      </c>
+      <c r="M9" t="s">
+        <v>563</v>
+      </c>
+      <c r="N9" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.72420106524633798</v>
-      </c>
-      <c r="C10">
-        <v>0.66344353722980598</v>
-      </c>
-      <c r="D10">
-        <v>0.57766321688729005</v>
-      </c>
-      <c r="E10">
-        <v>0.43597094342763199</v>
-      </c>
-      <c r="F10">
-        <v>0.82101738283491199</v>
-      </c>
-      <c r="G10">
-        <v>0.61758898123455697</v>
+      <c r="B10" t="s">
+        <v>493</v>
+      </c>
+      <c r="C10" t="s">
+        <v>494</v>
+      </c>
+      <c r="D10" t="s">
+        <v>495</v>
+      </c>
+      <c r="E10" t="s">
+        <v>496</v>
+      </c>
+      <c r="F10" t="s">
+        <v>497</v>
+      </c>
+      <c r="G10" t="s">
+        <v>498</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.72846800366147901</v>
-      </c>
-      <c r="J10">
-        <v>0.673273388221452</v>
-      </c>
-      <c r="K10">
-        <v>0.59018942941990904</v>
-      </c>
-      <c r="L10">
-        <v>0.44748062542096201</v>
-      </c>
-      <c r="M10">
-        <v>0.82470226890777198</v>
-      </c>
-      <c r="N10">
-        <v>0.628999652842684</v>
+      <c r="I10" t="s">
+        <v>565</v>
+      </c>
+      <c r="J10" t="s">
+        <v>566</v>
+      </c>
+      <c r="K10" t="s">
+        <v>567</v>
+      </c>
+      <c r="L10" t="s">
+        <v>568</v>
+      </c>
+      <c r="M10" t="s">
+        <v>569</v>
+      </c>
+      <c r="N10" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.63124167776298201</v>
-      </c>
-      <c r="C11">
-        <v>0.51330691564590902</v>
-      </c>
-      <c r="D11">
-        <v>0.46727448958118301</v>
-      </c>
-      <c r="E11">
-        <v>0.23602902385698299</v>
-      </c>
-      <c r="F11">
-        <v>0.60045586718588695</v>
-      </c>
-      <c r="G11">
-        <v>0.48921022921372997</v>
+      <c r="B11" t="s">
+        <v>499</v>
+      </c>
+      <c r="C11" t="s">
+        <v>500</v>
+      </c>
+      <c r="D11" t="s">
+        <v>501</v>
+      </c>
+      <c r="E11" t="s">
+        <v>502</v>
+      </c>
+      <c r="F11" t="s">
+        <v>503</v>
+      </c>
+      <c r="G11" t="s">
+        <v>504</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.62960805525505503</v>
-      </c>
-      <c r="J11">
-        <v>0.51226484251928694</v>
-      </c>
-      <c r="K11">
-        <v>0.47088694637543799</v>
-      </c>
-      <c r="L11">
-        <v>0.238772123982366</v>
-      </c>
-      <c r="M11">
-        <v>0.60316520978157795</v>
-      </c>
-      <c r="N11">
-        <v>0.49070515896753603</v>
+      <c r="I11" t="s">
+        <v>571</v>
+      </c>
+      <c r="J11" t="s">
+        <v>572</v>
+      </c>
+      <c r="K11" t="s">
+        <v>573</v>
+      </c>
+      <c r="L11" t="s">
+        <v>574</v>
+      </c>
+      <c r="M11" t="s">
+        <v>575</v>
+      </c>
+      <c r="N11" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.63848202396804199</v>
-      </c>
-      <c r="C12">
-        <v>0.53204580928192902</v>
-      </c>
-      <c r="D12">
-        <v>0.51842571713590202</v>
-      </c>
-      <c r="E12">
-        <v>0.298034984069454</v>
-      </c>
-      <c r="F12">
-        <v>0.64080097597530605</v>
-      </c>
-      <c r="G12">
-        <v>0.52514746623684105</v>
+      <c r="B12" t="s">
+        <v>505</v>
+      </c>
+      <c r="C12" t="s">
+        <v>506</v>
+      </c>
+      <c r="D12" t="s">
+        <v>507</v>
+      </c>
+      <c r="E12" t="s">
+        <v>508</v>
+      </c>
+      <c r="F12" t="s">
+        <v>509</v>
+      </c>
+      <c r="G12" t="s">
+        <v>510</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.64375468086876897</v>
-      </c>
-      <c r="J12">
-        <v>0.53764889712396002</v>
-      </c>
-      <c r="K12">
-        <v>0.52695227016790103</v>
-      </c>
-      <c r="L12">
-        <v>0.31301646128670801</v>
-      </c>
-      <c r="M12">
-        <v>0.64798544265717195</v>
-      </c>
-      <c r="N12">
-        <v>0.53224684623151097</v>
+      <c r="I12" t="s">
+        <v>577</v>
+      </c>
+      <c r="J12" t="s">
+        <v>578</v>
+      </c>
+      <c r="K12" t="s">
+        <v>579</v>
+      </c>
+      <c r="L12" t="s">
+        <v>580</v>
+      </c>
+      <c r="M12" t="s">
+        <v>581</v>
+      </c>
+      <c r="N12" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.73735019973368798</v>
-      </c>
-      <c r="C13">
-        <v>0.68227098889764504</v>
-      </c>
-      <c r="D13">
-        <v>0.59873607975397003</v>
-      </c>
-      <c r="E13">
-        <v>0.466464120658029</v>
-      </c>
-      <c r="F13">
-        <v>0.83843184709337704</v>
-      </c>
-      <c r="G13">
-        <v>0.637779864325693</v>
+      <c r="B13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C13" t="s">
+        <v>512</v>
+      </c>
+      <c r="D13" t="s">
+        <v>513</v>
+      </c>
+      <c r="E13" t="s">
+        <v>514</v>
+      </c>
+      <c r="F13" t="s">
+        <v>515</v>
+      </c>
+      <c r="G13" t="s">
+        <v>516</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.74469501539485705</v>
-      </c>
-      <c r="J13">
-        <v>0.69473265318436594</v>
-      </c>
-      <c r="K13">
-        <v>0.61124739042923804</v>
-      </c>
-      <c r="L13">
-        <v>0.48327825658033702</v>
-      </c>
-      <c r="M13">
-        <v>0.84371066475924905</v>
-      </c>
-      <c r="N13">
-        <v>0.65032160848326903</v>
+      <c r="I13" t="s">
+        <v>583</v>
+      </c>
+      <c r="J13" t="s">
+        <v>584</v>
+      </c>
+      <c r="K13" t="s">
+        <v>585</v>
+      </c>
+      <c r="L13" t="s">
+        <v>586</v>
+      </c>
+      <c r="M13" t="s">
+        <v>587</v>
+      </c>
+      <c r="N13" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.72345206391478001</v>
-      </c>
-      <c r="C14">
-        <v>0.69035079223469697</v>
-      </c>
-      <c r="D14">
-        <v>0.54128873093340901</v>
-      </c>
-      <c r="E14">
-        <v>0.42015357690010702</v>
-      </c>
-      <c r="F14">
-        <v>0.82506225600771399</v>
-      </c>
-      <c r="G14">
-        <v>0.60679946883547597</v>
+      <c r="B14" t="s">
+        <v>517</v>
+      </c>
+      <c r="C14" t="s">
+        <v>518</v>
+      </c>
+      <c r="D14" t="s">
+        <v>519</v>
+      </c>
+      <c r="E14" t="s">
+        <v>520</v>
+      </c>
+      <c r="F14" t="s">
+        <v>521</v>
+      </c>
+      <c r="G14" t="s">
+        <v>522</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.72439044686693799</v>
-      </c>
-      <c r="J14">
-        <v>0.69877030851794197</v>
-      </c>
-      <c r="K14">
-        <v>0.54369155242841305</v>
-      </c>
-      <c r="L14">
-        <v>0.42251716229380698</v>
-      </c>
-      <c r="M14">
-        <v>0.82580846226962801</v>
-      </c>
-      <c r="N14">
-        <v>0.61155279815129004</v>
+      <c r="I14" t="s">
+        <v>589</v>
+      </c>
+      <c r="J14" t="s">
+        <v>590</v>
+      </c>
+      <c r="K14" t="s">
+        <v>591</v>
+      </c>
+      <c r="L14" t="s">
+        <v>592</v>
+      </c>
+      <c r="M14" t="s">
+        <v>593</v>
+      </c>
+      <c r="N14" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -6154,7 +6582,7 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added BOW 2,2 KTKT results.
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB714F-A1A4-46CF-9050-6C7FC4BFD33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B2BC5-5166-476B-9AE0-A0E2F753167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="727">
   <si>
     <t>TRAINING</t>
   </si>
@@ -1818,6 +1818,402 @@
   </si>
   <si>
     <t>0.6128±0.0029</t>
+  </si>
+  <si>
+    <t>0.6813±0.0024</t>
+  </si>
+  <si>
+    <t>0.6375±0.0062</t>
+  </si>
+  <si>
+    <t>0.4664±0.0041</t>
+  </si>
+  <si>
+    <t>0.3022±0.0071</t>
+  </si>
+  <si>
+    <t>0.7024±0.0048</t>
+  </si>
+  <si>
+    <t>0.5387±0.0046</t>
+  </si>
+  <si>
+    <t>0.655±0.0023</t>
+  </si>
+  <si>
+    <t>0.5553±0.0038</t>
+  </si>
+  <si>
+    <t>0.5077±0.0053</t>
+  </si>
+  <si>
+    <t>0.297±0.0067</t>
+  </si>
+  <si>
+    <t>0.7211±0.0034</t>
+  </si>
+  <si>
+    <t>0.5304±0.0044</t>
+  </si>
+  <si>
+    <t>0.6438±0.0026</t>
+  </si>
+  <si>
+    <t>0.5403±0.0046</t>
+  </si>
+  <si>
+    <t>0.5034±0.0057</t>
+  </si>
+  <si>
+    <t>0.2819±0.0068</t>
+  </si>
+  <si>
+    <t>0.7017±0.0038</t>
+  </si>
+  <si>
+    <t>0.5212±0.0049</t>
+  </si>
+  <si>
+    <t>0.6622±0.0018</t>
+  </si>
+  <si>
+    <t>0.6955±0.0104</t>
+  </si>
+  <si>
+    <t>0.3979±0.0028</t>
+  </si>
+  <si>
+    <t>0.2254±0.0074</t>
+  </si>
+  <si>
+    <t>0.697±0.0024</t>
+  </si>
+  <si>
+    <t>0.5062±0.0046</t>
+  </si>
+  <si>
+    <t>0.6722±0.0018</t>
+  </si>
+  <si>
+    <t>0.6336±0.0057</t>
+  </si>
+  <si>
+    <t>0.4432±0.006</t>
+  </si>
+  <si>
+    <t>0.2698±0.0066</t>
+  </si>
+  <si>
+    <t>0.7041±0.0039</t>
+  </si>
+  <si>
+    <t>0.5215±0.0039</t>
+  </si>
+  <si>
+    <t>0.6536±0.011</t>
+  </si>
+  <si>
+    <t>0.5599±0.0275</t>
+  </si>
+  <si>
+    <t>0.5034±0.0153</t>
+  </si>
+  <si>
+    <t>0.2924±0.0101</t>
+  </si>
+  <si>
+    <t>0.7066±0.007</t>
+  </si>
+  <si>
+    <t>0.5295±0.0072</t>
+  </si>
+  <si>
+    <t>0.3463±0.1081</t>
+  </si>
+  <si>
+    <t>0.4716±0.0288</t>
+  </si>
+  <si>
+    <t>0.47±0.0125</t>
+  </si>
+  <si>
+    <t>0.1812±0.039</t>
+  </si>
+  <si>
+    <t>0.6258±0.0329</t>
+  </si>
+  <si>
+    <t>0.4707±0.02</t>
+  </si>
+  <si>
+    <t>0.576±0.0655</t>
+  </si>
+  <si>
+    <t>0.4767±0.0284</t>
+  </si>
+  <si>
+    <t>0.45±0.0197</t>
+  </si>
+  <si>
+    <t>0.1925±0.0389</t>
+  </si>
+  <si>
+    <t>0.5945±0.0359</t>
+  </si>
+  <si>
+    <t>0.4629±0.0231</t>
+  </si>
+  <si>
+    <t>0.6279±0.0122</t>
+  </si>
+  <si>
+    <t>0.5338±0.0573</t>
+  </si>
+  <si>
+    <t>0.4817±0.0308</t>
+  </si>
+  <si>
+    <t>0.2514±0.0104</t>
+  </si>
+  <si>
+    <t>0.6657±0.0107</t>
+  </si>
+  <si>
+    <t>0.5033±0.0038</t>
+  </si>
+  <si>
+    <t>0.686±0.0053</t>
+  </si>
+  <si>
+    <t>0.6331±0.0053</t>
+  </si>
+  <si>
+    <t>0.4925±0.0167</t>
+  </si>
+  <si>
+    <t>0.3242±0.0193</t>
+  </si>
+  <si>
+    <t>0.7385±0.0115</t>
+  </si>
+  <si>
+    <t>0.5538±0.0116</t>
+  </si>
+  <si>
+    <t>0.6835±0.0136</t>
+  </si>
+  <si>
+    <t>0.6587±0.0417</t>
+  </si>
+  <si>
+    <t>0.4728±0.0107</t>
+  </si>
+  <si>
+    <t>0.3143±0.0133</t>
+  </si>
+  <si>
+    <t>0.749±0.0157</t>
+  </si>
+  <si>
+    <t>0.5496±0.011</t>
+  </si>
+  <si>
+    <t>0.6856±0.003</t>
+  </si>
+  <si>
+    <t>0.6454±0.0097</t>
+  </si>
+  <si>
+    <t>0.4732±0.0032</t>
+  </si>
+  <si>
+    <t>0.315±0.0079</t>
+  </si>
+  <si>
+    <t>0.7131±0.0041</t>
+  </si>
+  <si>
+    <t>0.546±0.0055</t>
+  </si>
+  <si>
+    <t>0.6635±0.0035</t>
+  </si>
+  <si>
+    <t>0.5688±0.006</t>
+  </si>
+  <si>
+    <t>0.5141±0.0047</t>
+  </si>
+  <si>
+    <t>0.3113±0.0072</t>
+  </si>
+  <si>
+    <t>0.7325±0.0027</t>
+  </si>
+  <si>
+    <t>0.54±0.0051</t>
+  </si>
+  <si>
+    <t>0.6515±0.0043</t>
+  </si>
+  <si>
+    <t>0.551±0.0075</t>
+  </si>
+  <si>
+    <t>0.5069±0.0055</t>
+  </si>
+  <si>
+    <t>0.2926±0.0085</t>
+  </si>
+  <si>
+    <t>0.7093±0.0029</t>
+  </si>
+  <si>
+    <t>0.528±0.0064</t>
+  </si>
+  <si>
+    <t>0.6631±0.0014</t>
+  </si>
+  <si>
+    <t>0.7037±0.0107</t>
+  </si>
+  <si>
+    <t>0.3985±0.002</t>
+  </si>
+  <si>
+    <t>0.2293±0.0059</t>
+  </si>
+  <si>
+    <t>0.7037±0.0033</t>
+  </si>
+  <si>
+    <t>0.5088±0.0041</t>
+  </si>
+  <si>
+    <t>0.681±0.002</t>
+  </si>
+  <si>
+    <t>0.6601±0.0085</t>
+  </si>
+  <si>
+    <t>0.4555±0.0029</t>
+  </si>
+  <si>
+    <t>0.2967±0.0061</t>
+  </si>
+  <si>
+    <t>0.7258±0.0032</t>
+  </si>
+  <si>
+    <t>0.539±0.0042</t>
+  </si>
+  <si>
+    <t>0.6596±0.011</t>
+  </si>
+  <si>
+    <t>0.5684±0.0292</t>
+  </si>
+  <si>
+    <t>0.5059±0.0122</t>
+  </si>
+  <si>
+    <t>0.3011±0.0116</t>
+  </si>
+  <si>
+    <t>0.7117±0.005</t>
+  </si>
+  <si>
+    <t>0.5347±0.0084</t>
+  </si>
+  <si>
+    <t>0.3381±0.1162</t>
+  </si>
+  <si>
+    <t>0.4827±0.0342</t>
+  </si>
+  <si>
+    <t>0.4748±0.0162</t>
+  </si>
+  <si>
+    <t>0.1887±0.0462</t>
+  </si>
+  <si>
+    <t>0.6291±0.0387</t>
+  </si>
+  <si>
+    <t>0.4786±0.0244</t>
+  </si>
+  <si>
+    <t>0.5819±0.065</t>
+  </si>
+  <si>
+    <t>0.4834±0.0332</t>
+  </si>
+  <si>
+    <t>0.4553±0.0208</t>
+  </si>
+  <si>
+    <t>0.2026±0.0429</t>
+  </si>
+  <si>
+    <t>0.5992±0.0395</t>
+  </si>
+  <si>
+    <t>0.4688±0.0261</t>
+  </si>
+  <si>
+    <t>0.6353±0.0112</t>
+  </si>
+  <si>
+    <t>0.5443±0.0612</t>
+  </si>
+  <si>
+    <t>0.4854±0.0308</t>
+  </si>
+  <si>
+    <t>0.2614±0.015</t>
+  </si>
+  <si>
+    <t>0.671±0.013</t>
+  </si>
+  <si>
+    <t>0.51±0.008</t>
+  </si>
+  <si>
+    <t>0.6917±0.0042</t>
+  </si>
+  <si>
+    <t>0.6454±0.0096</t>
+  </si>
+  <si>
+    <t>0.5±0.0148</t>
+  </si>
+  <si>
+    <t>0.3394±0.0153</t>
+  </si>
+  <si>
+    <t>0.7475±0.0075</t>
+  </si>
+  <si>
+    <t>0.5632±0.0081</t>
+  </si>
+  <si>
+    <t>0.6879±0.0103</t>
+  </si>
+  <si>
+    <t>0.674±0.0388</t>
+  </si>
+  <si>
+    <t>0.475±0.014</t>
+  </si>
+  <si>
+    <t>0.3246±0.0108</t>
+  </si>
+  <si>
+    <t>0.7544±0.0151</t>
+  </si>
+  <si>
+    <t>0.5563±0.0082</t>
   </si>
 </sst>
 </file>
@@ -6583,7 +6979,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6602,9 +6998,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -6614,9 +7008,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -6666,504 +7058,480 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.66303262316910705</v>
-      </c>
-      <c r="C3">
-        <v>0.60038379721475998</v>
-      </c>
-      <c r="D3">
-        <v>0.43067838250017298</v>
-      </c>
-      <c r="E3">
-        <v>0.24183649216334199</v>
-      </c>
-      <c r="F3">
-        <v>0.64592377057401995</v>
-      </c>
-      <c r="G3">
-        <v>0.50156494487122905</v>
+      <c r="B3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D3" t="s">
+        <v>597</v>
+      </c>
+      <c r="E3" t="s">
+        <v>598</v>
+      </c>
+      <c r="F3" t="s">
+        <v>599</v>
+      </c>
+      <c r="G3" t="s">
+        <v>600</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.66014812349172003</v>
-      </c>
-      <c r="J3">
-        <v>0.58692496327347998</v>
-      </c>
-      <c r="K3">
-        <v>0.42541385787060998</v>
-      </c>
-      <c r="L3">
-        <v>0.23263418769094199</v>
-      </c>
-      <c r="M3">
-        <v>0.63808041454446696</v>
-      </c>
-      <c r="N3">
-        <v>0.49328546469166401</v>
+      <c r="I3" t="s">
+        <v>661</v>
+      </c>
+      <c r="J3" t="s">
+        <v>662</v>
+      </c>
+      <c r="K3" t="s">
+        <v>663</v>
+      </c>
+      <c r="L3" t="s">
+        <v>664</v>
+      </c>
+      <c r="M3" t="s">
+        <v>665</v>
+      </c>
+      <c r="N3" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.66927430093208995</v>
-      </c>
-      <c r="C4">
-        <v>0.632457488518825</v>
-      </c>
-      <c r="D4">
-        <v>0.43568788656948598</v>
-      </c>
-      <c r="E4">
-        <v>0.25887339928036801</v>
-      </c>
-      <c r="F4">
-        <v>0.68958553855735205</v>
-      </c>
-      <c r="G4">
-        <v>0.51594862074842596</v>
-      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.66580677373720498</v>
-      </c>
-      <c r="J4">
-        <v>0.60081918027481696</v>
-      </c>
-      <c r="K4">
-        <v>0.43940642905585597</v>
-      </c>
-      <c r="L4">
-        <v>0.25404457660653001</v>
-      </c>
-      <c r="M4">
-        <v>0.67583735897471298</v>
-      </c>
-      <c r="N4">
-        <v>0.50758952316641304</v>
-      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.64771970705725701</v>
-      </c>
-      <c r="C5">
-        <v>0.54150739144700399</v>
-      </c>
-      <c r="D5">
-        <v>0.45889275256878598</v>
-      </c>
-      <c r="E5">
-        <v>0.24249725336202599</v>
-      </c>
-      <c r="F5">
-        <v>0.682720761457978</v>
-      </c>
-      <c r="G5">
-        <v>0.496788847710395</v>
+      <c r="B5" t="s">
+        <v>601</v>
+      </c>
+      <c r="C5" t="s">
+        <v>602</v>
+      </c>
+      <c r="D5" t="s">
+        <v>603</v>
+      </c>
+      <c r="E5" t="s">
+        <v>604</v>
+      </c>
+      <c r="F5" t="s">
+        <v>605</v>
+      </c>
+      <c r="G5" t="s">
+        <v>606</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.64883082300074801</v>
-      </c>
-      <c r="J5">
-        <v>0.54257330974781404</v>
-      </c>
-      <c r="K5">
-        <v>0.45060759348145102</v>
-      </c>
-      <c r="L5">
-        <v>0.23650605521896101</v>
-      </c>
-      <c r="M5">
-        <v>0.67882712302186399</v>
-      </c>
-      <c r="N5">
-        <v>0.49233257022520699</v>
+      <c r="I5" t="s">
+        <v>667</v>
+      </c>
+      <c r="J5" t="s">
+        <v>668</v>
+      </c>
+      <c r="K5" t="s">
+        <v>669</v>
+      </c>
+      <c r="L5" t="s">
+        <v>670</v>
+      </c>
+      <c r="M5" t="s">
+        <v>671</v>
+      </c>
+      <c r="N5" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.64389147802929403</v>
-      </c>
-      <c r="C6">
-        <v>0.53305167281892496</v>
-      </c>
-      <c r="D6">
-        <v>0.45730473242133901</v>
-      </c>
-      <c r="E6">
-        <v>0.23703482462942199</v>
-      </c>
-      <c r="F6">
-        <v>0.66980264624395802</v>
-      </c>
-      <c r="G6">
-        <v>0.49228146819743601</v>
+      <c r="B6" t="s">
+        <v>607</v>
+      </c>
+      <c r="C6" t="s">
+        <v>608</v>
+      </c>
+      <c r="D6" t="s">
+        <v>609</v>
+      </c>
+      <c r="E6" t="s">
+        <v>610</v>
+      </c>
+      <c r="F6" t="s">
+        <v>611</v>
+      </c>
+      <c r="G6" t="s">
+        <v>612</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.64433718898227499</v>
-      </c>
-      <c r="J6">
-        <v>0.53479735114614002</v>
-      </c>
-      <c r="K6">
-        <v>0.45090715112853902</v>
-      </c>
-      <c r="L6">
-        <v>0.23065260144802899</v>
-      </c>
-      <c r="M6">
-        <v>0.66768203470930898</v>
-      </c>
-      <c r="N6">
-        <v>0.489282436024011</v>
+      <c r="I6" t="s">
+        <v>673</v>
+      </c>
+      <c r="J6" t="s">
+        <v>674</v>
+      </c>
+      <c r="K6" t="s">
+        <v>675</v>
+      </c>
+      <c r="L6" t="s">
+        <v>676</v>
+      </c>
+      <c r="M6" t="s">
+        <v>677</v>
+      </c>
+      <c r="N6" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.66186750998668398</v>
-      </c>
-      <c r="C7">
-        <v>0.67442793290037195</v>
-      </c>
-      <c r="D7">
-        <v>0.400955082161912</v>
-      </c>
-      <c r="E7">
-        <v>0.22429544541010701</v>
-      </c>
-      <c r="F7">
-        <v>0.68099840087997898</v>
-      </c>
-      <c r="G7">
-        <v>0.50291905946216797</v>
+      <c r="B7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C7" t="s">
+        <v>614</v>
+      </c>
+      <c r="D7" t="s">
+        <v>615</v>
+      </c>
+      <c r="E7" t="s">
+        <v>616</v>
+      </c>
+      <c r="F7" t="s">
+        <v>617</v>
+      </c>
+      <c r="G7" t="s">
+        <v>618</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.65914953815428101</v>
-      </c>
-      <c r="J7">
-        <v>0.66413567457559097</v>
-      </c>
-      <c r="K7">
-        <v>0.396008394440509</v>
-      </c>
-      <c r="L7">
-        <v>0.21276556377641401</v>
-      </c>
-      <c r="M7">
-        <v>0.67566274499132795</v>
-      </c>
-      <c r="N7">
-        <v>0.49616520974065798</v>
+      <c r="I7" t="s">
+        <v>679</v>
+      </c>
+      <c r="J7" t="s">
+        <v>680</v>
+      </c>
+      <c r="K7" t="s">
+        <v>681</v>
+      </c>
+      <c r="L7" t="s">
+        <v>682</v>
+      </c>
+      <c r="M7" t="s">
+        <v>683</v>
+      </c>
+      <c r="N7" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.67318575233022604</v>
-      </c>
-      <c r="C8">
-        <v>0.63461738728350703</v>
-      </c>
-      <c r="D8">
-        <v>0.447607197874824</v>
-      </c>
-      <c r="E8">
-        <v>0.274017907939473</v>
-      </c>
-      <c r="F8">
-        <v>0.70206505569790101</v>
-      </c>
-      <c r="G8">
-        <v>0.52495445832632603</v>
+      <c r="B8" t="s">
+        <v>619</v>
+      </c>
+      <c r="C8" t="s">
+        <v>620</v>
+      </c>
+      <c r="D8" t="s">
+        <v>621</v>
+      </c>
+      <c r="E8" t="s">
+        <v>622</v>
+      </c>
+      <c r="F8" t="s">
+        <v>623</v>
+      </c>
+      <c r="G8" t="s">
+        <v>624</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.67088291586918503</v>
-      </c>
-      <c r="J8">
-        <v>0.63024121402062805</v>
-      </c>
-      <c r="K8">
-        <v>0.43808605567390502</v>
-      </c>
-      <c r="L8">
-        <v>0.264430243399849</v>
-      </c>
-      <c r="M8">
-        <v>0.70036366750832302</v>
-      </c>
-      <c r="N8">
-        <v>0.51688259844265805</v>
+      <c r="I8" t="s">
+        <v>685</v>
+      </c>
+      <c r="J8" t="s">
+        <v>686</v>
+      </c>
+      <c r="K8" t="s">
+        <v>687</v>
+      </c>
+      <c r="L8" t="s">
+        <v>688</v>
+      </c>
+      <c r="M8" t="s">
+        <v>689</v>
+      </c>
+      <c r="N8" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.65312916111850805</v>
-      </c>
-      <c r="C9">
-        <v>0.55419950852826105</v>
-      </c>
-      <c r="D9">
-        <v>0.46432301218761801</v>
-      </c>
-      <c r="E9">
-        <v>0.253613017252455</v>
-      </c>
-      <c r="F9">
-        <v>0.67343636929968398</v>
-      </c>
-      <c r="G9">
-        <v>0.50529581804803703</v>
+      <c r="B9" t="s">
+        <v>625</v>
+      </c>
+      <c r="C9" t="s">
+        <v>626</v>
+      </c>
+      <c r="D9" t="s">
+        <v>627</v>
+      </c>
+      <c r="E9" t="s">
+        <v>628</v>
+      </c>
+      <c r="F9" t="s">
+        <v>629</v>
+      </c>
+      <c r="G9" t="s">
+        <v>630</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.64774902221852304</v>
-      </c>
-      <c r="J9">
-        <v>0.54069448598882397</v>
-      </c>
-      <c r="K9">
-        <v>0.45511922096004598</v>
-      </c>
-      <c r="L9">
-        <v>0.23924517994880701</v>
-      </c>
-      <c r="M9">
-        <v>0.67093008851092995</v>
-      </c>
-      <c r="N9">
-        <v>0.49422989766751801</v>
+      <c r="I9" t="s">
+        <v>691</v>
+      </c>
+      <c r="J9" t="s">
+        <v>692</v>
+      </c>
+      <c r="K9" t="s">
+        <v>693</v>
+      </c>
+      <c r="L9" t="s">
+        <v>694</v>
+      </c>
+      <c r="M9" t="s">
+        <v>695</v>
+      </c>
+      <c r="N9" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.67052263648468702</v>
-      </c>
-      <c r="C10">
-        <v>0.61183731590198498</v>
-      </c>
-      <c r="D10">
-        <v>0.45408496227828299</v>
-      </c>
-      <c r="E10">
-        <v>0.27234821478807703</v>
-      </c>
-      <c r="F10">
-        <v>0.70473765732017501</v>
-      </c>
-      <c r="G10">
-        <v>0.52128777153640304</v>
+      <c r="B10" t="s">
+        <v>631</v>
+      </c>
+      <c r="C10" t="s">
+        <v>632</v>
+      </c>
+      <c r="D10" t="s">
+        <v>633</v>
+      </c>
+      <c r="E10" t="s">
+        <v>634</v>
+      </c>
+      <c r="F10" t="s">
+        <v>635</v>
+      </c>
+      <c r="G10" t="s">
+        <v>636</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.66647249729549796</v>
-      </c>
-      <c r="J10">
-        <v>0.60072181700834104</v>
-      </c>
-      <c r="K10">
-        <v>0.44615805312819701</v>
-      </c>
-      <c r="L10">
-        <v>0.25943774139872799</v>
-      </c>
-      <c r="M10">
-        <v>0.69885571393789203</v>
-      </c>
-      <c r="N10">
-        <v>0.51202985938227796</v>
+      <c r="I10" t="s">
+        <v>697</v>
+      </c>
+      <c r="J10" t="s">
+        <v>698</v>
+      </c>
+      <c r="K10" t="s">
+        <v>699</v>
+      </c>
+      <c r="L10" t="s">
+        <v>700</v>
+      </c>
+      <c r="M10" t="s">
+        <v>701</v>
+      </c>
+      <c r="N10" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.59886817576564499</v>
-      </c>
-      <c r="C11">
-        <v>0.45684524759052098</v>
-      </c>
-      <c r="D11">
-        <v>0.42145239525939898</v>
-      </c>
-      <c r="E11">
-        <v>0.158372815229117</v>
-      </c>
-      <c r="F11">
-        <v>0.56608929644454897</v>
-      </c>
-      <c r="G11">
-        <v>0.43843570668172299</v>
+      <c r="B11" t="s">
+        <v>637</v>
+      </c>
+      <c r="C11" t="s">
+        <v>638</v>
+      </c>
+      <c r="D11" t="s">
+        <v>639</v>
+      </c>
+      <c r="E11" t="s">
+        <v>640</v>
+      </c>
+      <c r="F11" t="s">
+        <v>641</v>
+      </c>
+      <c r="G11" t="s">
+        <v>642</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.59565615378214198</v>
-      </c>
-      <c r="J11">
-        <v>0.45279439671595401</v>
-      </c>
-      <c r="K11">
-        <v>0.41859804138165901</v>
-      </c>
-      <c r="L11">
-        <v>0.15175985358673499</v>
-      </c>
-      <c r="M11">
-        <v>0.56394853103624398</v>
-      </c>
-      <c r="N11">
-        <v>0.43502522933910598</v>
+      <c r="I11" t="s">
+        <v>703</v>
+      </c>
+      <c r="J11" t="s">
+        <v>704</v>
+      </c>
+      <c r="K11" t="s">
+        <v>705</v>
+      </c>
+      <c r="L11" t="s">
+        <v>706</v>
+      </c>
+      <c r="M11" t="s">
+        <v>707</v>
+      </c>
+      <c r="N11" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.62857856191744299</v>
-      </c>
-      <c r="C12">
-        <v>0.50799868136361703</v>
-      </c>
-      <c r="D12">
-        <v>0.447886022464697</v>
-      </c>
-      <c r="E12">
-        <v>0.210776144631552</v>
-      </c>
-      <c r="F12">
-        <v>0.64130017206961898</v>
-      </c>
-      <c r="G12">
-        <v>0.47605220148836502</v>
+      <c r="B12" t="s">
+        <v>643</v>
+      </c>
+      <c r="C12" t="s">
+        <v>644</v>
+      </c>
+      <c r="D12" t="s">
+        <v>645</v>
+      </c>
+      <c r="E12" t="s">
+        <v>646</v>
+      </c>
+      <c r="F12" t="s">
+        <v>647</v>
+      </c>
+      <c r="G12" t="s">
+        <v>648</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.63526670550053999</v>
-      </c>
-      <c r="J12">
-        <v>0.51537181702636703</v>
-      </c>
-      <c r="K12">
-        <v>0.44705697077232498</v>
-      </c>
-      <c r="L12">
-        <v>0.21792740271379599</v>
-      </c>
-      <c r="M12">
-        <v>0.64843722504773105</v>
-      </c>
-      <c r="N12">
-        <v>0.47878984141407199</v>
+      <c r="I12" t="s">
+        <v>709</v>
+      </c>
+      <c r="J12" t="s">
+        <v>710</v>
+      </c>
+      <c r="K12" t="s">
+        <v>711</v>
+      </c>
+      <c r="L12" t="s">
+        <v>712</v>
+      </c>
+      <c r="M12" t="s">
+        <v>713</v>
+      </c>
+      <c r="N12" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.66885818908122496</v>
-      </c>
-      <c r="C13">
-        <v>0.61385907037862297</v>
-      </c>
-      <c r="D13">
-        <v>0.443678455969647</v>
-      </c>
-      <c r="E13">
-        <v>0.262648817735742</v>
-      </c>
-      <c r="F13">
-        <v>0.698771001299063</v>
-      </c>
-      <c r="G13">
-        <v>0.51507589611313198</v>
+      <c r="B13" t="s">
+        <v>649</v>
+      </c>
+      <c r="C13" t="s">
+        <v>650</v>
+      </c>
+      <c r="D13" t="s">
+        <v>651</v>
+      </c>
+      <c r="E13" t="s">
+        <v>652</v>
+      </c>
+      <c r="F13" t="s">
+        <v>653</v>
+      </c>
+      <c r="G13" t="s">
+        <v>654</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.66930182241823999</v>
-      </c>
-      <c r="J13">
-        <v>0.61588528812543797</v>
-      </c>
-      <c r="K13">
-        <v>0.44028557486258801</v>
-      </c>
-      <c r="L13">
-        <v>0.26201939151986797</v>
-      </c>
-      <c r="M13">
-        <v>0.69753378679446798</v>
-      </c>
-      <c r="N13">
-        <v>0.51348776534993901</v>
+      <c r="I13" t="s">
+        <v>715</v>
+      </c>
+      <c r="J13" t="s">
+        <v>716</v>
+      </c>
+      <c r="K13" t="s">
+        <v>717</v>
+      </c>
+      <c r="L13" t="s">
+        <v>718</v>
+      </c>
+      <c r="M13" t="s">
+        <v>719</v>
+      </c>
+      <c r="N13" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.667776298268974</v>
-      </c>
-      <c r="C14">
-        <v>0.65328224073317498</v>
-      </c>
-      <c r="D14">
-        <v>0.42316760108596602</v>
-      </c>
-      <c r="E14">
-        <v>0.24953926119011999</v>
-      </c>
-      <c r="F14">
-        <v>0.70253147435249796</v>
-      </c>
-      <c r="G14">
-        <v>0.51362890847926601</v>
+      <c r="B14" t="s">
+        <v>655</v>
+      </c>
+      <c r="C14" t="s">
+        <v>656</v>
+      </c>
+      <c r="D14" t="s">
+        <v>657</v>
+      </c>
+      <c r="E14" t="s">
+        <v>658</v>
+      </c>
+      <c r="F14" t="s">
+        <v>659</v>
+      </c>
+      <c r="G14" t="s">
+        <v>660</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.66464175751019305</v>
-      </c>
-      <c r="J14">
-        <v>0.64600801366796401</v>
-      </c>
-      <c r="K14">
-        <v>0.41329343258697798</v>
-      </c>
-      <c r="L14">
-        <v>0.236671974697749</v>
-      </c>
-      <c r="M14">
-        <v>0.69659806151396297</v>
-      </c>
-      <c r="N14">
-        <v>0.50408855834465005</v>
+      <c r="I14" t="s">
+        <v>721</v>
+      </c>
+      <c r="J14" t="s">
+        <v>722</v>
+      </c>
+      <c r="K14" t="s">
+        <v>723</v>
+      </c>
+      <c r="L14" t="s">
+        <v>724</v>
+      </c>
+      <c r="M14" t="s">
+        <v>725</v>
+      </c>
+      <c r="N14" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added TFIDF 2,2 KTKT
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B2BC5-5166-476B-9AE0-A0E2F753167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA01BA-29DD-4B8C-84A3-ECBA170F1422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="871">
   <si>
     <t>TRAINING</t>
   </si>
@@ -95,9 +95,6 @@
     <t>PLS</t>
   </si>
   <si>
-    <t>one seed only</t>
-  </si>
-  <si>
     <t>0.7336±0.0021</t>
   </si>
   <si>
@@ -2214,6 +2211,441 @@
   </si>
   <si>
     <t>0.5563±0.0082</t>
+  </si>
+  <si>
+    <t>0.6859±0.0012</t>
+  </si>
+  <si>
+    <t>0.6596±0.0208</t>
+  </si>
+  <si>
+    <t>0.4708±0.0139</t>
+  </si>
+  <si>
+    <t>0.3151±0.0058</t>
+  </si>
+  <si>
+    <t>0.7201±0.0023</t>
+  </si>
+  <si>
+    <t>0.549±0.0033</t>
+  </si>
+  <si>
+    <t>0.6888±0.0032</t>
+  </si>
+  <si>
+    <t>0.6345±0.0071</t>
+  </si>
+  <si>
+    <t>0.4981±0.0048</t>
+  </si>
+  <si>
+    <t>0.3332±0.0081</t>
+  </si>
+  <si>
+    <t>0.0±0.0</t>
+  </si>
+  <si>
+    <t>0.558±0.0052</t>
+  </si>
+  <si>
+    <t>0.6723±0.0017</t>
+  </si>
+  <si>
+    <t>0.5887±0.0035</t>
+  </si>
+  <si>
+    <t>0.4922±0.0045</t>
+  </si>
+  <si>
+    <t>0.3038±0.0052</t>
+  </si>
+  <si>
+    <t>0.726±0.004</t>
+  </si>
+  <si>
+    <t>0.5362±0.0038</t>
+  </si>
+  <si>
+    <t>0.6663±0.0024</t>
+  </si>
+  <si>
+    <t>0.5748±0.0046</t>
+  </si>
+  <si>
+    <t>0.5009±0.0048</t>
+  </si>
+  <si>
+    <t>0.3027±0.0064</t>
+  </si>
+  <si>
+    <t>0.7156±0.0041</t>
+  </si>
+  <si>
+    <t>0.5353±0.0045</t>
+  </si>
+  <si>
+    <t>0.6625±0.0018</t>
+  </si>
+  <si>
+    <t>0.6939±0.008</t>
+  </si>
+  <si>
+    <t>0.3984±0.0029</t>
+  </si>
+  <si>
+    <t>0.2264±0.0075</t>
+  </si>
+  <si>
+    <t>0.6945±0.0038</t>
+  </si>
+  <si>
+    <t>0.5062±0.0038</t>
+  </si>
+  <si>
+    <t>0.6712±0.0029</t>
+  </si>
+  <si>
+    <t>0.6289±0.0173</t>
+  </si>
+  <si>
+    <t>0.4426±0.0058</t>
+  </si>
+  <si>
+    <t>0.2677±0.0076</t>
+  </si>
+  <si>
+    <t>0.7009±0.0033</t>
+  </si>
+  <si>
+    <t>0.5194±0.0057</t>
+  </si>
+  <si>
+    <t>0.6589±0.0105</t>
+  </si>
+  <si>
+    <t>0.5701±0.0361</t>
+  </si>
+  <si>
+    <t>0.5078±0.0161</t>
+  </si>
+  <si>
+    <t>0.3021±0.0105</t>
+  </si>
+  <si>
+    <t>0.7168±0.0069</t>
+  </si>
+  <si>
+    <t>0.5362±0.0082</t>
+  </si>
+  <si>
+    <t>0.3754±0.1113</t>
+  </si>
+  <si>
+    <t>0.4816±0.0556</t>
+  </si>
+  <si>
+    <t>0.4832±0.0092</t>
+  </si>
+  <si>
+    <t>0.1987±0.051</t>
+  </si>
+  <si>
+    <t>0.5538±0.1947</t>
+  </si>
+  <si>
+    <t>0.4815±0.0297</t>
+  </si>
+  <si>
+    <t>0.5783±0.0814</t>
+  </si>
+  <si>
+    <t>0.4927±0.0403</t>
+  </si>
+  <si>
+    <t>0.4526±0.0165</t>
+  </si>
+  <si>
+    <t>0.2026±0.0435</t>
+  </si>
+  <si>
+    <t>0.6005±0.047</t>
+  </si>
+  <si>
+    <t>0.4716±0.0265</t>
+  </si>
+  <si>
+    <t>0.6359±0.0122</t>
+  </si>
+  <si>
+    <t>0.5275±0.0197</t>
+  </si>
+  <si>
+    <t>0.4871±0.0082</t>
+  </si>
+  <si>
+    <t>0.2599±0.0192</t>
+  </si>
+  <si>
+    <t>0.6487±0.0263</t>
+  </si>
+  <si>
+    <t>0.5065±0.0131</t>
+  </si>
+  <si>
+    <t>0.6885±0.0088</t>
+  </si>
+  <si>
+    <t>0.6479±0.0212</t>
+  </si>
+  <si>
+    <t>0.4903±0.0315</t>
+  </si>
+  <si>
+    <t>0.3282±0.0333</t>
+  </si>
+  <si>
+    <t>0.7459±0.0159</t>
+  </si>
+  <si>
+    <t>0.557±0.0165</t>
+  </si>
+  <si>
+    <t>0.6633±0.0028</t>
+  </si>
+  <si>
+    <t>0.6683±0.0039</t>
+  </si>
+  <si>
+    <t>0.6717±0.0035</t>
+  </si>
+  <si>
+    <t>0.6639±0.0017</t>
+  </si>
+  <si>
+    <t>0.6795±0.0022</t>
+  </si>
+  <si>
+    <t>0.6682±0.0099</t>
+  </si>
+  <si>
+    <t>0.3692±0.1044</t>
+  </si>
+  <si>
+    <t>0.5836±0.081</t>
+  </si>
+  <si>
+    <t>0.641±0.0106</t>
+  </si>
+  <si>
+    <t>0.694±0.0116</t>
+  </si>
+  <si>
+    <t>0.6915±0.0028</t>
+  </si>
+  <si>
+    <t>0.6674±0.0207</t>
+  </si>
+  <si>
+    <t>0.4799±0.0131</t>
+  </si>
+  <si>
+    <t>0.3315±0.0095</t>
+  </si>
+  <si>
+    <t>0.7283±0.0034</t>
+  </si>
+  <si>
+    <t>0.558±0.0059</t>
+  </si>
+  <si>
+    <t>0.5709±0.005</t>
+  </si>
+  <si>
+    <t>0.5168±0.0037</t>
+  </si>
+  <si>
+    <t>0.3135±0.0051</t>
+  </si>
+  <si>
+    <t>0.7127±0.0042</t>
+  </si>
+  <si>
+    <t>0.5425±0.004</t>
+  </si>
+  <si>
+    <t>0.5773±0.0067</t>
+  </si>
+  <si>
+    <t>0.5052±0.0047</t>
+  </si>
+  <si>
+    <t>0.3093±0.0084</t>
+  </si>
+  <si>
+    <t>0.7305±0.0034</t>
+  </si>
+  <si>
+    <t>0.5389±0.0054</t>
+  </si>
+  <si>
+    <t>0.5855±0.0071</t>
+  </si>
+  <si>
+    <t>0.5045±0.0037</t>
+  </si>
+  <si>
+    <t>0.3122±0.0071</t>
+  </si>
+  <si>
+    <t>0.7239±0.0035</t>
+  </si>
+  <si>
+    <t>0.542±0.0048</t>
+  </si>
+  <si>
+    <t>0.7033±0.0141</t>
+  </si>
+  <si>
+    <t>0.3997±0.0027</t>
+  </si>
+  <si>
+    <t>0.2325±0.0073</t>
+  </si>
+  <si>
+    <t>0.7014±0.0041</t>
+  </si>
+  <si>
+    <t>0.5097±0.0051</t>
+  </si>
+  <si>
+    <t>0.6476±0.0072</t>
+  </si>
+  <si>
+    <t>0.4572±0.003</t>
+  </si>
+  <si>
+    <t>0.2938±0.0064</t>
+  </si>
+  <si>
+    <t>0.723±0.003</t>
+  </si>
+  <si>
+    <t>0.536±0.0034</t>
+  </si>
+  <si>
+    <t>0.5859±0.0348</t>
+  </si>
+  <si>
+    <t>0.5084±0.0135</t>
+  </si>
+  <si>
+    <t>0.3125±0.0112</t>
+  </si>
+  <si>
+    <t>0.7195±0.0057</t>
+  </si>
+  <si>
+    <t>0.5436±0.0086</t>
+  </si>
+  <si>
+    <t>0.4847±0.0331</t>
+  </si>
+  <si>
+    <t>0.4901±0.0116</t>
+  </si>
+  <si>
+    <t>0.2042±0.0401</t>
+  </si>
+  <si>
+    <t>0.6344±0.0297</t>
+  </si>
+  <si>
+    <t>0.4872±0.0214</t>
+  </si>
+  <si>
+    <t>0.5004±0.0359</t>
+  </si>
+  <si>
+    <t>0.4604±0.0175</t>
+  </si>
+  <si>
+    <t>0.2143±0.0439</t>
+  </si>
+  <si>
+    <t>0.6054±0.045</t>
+  </si>
+  <si>
+    <t>0.4794±0.0254</t>
+  </si>
+  <si>
+    <t>0.5346±0.0184</t>
+  </si>
+  <si>
+    <t>0.4894±0.0056</t>
+  </si>
+  <si>
+    <t>0.2667±0.015</t>
+  </si>
+  <si>
+    <t>0.6524±0.0253</t>
+  </si>
+  <si>
+    <t>0.5109±0.0111</t>
+  </si>
+  <si>
+    <t>0.6551±0.0154</t>
+  </si>
+  <si>
+    <t>0.4991±0.0357</t>
+  </si>
+  <si>
+    <t>0.3426±0.0418</t>
+  </si>
+  <si>
+    <t>0.7532±0.0188</t>
+  </si>
+  <si>
+    <t>0.5654±0.0218</t>
+  </si>
+  <si>
+    <t>0.6918±0.0071</t>
+  </si>
+  <si>
+    <t>0.6419±0.008</t>
+  </si>
+  <si>
+    <t>0.5008±0.0229</t>
+  </si>
+  <si>
+    <t>0.3402±0.0253</t>
+  </si>
+  <si>
+    <t>0.7488±0.0165</t>
+  </si>
+  <si>
+    <t>0.5623±0.0146</t>
+  </si>
+  <si>
+    <t>0.6977±0.0074</t>
+  </si>
+  <si>
+    <t>0.6575±0.007</t>
+  </si>
+  <si>
+    <t>0.505±0.0192</t>
+  </si>
+  <si>
+    <t>0.3534±0.0241</t>
+  </si>
+  <si>
+    <t>0.7578±0.0118</t>
+  </si>
+  <si>
+    <t>0.5711±0.0138</t>
+  </si>
+  <si>
+    <t>remove prob for faster computation</t>
   </si>
 </sst>
 </file>
@@ -2249,7 +2681,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2259,6 +2691,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2296,7 +2734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2310,6 +2748,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2691,41 +3131,41 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
         <v>165</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>166</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>167</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>168</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>169</v>
-      </c>
-      <c r="G3" t="s">
-        <v>170</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" t="s">
         <v>237</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>238</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>239</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>240</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>241</v>
-      </c>
-      <c r="N3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2733,41 +3173,41 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
         <v>171</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>173</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>174</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>175</v>
-      </c>
-      <c r="G4" t="s">
-        <v>176</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J4" t="s">
         <v>243</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>244</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>245</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>246</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>247</v>
-      </c>
-      <c r="N4" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2775,41 +3215,41 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
         <v>177</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>178</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>179</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>180</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>181</v>
-      </c>
-      <c r="G5" t="s">
-        <v>182</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" t="s">
         <v>249</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>250</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>251</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>252</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>253</v>
-      </c>
-      <c r="N5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2817,41 +3257,41 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
         <v>183</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>184</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>185</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>186</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>187</v>
-      </c>
-      <c r="G6" t="s">
-        <v>188</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
+        <v>254</v>
+      </c>
+      <c r="J6" t="s">
         <v>255</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>256</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>257</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>258</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>259</v>
-      </c>
-      <c r="N6" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2859,41 +3299,41 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" t="s">
         <v>189</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>190</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>191</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>192</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>193</v>
-      </c>
-      <c r="G7" t="s">
-        <v>194</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" t="s">
         <v>261</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>262</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>263</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>264</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>265</v>
-      </c>
-      <c r="N7" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2901,41 +3341,41 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" t="s">
         <v>195</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>196</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>197</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>198</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>199</v>
-      </c>
-      <c r="G8" t="s">
-        <v>200</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
+        <v>266</v>
+      </c>
+      <c r="J8" t="s">
         <v>267</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>268</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>269</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>270</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>271</v>
-      </c>
-      <c r="N8" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2943,41 +3383,41 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>202</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>203</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>204</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>205</v>
-      </c>
-      <c r="G9" t="s">
-        <v>206</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
+        <v>272</v>
+      </c>
+      <c r="J9" t="s">
         <v>273</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>274</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>275</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>276</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>277</v>
-      </c>
-      <c r="N9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2985,41 +3425,41 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="s">
         <v>207</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>208</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>209</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>210</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>211</v>
-      </c>
-      <c r="G10" t="s">
-        <v>212</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
+        <v>278</v>
+      </c>
+      <c r="J10" t="s">
         <v>279</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>280</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>281</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>282</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>283</v>
-      </c>
-      <c r="N10" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3027,41 +3467,41 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" t="s">
         <v>213</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>214</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>215</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>216</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>217</v>
-      </c>
-      <c r="G11" t="s">
-        <v>218</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
+        <v>284</v>
+      </c>
+      <c r="J11" t="s">
         <v>285</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>286</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>287</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>288</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>289</v>
-      </c>
-      <c r="N11" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3069,41 +3509,41 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
         <v>219</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>220</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>221</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>222</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>223</v>
-      </c>
-      <c r="G12" t="s">
-        <v>224</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
+        <v>290</v>
+      </c>
+      <c r="J12" t="s">
         <v>291</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>292</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>293</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>294</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>295</v>
-      </c>
-      <c r="N12" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3111,41 +3551,41 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" t="s">
         <v>225</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>226</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>227</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>228</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>229</v>
-      </c>
-      <c r="G13" t="s">
-        <v>230</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
+        <v>296</v>
+      </c>
+      <c r="J13" t="s">
         <v>297</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>298</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>299</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>300</v>
       </c>
-      <c r="M13" t="s">
-        <v>301</v>
-      </c>
       <c r="N13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3153,41 +3593,41 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" t="s">
         <v>231</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>232</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>233</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>234</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>235</v>
-      </c>
-      <c r="G14" t="s">
-        <v>236</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
+        <v>301</v>
+      </c>
+      <c r="J14" t="s">
         <v>302</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>303</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>304</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>305</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>306</v>
-      </c>
-      <c r="N14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5185,41 +5625,41 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" t="s">
         <v>308</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>309</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>310</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>311</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>312</v>
-      </c>
-      <c r="G3" t="s">
-        <v>313</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" t="s">
+        <v>378</v>
+      </c>
+      <c r="J3" t="s">
         <v>379</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>380</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>381</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>382</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>383</v>
-      </c>
-      <c r="N3" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5227,41 +5667,41 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" t="s">
         <v>314</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>315</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>316</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>317</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>318</v>
-      </c>
-      <c r="G4" t="s">
-        <v>319</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" t="s">
+        <v>384</v>
+      </c>
+      <c r="J4" t="s">
         <v>385</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>386</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>387</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>388</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>389</v>
-      </c>
-      <c r="N4" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5269,41 +5709,41 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" t="s">
         <v>320</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>321</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>322</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>323</v>
-      </c>
-      <c r="G5" t="s">
-        <v>324</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
+        <v>390</v>
+      </c>
+      <c r="J5" t="s">
         <v>391</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>392</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>393</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>394</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>395</v>
-      </c>
-      <c r="N5" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5311,41 +5751,41 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" t="s">
         <v>325</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>326</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>327</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>328</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>329</v>
-      </c>
-      <c r="G6" t="s">
-        <v>330</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" t="s">
         <v>397</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>398</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>399</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>400</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>401</v>
-      </c>
-      <c r="N6" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5353,41 +5793,41 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" t="s">
         <v>331</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>332</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>333</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>334</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>335</v>
-      </c>
-      <c r="G7" t="s">
-        <v>336</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
+        <v>402</v>
+      </c>
+      <c r="J7" t="s">
         <v>403</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>404</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>405</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>406</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>407</v>
-      </c>
-      <c r="N7" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5395,41 +5835,41 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8" t="s">
         <v>337</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>338</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>339</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>340</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>341</v>
-      </c>
-      <c r="G8" t="s">
-        <v>342</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
+        <v>408</v>
+      </c>
+      <c r="J8" t="s">
         <v>409</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>410</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>411</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>412</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>413</v>
-      </c>
-      <c r="N8" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5437,41 +5877,41 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" t="s">
         <v>343</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>344</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>345</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>346</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>347</v>
-      </c>
-      <c r="G9" t="s">
-        <v>348</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
+        <v>414</v>
+      </c>
+      <c r="J9" t="s">
         <v>415</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>416</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>417</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>418</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>419</v>
-      </c>
-      <c r="N9" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5479,41 +5919,41 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" t="s">
         <v>349</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>350</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>351</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>352</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>353</v>
-      </c>
-      <c r="G10" t="s">
-        <v>354</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
+        <v>420</v>
+      </c>
+      <c r="J10" t="s">
         <v>421</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>422</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>423</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>424</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>425</v>
-      </c>
-      <c r="N10" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5521,41 +5961,41 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>354</v>
+      </c>
+      <c r="C11" t="s">
         <v>355</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>356</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>357</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>358</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>359</v>
-      </c>
-      <c r="G11" t="s">
-        <v>360</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J11" t="s">
         <v>427</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>428</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>429</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>430</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>431</v>
-      </c>
-      <c r="N11" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5563,41 +6003,41 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" t="s">
         <v>361</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>362</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>363</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>364</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>365</v>
-      </c>
-      <c r="G12" t="s">
-        <v>366</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
+        <v>432</v>
+      </c>
+      <c r="J12" t="s">
         <v>433</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>434</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>435</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>436</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>437</v>
-      </c>
-      <c r="N12" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5605,41 +6045,41 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" t="s">
         <v>367</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>368</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>369</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>370</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>371</v>
-      </c>
-      <c r="G13" t="s">
-        <v>372</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
+        <v>438</v>
+      </c>
+      <c r="J13" t="s">
         <v>439</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>440</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>441</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>442</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>443</v>
-      </c>
-      <c r="N13" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5647,41 +6087,41 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" t="s">
         <v>373</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>374</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>375</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>376</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>377</v>
-      </c>
-      <c r="G14" t="s">
-        <v>378</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
+        <v>444</v>
+      </c>
+      <c r="J14" t="s">
         <v>445</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>446</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>447</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>448</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>449</v>
-      </c>
-      <c r="N14" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5882,41 +6322,41 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
         <v>93</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>94</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>96</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>97</v>
-      </c>
-      <c r="N3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5924,41 +6364,41 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" t="s">
         <v>99</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>100</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>101</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>102</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>103</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5966,41 +6406,41 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" t="s">
         <v>105</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>106</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>107</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>108</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>109</v>
-      </c>
-      <c r="N5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6008,41 +6448,41 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" t="s">
         <v>111</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>112</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>113</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>114</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>115</v>
-      </c>
-      <c r="N6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6050,41 +6490,41 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" t="s">
         <v>117</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>118</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>119</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>120</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>121</v>
-      </c>
-      <c r="N7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6092,41 +6532,41 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>54</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
         <v>123</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>124</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>125</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>126</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>127</v>
-      </c>
-      <c r="N8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6134,41 +6574,41 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
         <v>57</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
         <v>129</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>130</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>131</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>132</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>133</v>
-      </c>
-      <c r="N9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6176,41 +6616,41 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>66</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>67</v>
-      </c>
-      <c r="G10" t="s">
-        <v>68</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" t="s">
         <v>135</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>136</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>137</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>138</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>139</v>
-      </c>
-      <c r="N10" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6218,41 +6658,41 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>70</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>71</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>72</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" t="s">
         <v>141</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>142</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>143</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>144</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>145</v>
-      </c>
-      <c r="N11" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6260,41 +6700,41 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>78</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>79</v>
-      </c>
-      <c r="G12" t="s">
-        <v>80</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J12" t="s">
         <v>147</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>148</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>149</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>150</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>151</v>
-      </c>
-      <c r="N12" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6302,41 +6742,41 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
         <v>81</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>82</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>83</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>84</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" t="s">
         <v>153</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>154</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>155</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>156</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>157</v>
-      </c>
-      <c r="N13" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6344,41 +6784,41 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>88</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>89</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>90</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>91</v>
-      </c>
-      <c r="G14" t="s">
-        <v>92</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J14" t="s">
         <v>159</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>160</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>161</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>162</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>163</v>
-      </c>
-      <c r="N14" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -6467,41 +6907,41 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" t="s">
         <v>451</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>452</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>453</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>454</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>455</v>
-      </c>
-      <c r="G3" t="s">
-        <v>456</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" t="s">
+        <v>522</v>
+      </c>
+      <c r="J3" t="s">
         <v>523</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>524</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>525</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>526</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>527</v>
-      </c>
-      <c r="N3" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6509,41 +6949,41 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" t="s">
         <v>457</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>458</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>459</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>460</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>461</v>
-      </c>
-      <c r="G4" t="s">
-        <v>462</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" t="s">
+        <v>528</v>
+      </c>
+      <c r="J4" t="s">
         <v>529</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>530</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>531</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>532</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>533</v>
-      </c>
-      <c r="N4" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6551,41 +6991,41 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C5" t="s">
         <v>463</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>464</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>465</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>466</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>467</v>
-      </c>
-      <c r="G5" t="s">
-        <v>468</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
+        <v>534</v>
+      </c>
+      <c r="J5" t="s">
         <v>535</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>536</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>537</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>538</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>539</v>
-      </c>
-      <c r="N5" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6593,41 +7033,41 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" t="s">
         <v>469</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>470</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>471</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>472</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>473</v>
-      </c>
-      <c r="G6" t="s">
-        <v>474</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
+        <v>540</v>
+      </c>
+      <c r="J6" t="s">
         <v>541</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>542</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>543</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>544</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>545</v>
-      </c>
-      <c r="N6" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6635,41 +7075,41 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C7" t="s">
         <v>475</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>476</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>477</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>478</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>479</v>
-      </c>
-      <c r="G7" t="s">
-        <v>480</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
+        <v>546</v>
+      </c>
+      <c r="J7" t="s">
         <v>547</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>548</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>549</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>550</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>551</v>
-      </c>
-      <c r="N7" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6677,41 +7117,41 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C8" t="s">
         <v>481</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>482</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>483</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>484</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>485</v>
-      </c>
-      <c r="G8" t="s">
-        <v>486</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
+        <v>552</v>
+      </c>
+      <c r="J8" t="s">
         <v>553</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>554</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>555</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>556</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>557</v>
-      </c>
-      <c r="N8" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6719,41 +7159,41 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>486</v>
+      </c>
+      <c r="C9" t="s">
         <v>487</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>488</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>489</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>490</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>491</v>
-      </c>
-      <c r="G9" t="s">
-        <v>492</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
+        <v>558</v>
+      </c>
+      <c r="J9" t="s">
         <v>559</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>560</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>561</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>562</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>563</v>
-      </c>
-      <c r="N9" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6761,41 +7201,41 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>492</v>
+      </c>
+      <c r="C10" t="s">
         <v>493</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>494</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>495</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>496</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>497</v>
-      </c>
-      <c r="G10" t="s">
-        <v>498</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
+        <v>564</v>
+      </c>
+      <c r="J10" t="s">
         <v>565</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>566</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>567</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>568</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>569</v>
-      </c>
-      <c r="N10" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6803,41 +7243,41 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>498</v>
+      </c>
+      <c r="C11" t="s">
         <v>499</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>500</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>501</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>502</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>503</v>
-      </c>
-      <c r="G11" t="s">
-        <v>504</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
+        <v>570</v>
+      </c>
+      <c r="J11" t="s">
         <v>571</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>572</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>573</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>574</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>575</v>
-      </c>
-      <c r="N11" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6845,41 +7285,41 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12" t="s">
         <v>505</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>506</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>507</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>508</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>509</v>
-      </c>
-      <c r="G12" t="s">
-        <v>510</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
+        <v>576</v>
+      </c>
+      <c r="J12" t="s">
         <v>577</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>578</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>579</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>580</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>581</v>
-      </c>
-      <c r="N12" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6887,41 +7327,41 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>510</v>
+      </c>
+      <c r="C13" t="s">
         <v>511</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>513</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>514</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>515</v>
-      </c>
-      <c r="G13" t="s">
-        <v>516</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
+        <v>582</v>
+      </c>
+      <c r="J13" t="s">
         <v>583</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>584</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>585</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>586</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>587</v>
-      </c>
-      <c r="N13" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6929,41 +7369,41 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C14" t="s">
         <v>517</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>518</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>519</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>520</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>521</v>
-      </c>
-      <c r="G14" t="s">
-        <v>522</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
+        <v>588</v>
+      </c>
+      <c r="J14" t="s">
         <v>589</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>590</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>591</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>592</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>593</v>
-      </c>
-      <c r="N14" t="s">
-        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -6978,7 +7418,7 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -7059,41 +7499,41 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>594</v>
+      </c>
+      <c r="C3" t="s">
         <v>595</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>596</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>597</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>598</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>599</v>
-      </c>
-      <c r="G3" t="s">
-        <v>600</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" t="s">
+        <v>660</v>
+      </c>
+      <c r="J3" t="s">
         <v>661</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>662</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>663</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>664</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>665</v>
-      </c>
-      <c r="N3" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7119,41 +7559,41 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>600</v>
+      </c>
+      <c r="C5" t="s">
         <v>601</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>602</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>603</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>604</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>605</v>
-      </c>
-      <c r="G5" t="s">
-        <v>606</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
+        <v>666</v>
+      </c>
+      <c r="J5" t="s">
         <v>667</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>668</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>669</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>670</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>671</v>
-      </c>
-      <c r="N5" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7161,41 +7601,41 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>606</v>
+      </c>
+      <c r="C6" t="s">
         <v>607</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>608</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>609</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>610</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>611</v>
-      </c>
-      <c r="G6" t="s">
-        <v>612</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
+        <v>672</v>
+      </c>
+      <c r="J6" t="s">
         <v>673</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>674</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>675</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>676</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>677</v>
-      </c>
-      <c r="N6" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7203,41 +7643,41 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>612</v>
+      </c>
+      <c r="C7" t="s">
         <v>613</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>614</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>615</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>616</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>617</v>
-      </c>
-      <c r="G7" t="s">
-        <v>618</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
+        <v>678</v>
+      </c>
+      <c r="J7" t="s">
         <v>679</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>680</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>681</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>682</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>683</v>
-      </c>
-      <c r="N7" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7245,41 +7685,41 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>618</v>
+      </c>
+      <c r="C8" t="s">
         <v>619</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>620</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>621</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>622</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>623</v>
-      </c>
-      <c r="G8" t="s">
-        <v>624</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
+        <v>684</v>
+      </c>
+      <c r="J8" t="s">
         <v>685</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>686</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>687</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>688</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>689</v>
-      </c>
-      <c r="N8" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7287,41 +7727,41 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>624</v>
+      </c>
+      <c r="C9" t="s">
         <v>625</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>626</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>627</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>628</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>629</v>
-      </c>
-      <c r="G9" t="s">
-        <v>630</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
+        <v>690</v>
+      </c>
+      <c r="J9" t="s">
         <v>691</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>692</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>693</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>694</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>695</v>
-      </c>
-      <c r="N9" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7329,41 +7769,41 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>630</v>
+      </c>
+      <c r="C10" t="s">
         <v>631</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>632</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>633</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>634</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>635</v>
-      </c>
-      <c r="G10" t="s">
-        <v>636</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
+        <v>696</v>
+      </c>
+      <c r="J10" t="s">
         <v>697</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>698</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>699</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>700</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>701</v>
-      </c>
-      <c r="N10" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7371,41 +7811,41 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>636</v>
+      </c>
+      <c r="C11" t="s">
         <v>637</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>638</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>639</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>640</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>641</v>
-      </c>
-      <c r="G11" t="s">
-        <v>642</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
+        <v>702</v>
+      </c>
+      <c r="J11" t="s">
         <v>703</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>704</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>705</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>706</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>707</v>
-      </c>
-      <c r="N11" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7413,41 +7853,41 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>642</v>
+      </c>
+      <c r="C12" t="s">
         <v>643</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>644</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>645</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>646</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>647</v>
-      </c>
-      <c r="G12" t="s">
-        <v>648</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
+        <v>708</v>
+      </c>
+      <c r="J12" t="s">
         <v>709</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>710</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>711</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>712</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>713</v>
-      </c>
-      <c r="N12" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7455,41 +7895,41 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>648</v>
+      </c>
+      <c r="C13" t="s">
         <v>649</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>650</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>651</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>652</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>653</v>
-      </c>
-      <c r="G13" t="s">
-        <v>654</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
+        <v>714</v>
+      </c>
+      <c r="J13" t="s">
         <v>715</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>716</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>717</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>718</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>719</v>
-      </c>
-      <c r="N13" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7497,41 +7937,41 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>654</v>
+      </c>
+      <c r="C14" t="s">
         <v>655</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>656</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>657</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>658</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>659</v>
-      </c>
-      <c r="G14" t="s">
-        <v>660</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
+        <v>720</v>
+      </c>
+      <c r="J14" t="s">
         <v>721</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>722</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>723</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>724</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>725</v>
-      </c>
-      <c r="N14" t="s">
-        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -7544,10 +7984,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7563,9 +8003,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -7575,9 +8013,7 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="J1" s="6"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -7627,504 +8063,509 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>0.66636151797603105</v>
-      </c>
-      <c r="C3">
-        <v>0.61842543810539197</v>
-      </c>
-      <c r="D3">
-        <v>0.429114094021255</v>
-      </c>
-      <c r="E3">
-        <v>0.24860754266985999</v>
-      </c>
-      <c r="F3">
-        <v>0.65916604760306796</v>
-      </c>
-      <c r="G3">
-        <v>0.50666359302649999</v>
+      <c r="B3" t="s">
+        <v>726</v>
+      </c>
+      <c r="C3" t="s">
+        <v>727</v>
+      </c>
+      <c r="D3" t="s">
+        <v>728</v>
+      </c>
+      <c r="E3" t="s">
+        <v>729</v>
+      </c>
+      <c r="F3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G3" t="s">
+        <v>731</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3">
-        <v>0.67387867188150097</v>
-      </c>
-      <c r="J3">
-        <v>0.63895504435202299</v>
-      </c>
-      <c r="K3">
-        <v>0.44588321145986098</v>
-      </c>
-      <c r="L3">
-        <v>0.27500072178981599</v>
-      </c>
-      <c r="M3">
-        <v>0.67094854179701302</v>
-      </c>
-      <c r="N3">
-        <v>0.52523834890195997</v>
+      <c r="I3" t="s">
+        <v>802</v>
+      </c>
+      <c r="J3" t="s">
+        <v>803</v>
+      </c>
+      <c r="K3" t="s">
+        <v>804</v>
+      </c>
+      <c r="L3" t="s">
+        <v>805</v>
+      </c>
+      <c r="M3" t="s">
+        <v>806</v>
+      </c>
+      <c r="N3" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.66952396804260905</v>
-      </c>
-      <c r="C4">
-        <v>0.61370863930507902</v>
-      </c>
-      <c r="D4">
-        <v>0.44488550493210499</v>
-      </c>
-      <c r="E4">
-        <v>0.26500229649323798</v>
-      </c>
-      <c r="F4">
-        <v>0.68251849731966696</v>
-      </c>
-      <c r="G4">
-        <v>0.51583523178314805</v>
+      <c r="B4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D4" t="s">
+        <v>734</v>
+      </c>
+      <c r="E4" t="s">
+        <v>735</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="G4" t="s">
+        <v>737</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <v>0.67138220853790398</v>
-      </c>
-      <c r="J4">
-        <v>0.61252897338582002</v>
-      </c>
-      <c r="K4">
-        <v>0.45780184077647801</v>
-      </c>
-      <c r="L4">
-        <v>0.27629770520650199</v>
-      </c>
-      <c r="M4">
-        <v>0.69038004293155497</v>
-      </c>
-      <c r="N4">
-        <v>0.52398172197709803</v>
+      <c r="I4" t="s">
+        <v>792</v>
+      </c>
+      <c r="J4" t="s">
+        <v>808</v>
+      </c>
+      <c r="K4" t="s">
+        <v>809</v>
+      </c>
+      <c r="L4" t="s">
+        <v>810</v>
+      </c>
+      <c r="M4" t="s">
+        <v>811</v>
+      </c>
+      <c r="N4" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.65570905459387396</v>
-      </c>
-      <c r="C5">
-        <v>0.55692447901986197</v>
-      </c>
-      <c r="D5">
-        <v>0.44016985711446399</v>
-      </c>
-      <c r="E5">
-        <v>0.23773782586126399</v>
-      </c>
-      <c r="F5">
-        <v>0.680022141979858</v>
-      </c>
-      <c r="G5">
-        <v>0.491711485001746</v>
+      <c r="B5" t="s">
+        <v>738</v>
+      </c>
+      <c r="C5" t="s">
+        <v>739</v>
+      </c>
+      <c r="D5" t="s">
+        <v>740</v>
+      </c>
+      <c r="E5" t="s">
+        <v>741</v>
+      </c>
+      <c r="F5" t="s">
+        <v>742</v>
+      </c>
+      <c r="G5" t="s">
+        <v>743</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <v>0.65815095281684199</v>
-      </c>
-      <c r="J5">
-        <v>0.568535878837513</v>
-      </c>
-      <c r="K5">
-        <v>0.447506427807635</v>
-      </c>
-      <c r="L5">
-        <v>0.24642339585818601</v>
-      </c>
-      <c r="M5">
-        <v>0.69316479115688401</v>
-      </c>
-      <c r="N5">
-        <v>0.50081272906662</v>
+      <c r="I5" t="s">
+        <v>793</v>
+      </c>
+      <c r="J5" t="s">
+        <v>813</v>
+      </c>
+      <c r="K5" t="s">
+        <v>814</v>
+      </c>
+      <c r="L5" t="s">
+        <v>815</v>
+      </c>
+      <c r="M5" t="s">
+        <v>816</v>
+      </c>
+      <c r="N5" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0.65188082556591198</v>
-      </c>
-      <c r="C6">
-        <v>0.545216975089164</v>
-      </c>
-      <c r="D6">
-        <v>0.44517106195682699</v>
-      </c>
-      <c r="E6">
-        <v>0.23717132950921099</v>
-      </c>
-      <c r="F6">
-        <v>0.67465198517518998</v>
-      </c>
-      <c r="G6">
-        <v>0.490140855338423</v>
+      <c r="B6" t="s">
+        <v>744</v>
+      </c>
+      <c r="C6" t="s">
+        <v>745</v>
+      </c>
+      <c r="D6" t="s">
+        <v>746</v>
+      </c>
+      <c r="E6" t="s">
+        <v>747</v>
+      </c>
+      <c r="F6" t="s">
+        <v>748</v>
+      </c>
+      <c r="G6" t="s">
+        <v>749</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <v>0.65540484313888603</v>
-      </c>
-      <c r="J6">
-        <v>0.56008812346927705</v>
-      </c>
-      <c r="K6">
-        <v>0.45205151322116199</v>
-      </c>
-      <c r="L6">
-        <v>0.246105779831051</v>
-      </c>
-      <c r="M6">
-        <v>0.68825763429401798</v>
-      </c>
-      <c r="N6">
-        <v>0.50030386040286101</v>
+      <c r="I6" t="s">
+        <v>794</v>
+      </c>
+      <c r="J6" t="s">
+        <v>818</v>
+      </c>
+      <c r="K6" t="s">
+        <v>819</v>
+      </c>
+      <c r="L6" t="s">
+        <v>820</v>
+      </c>
+      <c r="M6" t="s">
+        <v>821</v>
+      </c>
+      <c r="N6" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>0.661118508655126</v>
-      </c>
-      <c r="C7">
-        <v>0.67847658987497905</v>
-      </c>
-      <c r="D7">
-        <v>0.39770443470585898</v>
-      </c>
-      <c r="E7">
-        <v>0.22101995292867799</v>
-      </c>
-      <c r="F7">
-        <v>0.673252986575965</v>
-      </c>
-      <c r="G7">
-        <v>0.50146423784508698</v>
+      <c r="B7" t="s">
+        <v>750</v>
+      </c>
+      <c r="C7" t="s">
+        <v>751</v>
+      </c>
+      <c r="D7" t="s">
+        <v>752</v>
+      </c>
+      <c r="E7" t="s">
+        <v>753</v>
+      </c>
+      <c r="F7" t="s">
+        <v>754</v>
+      </c>
+      <c r="G7" t="s">
+        <v>755</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <v>0.66089706249479896</v>
-      </c>
-      <c r="J7">
-        <v>0.67578142963284804</v>
-      </c>
-      <c r="K7">
-        <v>0.39763205302369797</v>
-      </c>
-      <c r="L7">
-        <v>0.22025656868101001</v>
-      </c>
-      <c r="M7">
-        <v>0.68606089808728299</v>
-      </c>
-      <c r="N7">
-        <v>0.50066886917644104</v>
+      <c r="I7" t="s">
+        <v>795</v>
+      </c>
+      <c r="J7" t="s">
+        <v>823</v>
+      </c>
+      <c r="K7" t="s">
+        <v>824</v>
+      </c>
+      <c r="L7" t="s">
+        <v>825</v>
+      </c>
+      <c r="M7" t="s">
+        <v>826</v>
+      </c>
+      <c r="N7" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.67235352862849496</v>
-      </c>
-      <c r="C8">
-        <v>0.62371793760384597</v>
-      </c>
-      <c r="D8">
-        <v>0.44716046297354001</v>
-      </c>
-      <c r="E8">
-        <v>0.27265354127031999</v>
-      </c>
-      <c r="F8">
-        <v>0.69603163774640497</v>
-      </c>
-      <c r="G8">
-        <v>0.52088454038005005</v>
+      <c r="B8" t="s">
+        <v>756</v>
+      </c>
+      <c r="C8" t="s">
+        <v>757</v>
+      </c>
+      <c r="D8" t="s">
+        <v>758</v>
+      </c>
+      <c r="E8" t="s">
+        <v>759</v>
+      </c>
+      <c r="F8" t="s">
+        <v>760</v>
+      </c>
+      <c r="G8" t="s">
+        <v>761</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8">
-        <v>0.67554298077723196</v>
-      </c>
-      <c r="J8">
-        <v>0.634764399659411</v>
-      </c>
-      <c r="K8">
-        <v>0.45199953582610197</v>
-      </c>
-      <c r="L8">
-        <v>0.28216582688710001</v>
-      </c>
-      <c r="M8">
-        <v>0.712469698324254</v>
-      </c>
-      <c r="N8">
-        <v>0.52801386692466801</v>
+      <c r="I8" t="s">
+        <v>796</v>
+      </c>
+      <c r="J8" t="s">
+        <v>828</v>
+      </c>
+      <c r="K8" t="s">
+        <v>829</v>
+      </c>
+      <c r="L8" t="s">
+        <v>830</v>
+      </c>
+      <c r="M8" t="s">
+        <v>831</v>
+      </c>
+      <c r="N8" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0.65346205059920104</v>
-      </c>
-      <c r="C9">
-        <v>0.55503900604202105</v>
-      </c>
-      <c r="D9">
-        <v>0.45304330133257298</v>
-      </c>
-      <c r="E9">
-        <v>0.24409863688601199</v>
-      </c>
-      <c r="F9">
-        <v>0.66982124913301</v>
-      </c>
-      <c r="G9">
-        <v>0.49888129535872899</v>
+      <c r="B9" t="s">
+        <v>762</v>
+      </c>
+      <c r="C9" t="s">
+        <v>763</v>
+      </c>
+      <c r="D9" t="s">
+        <v>764</v>
+      </c>
+      <c r="E9" t="s">
+        <v>765</v>
+      </c>
+      <c r="F9" t="s">
+        <v>766</v>
+      </c>
+      <c r="G9" t="s">
+        <v>767</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <v>0.651327286344345</v>
-      </c>
-      <c r="J9">
-        <v>0.55130032592508704</v>
-      </c>
-      <c r="K9">
-        <v>0.46756330715026301</v>
-      </c>
-      <c r="L9">
-        <v>0.25405181781526598</v>
-      </c>
-      <c r="M9">
-        <v>0.686495048654304</v>
-      </c>
-      <c r="N9">
-        <v>0.50599078277924603</v>
+      <c r="I9" t="s">
+        <v>797</v>
+      </c>
+      <c r="J9" t="s">
+        <v>833</v>
+      </c>
+      <c r="K9" t="s">
+        <v>834</v>
+      </c>
+      <c r="L9" t="s">
+        <v>835</v>
+      </c>
+      <c r="M9" t="s">
+        <v>836</v>
+      </c>
+      <c r="N9" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0.67085552596537901</v>
-      </c>
-      <c r="C10">
-        <v>0.63556217176950303</v>
-      </c>
-      <c r="D10">
-        <v>0.43264649304657399</v>
-      </c>
-      <c r="E10">
-        <v>0.26200466711903297</v>
-      </c>
-      <c r="F10">
-        <v>0.70086730057860802</v>
-      </c>
-      <c r="G10">
-        <v>0.51483151894575696</v>
+      <c r="B10" t="s">
+        <v>768</v>
+      </c>
+      <c r="C10" t="s">
+        <v>769</v>
+      </c>
+      <c r="D10" t="s">
+        <v>770</v>
+      </c>
+      <c r="E10" t="s">
+        <v>771</v>
+      </c>
+      <c r="F10" t="s">
+        <v>772</v>
+      </c>
+      <c r="G10" t="s">
+        <v>773</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <v>0.67645835066988402</v>
-      </c>
-      <c r="J10">
-        <v>0.64907597154401098</v>
-      </c>
-      <c r="K10">
-        <v>0.44599844292319102</v>
-      </c>
-      <c r="L10">
-        <v>0.28171584453283799</v>
-      </c>
-      <c r="M10">
-        <v>0.71695920619331099</v>
-      </c>
-      <c r="N10">
-        <v>0.52870721628234396</v>
+      <c r="I10" t="s">
+        <v>798</v>
+      </c>
+      <c r="J10" t="s">
+        <v>838</v>
+      </c>
+      <c r="K10" t="s">
+        <v>839</v>
+      </c>
+      <c r="L10" t="s">
+        <v>840</v>
+      </c>
+      <c r="M10" t="s">
+        <v>841</v>
+      </c>
+      <c r="N10" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>0.60818908122503301</v>
-      </c>
-      <c r="C11">
-        <v>0.466035892315457</v>
-      </c>
-      <c r="D11">
-        <v>0.41897103934264002</v>
-      </c>
-      <c r="E11">
-        <v>0.16027253710258799</v>
-      </c>
-      <c r="F11">
-        <v>0.56422827950697996</v>
-      </c>
-      <c r="G11">
-        <v>0.441252006486689</v>
+      <c r="B11" t="s">
+        <v>774</v>
+      </c>
+      <c r="C11" t="s">
+        <v>775</v>
+      </c>
+      <c r="D11" t="s">
+        <v>776</v>
+      </c>
+      <c r="E11" t="s">
+        <v>777</v>
+      </c>
+      <c r="F11" t="s">
+        <v>778</v>
+      </c>
+      <c r="G11" t="s">
+        <v>779</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <v>0.60647416160439305</v>
-      </c>
-      <c r="J11">
-        <v>0.46986679861337799</v>
-      </c>
-      <c r="K11">
-        <v>0.426062069597337</v>
-      </c>
-      <c r="L11">
-        <v>0.16642250342071599</v>
-      </c>
-      <c r="M11">
-        <v>0.56954655219800299</v>
-      </c>
-      <c r="N11">
-        <v>0.44689355986954798</v>
+      <c r="I11" t="s">
+        <v>799</v>
+      </c>
+      <c r="J11" t="s">
+        <v>843</v>
+      </c>
+      <c r="K11" t="s">
+        <v>844</v>
+      </c>
+      <c r="L11" t="s">
+        <v>845</v>
+      </c>
+      <c r="M11" t="s">
+        <v>846</v>
+      </c>
+      <c r="N11" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0.63057589880159703</v>
-      </c>
-      <c r="C12">
-        <v>0.50526534776828702</v>
-      </c>
-      <c r="D12">
-        <v>0.44174339284298803</v>
-      </c>
-      <c r="E12">
-        <v>0.208407132474695</v>
-      </c>
-      <c r="F12">
-        <v>0.61776360244639805</v>
-      </c>
-      <c r="G12">
-        <v>0.47137395767875601</v>
+      <c r="B12" t="s">
+        <v>780</v>
+      </c>
+      <c r="C12" t="s">
+        <v>781</v>
+      </c>
+      <c r="D12" t="s">
+        <v>782</v>
+      </c>
+      <c r="E12" t="s">
+        <v>783</v>
+      </c>
+      <c r="F12" t="s">
+        <v>784</v>
+      </c>
+      <c r="G12" t="s">
+        <v>785</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <v>0.63052342514770698</v>
-      </c>
-      <c r="J12">
-        <v>0.50845349484278801</v>
-      </c>
-      <c r="K12">
-        <v>0.446348666432763</v>
-      </c>
-      <c r="L12">
-        <v>0.21195516935738701</v>
-      </c>
-      <c r="M12">
-        <v>0.62810872024247499</v>
-      </c>
-      <c r="N12">
-        <v>0.47538128540255797</v>
+      <c r="I12" t="s">
+        <v>800</v>
+      </c>
+      <c r="J12" t="s">
+        <v>848</v>
+      </c>
+      <c r="K12" t="s">
+        <v>849</v>
+      </c>
+      <c r="L12" t="s">
+        <v>850</v>
+      </c>
+      <c r="M12" t="s">
+        <v>851</v>
+      </c>
+      <c r="N12" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0.67127163781624499</v>
-      </c>
-      <c r="C13">
-        <v>0.62181432025689298</v>
-      </c>
-      <c r="D13">
-        <v>0.44829773632443398</v>
-      </c>
-      <c r="E13">
-        <v>0.27031324135002699</v>
-      </c>
-      <c r="F13">
-        <v>0.69951526866832203</v>
-      </c>
-      <c r="G13">
-        <v>0.520988340372178</v>
+      <c r="B13" t="s">
+        <v>786</v>
+      </c>
+      <c r="C13" t="s">
+        <v>787</v>
+      </c>
+      <c r="D13" t="s">
+        <v>788</v>
+      </c>
+      <c r="E13" t="s">
+        <v>789</v>
+      </c>
+      <c r="F13" t="s">
+        <v>790</v>
+      </c>
+      <c r="G13" t="s">
+        <v>791</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <v>0.67562619622201803</v>
-      </c>
-      <c r="J13">
-        <v>0.62499363054930401</v>
-      </c>
-      <c r="K13">
-        <v>0.45896175829639402</v>
-      </c>
-      <c r="L13">
-        <v>0.28603796526252401</v>
-      </c>
-      <c r="M13">
-        <v>0.71604386700423395</v>
-      </c>
-      <c r="N13">
-        <v>0.52926195773872098</v>
+      <c r="I13" t="s">
+        <v>801</v>
+      </c>
+      <c r="J13" t="s">
+        <v>853</v>
+      </c>
+      <c r="K13" t="s">
+        <v>854</v>
+      </c>
+      <c r="L13" t="s">
+        <v>855</v>
+      </c>
+      <c r="M13" t="s">
+        <v>856</v>
+      </c>
+      <c r="N13" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0.66960719041278205</v>
-      </c>
-      <c r="C14">
-        <v>0.62614515887394995</v>
-      </c>
-      <c r="D14">
-        <v>0.432753195974867</v>
-      </c>
-      <c r="E14">
-        <v>0.25903916301749902</v>
-      </c>
-      <c r="F14">
-        <v>0.70250543388277897</v>
-      </c>
-      <c r="G14">
-        <v>0.51178910120335397</v>
+      <c r="B14" t="s">
+        <v>858</v>
+      </c>
+      <c r="C14" t="s">
+        <v>859</v>
+      </c>
+      <c r="D14" t="s">
+        <v>860</v>
+      </c>
+      <c r="E14" t="s">
+        <v>861</v>
+      </c>
+      <c r="F14" t="s">
+        <v>862</v>
+      </c>
+      <c r="G14" t="s">
+        <v>863</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <v>0.67687442789381702</v>
-      </c>
-      <c r="J14">
-        <v>0.64886857996486302</v>
-      </c>
-      <c r="K14">
-        <v>0.44561042675796397</v>
-      </c>
-      <c r="L14">
-        <v>0.28292371405191802</v>
-      </c>
-      <c r="M14">
-        <v>0.71396400202702903</v>
-      </c>
-      <c r="N14">
-        <v>0.528365739410114</v>
+      <c r="I14" t="s">
+        <v>864</v>
+      </c>
+      <c r="J14" t="s">
+        <v>865</v>
+      </c>
+      <c r="K14" t="s">
+        <v>866</v>
+      </c>
+      <c r="L14" t="s">
+        <v>867</v>
+      </c>
+      <c r="M14" t="s">
+        <v>868</v>
+      </c>
+      <c r="N14" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added W2V results kt.
</commit_message>
<xml_diff>
--- a/output/KTKT.xlsx
+++ b/output/KTKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED76795-EF6E-41C6-BC64-9CE19B94E6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2516D5CF-1621-42A8-9D0A-7F4253998B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="796" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="796" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1450">
   <si>
     <t>TRAINING</t>
   </si>
@@ -3534,6 +3534,855 @@
   </si>
   <si>
     <t>0.1631±0.0825</t>
+  </si>
+  <si>
+    <t>0.7545±0.0017</t>
+  </si>
+  <si>
+    <t>0.7235±0.0063</t>
+  </si>
+  <si>
+    <t>0.6123±0.0094</t>
+  </si>
+  <si>
+    <t>0.5±0.0055</t>
+  </si>
+  <si>
+    <t>0.8402±0.0013</t>
+  </si>
+  <si>
+    <t>0.6632±0.0042</t>
+  </si>
+  <si>
+    <t>0.7121±0.0025</t>
+  </si>
+  <si>
+    <t>0.6776±0.0056</t>
+  </si>
+  <si>
+    <t>0.522±0.0053</t>
+  </si>
+  <si>
+    <t>0.3903±0.0067</t>
+  </si>
+  <si>
+    <t>0.7923±0.0017</t>
+  </si>
+  <si>
+    <t>0.7018±0.0031</t>
+  </si>
+  <si>
+    <t>0.7217±0.0066</t>
+  </si>
+  <si>
+    <t>0.4762±0.0059</t>
+  </si>
+  <si>
+    <t>0.3581±0.0093</t>
+  </si>
+  <si>
+    <t>0.7826±0.0069</t>
+  </si>
+  <si>
+    <t>0.5738±0.006</t>
+  </si>
+  <si>
+    <t>0.6951±0.0025</t>
+  </si>
+  <si>
+    <t>0.7392±0.0075</t>
+  </si>
+  <si>
+    <t>0.4581±0.0046</t>
+  </si>
+  <si>
+    <t>0.3398±0.0079</t>
+  </si>
+  <si>
+    <t>0.796±0.0063</t>
+  </si>
+  <si>
+    <t>0.5656±0.0052</t>
+  </si>
+  <si>
+    <t>0.7354±0.0029</t>
+  </si>
+  <si>
+    <t>0.6955±0.0047</t>
+  </si>
+  <si>
+    <t>0.5788±0.0048</t>
+  </si>
+  <si>
+    <t>0.4547±0.0067</t>
+  </si>
+  <si>
+    <t>0.8403±0.0032</t>
+  </si>
+  <si>
+    <t>0.6318±0.0045</t>
+  </si>
+  <si>
+    <t>0.6911±0.0055</t>
+  </si>
+  <si>
+    <t>0.5827±0.0051</t>
+  </si>
+  <si>
+    <t>0.4562±0.0067</t>
+  </si>
+  <si>
+    <t>0.8398±0.0031</t>
+  </si>
+  <si>
+    <t>0.6323±0.0047</t>
+  </si>
+  <si>
+    <t>0.7183±0.0029</t>
+  </si>
+  <si>
+    <t>0.6464±0.0036</t>
+  </si>
+  <si>
+    <t>0.6198±0.0079</t>
+  </si>
+  <si>
+    <t>0.4518±0.0078</t>
+  </si>
+  <si>
+    <t>0.8303±0.0032</t>
+  </si>
+  <si>
+    <t>0.6328±0.0049</t>
+  </si>
+  <si>
+    <t>0.4833±0.0059</t>
+  </si>
+  <si>
+    <t>0.5179±0.0061</t>
+  </si>
+  <si>
+    <t>0.5241±0.0063</t>
+  </si>
+  <si>
+    <t>0.2624±0.0085</t>
+  </si>
+  <si>
+    <t>0.7176±0.0052</t>
+  </si>
+  <si>
+    <t>0.521±0.006</t>
+  </si>
+  <si>
+    <t>0.6205±0.0033</t>
+  </si>
+  <si>
+    <t>0.5334±0.003</t>
+  </si>
+  <si>
+    <t>0.5476±0.0032</t>
+  </si>
+  <si>
+    <t>0.3107±0.0049</t>
+  </si>
+  <si>
+    <t>0.6607±0.0024</t>
+  </si>
+  <si>
+    <t>0.5404±0.0029</t>
+  </si>
+  <si>
+    <t>0.555±0.0047</t>
+  </si>
+  <si>
+    <t>0.4465±0.0061</t>
+  </si>
+  <si>
+    <t>0.4519±0.0067</t>
+  </si>
+  <si>
+    <t>0.18±0.0089</t>
+  </si>
+  <si>
+    <t>0.5889±0.0051</t>
+  </si>
+  <si>
+    <t>0.4492±0.0064</t>
+  </si>
+  <si>
+    <t>0.7129±0.0026</t>
+  </si>
+  <si>
+    <t>0.6582±0.0039</t>
+  </si>
+  <si>
+    <t>0.5502±0.0057</t>
+  </si>
+  <si>
+    <t>0.4029±0.007</t>
+  </si>
+  <si>
+    <t>0.8184±0.0017</t>
+  </si>
+  <si>
+    <t>0.5994±0.0043</t>
+  </si>
+  <si>
+    <t>0.6894±0.0026</t>
+  </si>
+  <si>
+    <t>0.6442±0.0065</t>
+  </si>
+  <si>
+    <t>0.4745±0.0049</t>
+  </si>
+  <si>
+    <t>0.325±0.0077</t>
+  </si>
+  <si>
+    <t>0.7804±0.0028</t>
+  </si>
+  <si>
+    <t>0.5465±0.0051</t>
+  </si>
+  <si>
+    <t>0.7601±0.0026</t>
+  </si>
+  <si>
+    <t>0.7326±0.0086</t>
+  </si>
+  <si>
+    <t>0.6213±0.0093</t>
+  </si>
+  <si>
+    <t>0.5127±0.0061</t>
+  </si>
+  <si>
+    <t>0.8452±0.0022</t>
+  </si>
+  <si>
+    <t>0.6723±0.0049</t>
+  </si>
+  <si>
+    <t>0.7115±0.0031</t>
+  </si>
+  <si>
+    <t>0.6784±0.0062</t>
+  </si>
+  <si>
+    <t>0.5192±0.0053</t>
+  </si>
+  <si>
+    <t>0.3883±0.0082</t>
+  </si>
+  <si>
+    <t>0.7919±0.003</t>
+  </si>
+  <si>
+    <t>0.5882±0.0054</t>
+  </si>
+  <si>
+    <t>0.7044±0.0015</t>
+  </si>
+  <si>
+    <t>0.7287±0.0072</t>
+  </si>
+  <si>
+    <t>0.4805±0.0023</t>
+  </si>
+  <si>
+    <t>0.366±0.0042</t>
+  </si>
+  <si>
+    <t>0.7878±0.0051</t>
+  </si>
+  <si>
+    <t>0.5791±0.0028</t>
+  </si>
+  <si>
+    <t>0.6972±0.0029</t>
+  </si>
+  <si>
+    <t>0.7406±0.0128</t>
+  </si>
+  <si>
+    <t>0.4617±0.0044</t>
+  </si>
+  <si>
+    <t>0.3464±0.0091</t>
+  </si>
+  <si>
+    <t>0.7994±0.0044</t>
+  </si>
+  <si>
+    <t>0.5687±0.0062</t>
+  </si>
+  <si>
+    <t>0.7378±0.0026</t>
+  </si>
+  <si>
+    <t>0.6986±0.0063</t>
+  </si>
+  <si>
+    <t>0.5829±0.0039</t>
+  </si>
+  <si>
+    <t>0.4605±0.0058</t>
+  </si>
+  <si>
+    <t>0.8435±0.0017</t>
+  </si>
+  <si>
+    <t>0.6355±0.0043</t>
+  </si>
+  <si>
+    <t>0.7385±0.0021</t>
+  </si>
+  <si>
+    <t>0.6965±0.0054</t>
+  </si>
+  <si>
+    <t>0.5869±0.0035</t>
+  </si>
+  <si>
+    <t>0.4632±0.0047</t>
+  </si>
+  <si>
+    <t>0.8427±0.0011</t>
+  </si>
+  <si>
+    <t>0.637±0.0036</t>
+  </si>
+  <si>
+    <t>0.7306±0.0053</t>
+  </si>
+  <si>
+    <t>0.6649±0.0077</t>
+  </si>
+  <si>
+    <t>0.631±0.007</t>
+  </si>
+  <si>
+    <t>0.4727±0.0099</t>
+  </si>
+  <si>
+    <t>0.8423±0.0036</t>
+  </si>
+  <si>
+    <t>0.6475±0.0064</t>
+  </si>
+  <si>
+    <t>0.4847±0.0032</t>
+  </si>
+  <si>
+    <t>0.5188±0.0031</t>
+  </si>
+  <si>
+    <t>0.5246±0.0032</t>
+  </si>
+  <si>
+    <t>0.2637±0.0041</t>
+  </si>
+  <si>
+    <t>0.7172±0.0039</t>
+  </si>
+  <si>
+    <t>0.5217±0.0029</t>
+  </si>
+  <si>
+    <t>0.5361±0.0047</t>
+  </si>
+  <si>
+    <t>0.5511±0.0056</t>
+  </si>
+  <si>
+    <t>0.3154±0.0075</t>
+  </si>
+  <si>
+    <t>0.6633±0.0042</t>
+  </si>
+  <si>
+    <t>0.5435±0.0052</t>
+  </si>
+  <si>
+    <t>0.56±0.0037</t>
+  </si>
+  <si>
+    <t>0.4511±0.0041</t>
+  </si>
+  <si>
+    <t>0.4561±0.0043</t>
+  </si>
+  <si>
+    <t>0.1871±0.0062</t>
+  </si>
+  <si>
+    <t>0.5921±0.0032</t>
+  </si>
+  <si>
+    <t>0.4536±0.0042</t>
+  </si>
+  <si>
+    <t>0.7124±0.0026</t>
+  </si>
+  <si>
+    <t>0.6568±0.0048</t>
+  </si>
+  <si>
+    <t>0.5496±0.0057</t>
+  </si>
+  <si>
+    <t>0.4019±0.0067</t>
+  </si>
+  <si>
+    <t>0.8188±0.0027</t>
+  </si>
+  <si>
+    <t>0.5984±0.005</t>
+  </si>
+  <si>
+    <t>0.6903±0.0029</t>
+  </si>
+  <si>
+    <t>0.6463±0.0094</t>
+  </si>
+  <si>
+    <t>0.4761±0.0051</t>
+  </si>
+  <si>
+    <t>0.3276±0.0083</t>
+  </si>
+  <si>
+    <t>0.7809±0.0037</t>
+  </si>
+  <si>
+    <t>0.5483±0.0064</t>
+  </si>
+  <si>
+    <t>0.7429±0.0029</t>
+  </si>
+  <si>
+    <t>0.7136±0.0073</t>
+  </si>
+  <si>
+    <t>0.5871±0.0118</t>
+  </si>
+  <si>
+    <t>0.4711±0.0084</t>
+  </si>
+  <si>
+    <t>0.8253±0.0025</t>
+  </si>
+  <si>
+    <t>0.6441±0.0062</t>
+  </si>
+  <si>
+    <t>0.7119±0.0027</t>
+  </si>
+  <si>
+    <t>0.6699±0.0057</t>
+  </si>
+  <si>
+    <t>0.526±0.0054</t>
+  </si>
+  <si>
+    <t>0.3916±0.0071</t>
+  </si>
+  <si>
+    <t>0.7846±0.0031</t>
+  </si>
+  <si>
+    <t>0.5893±0.0048</t>
+  </si>
+  <si>
+    <t>0.6922±0.003</t>
+  </si>
+  <si>
+    <t>0.6961±0.0122</t>
+  </si>
+  <si>
+    <t>0.4604±0.0042</t>
+  </si>
+  <si>
+    <t>0.3295±0.0093</t>
+  </si>
+  <si>
+    <t>0.7646±0.0062</t>
+  </si>
+  <si>
+    <t>0.5542±0.0064</t>
+  </si>
+  <si>
+    <t>0.6861±0.0028</t>
+  </si>
+  <si>
+    <t>0.7029±0.0147</t>
+  </si>
+  <si>
+    <t>0.4447±0.0056</t>
+  </si>
+  <si>
+    <t>0.3107±0.0092</t>
+  </si>
+  <si>
+    <t>0.7721±0.0109</t>
+  </si>
+  <si>
+    <t>0.5447±0.0063</t>
+  </si>
+  <si>
+    <t>0.7207±0.0034</t>
+  </si>
+  <si>
+    <t>0.6754±0.0058</t>
+  </si>
+  <si>
+    <t>0.553±0.0051</t>
+  </si>
+  <si>
+    <t>0.4183±0.0081</t>
+  </si>
+  <si>
+    <t>0.8211±0.0034</t>
+  </si>
+  <si>
+    <t>0.6081±0.0053</t>
+  </si>
+  <si>
+    <t>0.7228±0.0032</t>
+  </si>
+  <si>
+    <t>0.6761±0.0057</t>
+  </si>
+  <si>
+    <t>0.5572±0.0038</t>
+  </si>
+  <si>
+    <t>0.424±0.0073</t>
+  </si>
+  <si>
+    <t>0.8208±0.004</t>
+  </si>
+  <si>
+    <t>0.6109±0.0043</t>
+  </si>
+  <si>
+    <t>0.7074±0.0059</t>
+  </si>
+  <si>
+    <t>0.6319±0.0094</t>
+  </si>
+  <si>
+    <t>0.5964±0.009</t>
+  </si>
+  <si>
+    <t>0.4242±0.0095</t>
+  </si>
+  <si>
+    <t>0.8139±0.004</t>
+  </si>
+  <si>
+    <t>0.6136±0.0068</t>
+  </si>
+  <si>
+    <t>0.5129±0.0064</t>
+  </si>
+  <si>
+    <t>0.5044±0.0055</t>
+  </si>
+  <si>
+    <t>0.5351±0.0065</t>
+  </si>
+  <si>
+    <t>0.2742±0.0092</t>
+  </si>
+  <si>
+    <t>0.7209±0.0059</t>
+  </si>
+  <si>
+    <t>0.5193±0.0059</t>
+  </si>
+  <si>
+    <t>0.6065±0.0028</t>
+  </si>
+  <si>
+    <t>0.5164±0.0028</t>
+  </si>
+  <si>
+    <t>0.5309±0.0037</t>
+  </si>
+  <si>
+    <t>0.2871±0.0047</t>
+  </si>
+  <si>
+    <t>0.6482±0.0028</t>
+  </si>
+  <si>
+    <t>0.5235±0.0032</t>
+  </si>
+  <si>
+    <t>0.5448±0.005</t>
+  </si>
+  <si>
+    <t>0.4345±0.0064</t>
+  </si>
+  <si>
+    <t>0.4395±0.0066</t>
+  </si>
+  <si>
+    <t>0.1625±0.0084</t>
+  </si>
+  <si>
+    <t>0.5797±0.005</t>
+  </si>
+  <si>
+    <t>0.437±0.0065</t>
+  </si>
+  <si>
+    <t>0.7124±0.0028</t>
+  </si>
+  <si>
+    <t>0.6518±0.0051</t>
+  </si>
+  <si>
+    <t>0.5524±0.0034</t>
+  </si>
+  <si>
+    <t>0.404±0.0061</t>
+  </si>
+  <si>
+    <t>0.8102±0.0027</t>
+  </si>
+  <si>
+    <t>0.598±0.0037</t>
+  </si>
+  <si>
+    <t>0.6803±0.0027</t>
+  </si>
+  <si>
+    <t>0.6217±0.0074</t>
+  </si>
+  <si>
+    <t>0.4553±0.0036</t>
+  </si>
+  <si>
+    <t>0.2972±0.0078</t>
+  </si>
+  <si>
+    <t>0.763±0.0036</t>
+  </si>
+  <si>
+    <t>0.5256±0.0049</t>
+  </si>
+  <si>
+    <t>0.7481±0.0033</t>
+  </si>
+  <si>
+    <t>0.7223±0.0089</t>
+  </si>
+  <si>
+    <t>0.5946±0.011</t>
+  </si>
+  <si>
+    <t>0.4832±0.0082</t>
+  </si>
+  <si>
+    <t>0.8307±0.0026</t>
+  </si>
+  <si>
+    <t>0.6522±0.0059</t>
+  </si>
+  <si>
+    <t>0.6708±0.0063</t>
+  </si>
+  <si>
+    <t>0.5228±0.0057</t>
+  </si>
+  <si>
+    <t>0.3898±0.0081</t>
+  </si>
+  <si>
+    <t>0.7854±0.0024</t>
+  </si>
+  <si>
+    <t>0.5876±0.0057</t>
+  </si>
+  <si>
+    <t>0.6956±0.0031</t>
+  </si>
+  <si>
+    <t>0.7091±0.0116</t>
+  </si>
+  <si>
+    <t>0.4646±0.0046</t>
+  </si>
+  <si>
+    <t>0.34±0.0094</t>
+  </si>
+  <si>
+    <t>0.7722±0.0034</t>
+  </si>
+  <si>
+    <t>0.5614±0.0062</t>
+  </si>
+  <si>
+    <t>0.6887±0.0025</t>
+  </si>
+  <si>
+    <t>0.7119±0.0198</t>
+  </si>
+  <si>
+    <t>0.4492±0.0042</t>
+  </si>
+  <si>
+    <t>0.3197±0.0083</t>
+  </si>
+  <si>
+    <t>0.7771±0.0133</t>
+  </si>
+  <si>
+    <t>0.5507±0.0061</t>
+  </si>
+  <si>
+    <t>0.7259±0.0034</t>
+  </si>
+  <si>
+    <t>0.6842±0.0072</t>
+  </si>
+  <si>
+    <t>0.5581±0.0047</t>
+  </si>
+  <si>
+    <t>0.4302±0.0079</t>
+  </si>
+  <si>
+    <t>0.8258±0.0032</t>
+  </si>
+  <si>
+    <t>0.6148±0.0057</t>
+  </si>
+  <si>
+    <t>0.7254±0.0033</t>
+  </si>
+  <si>
+    <t>0.6796±0.0071</t>
+  </si>
+  <si>
+    <t>0.5606±0.0051</t>
+  </si>
+  <si>
+    <t>0.4302±0.0077</t>
+  </si>
+  <si>
+    <t>0.8252±0.0028</t>
+  </si>
+  <si>
+    <t>0.6144±0.0058</t>
+  </si>
+  <si>
+    <t>0.7188±0.0058</t>
+  </si>
+  <si>
+    <t>0.651±0.0108</t>
+  </si>
+  <si>
+    <t>0.6031±0.0085</t>
+  </si>
+  <si>
+    <t>0.4416±0.0092</t>
+  </si>
+  <si>
+    <t>0.8261±0.0037</t>
+  </si>
+  <si>
+    <t>0.6261±0.0068</t>
+  </si>
+  <si>
+    <t>0.51±0.0052</t>
+  </si>
+  <si>
+    <t>0.5037±0.0042</t>
+  </si>
+  <si>
+    <t>0.535±0.0053</t>
+  </si>
+  <si>
+    <t>0.2729±0.0067</t>
+  </si>
+  <si>
+    <t>0.7206±0.0056</t>
+  </si>
+  <si>
+    <t>0.5189±0.0045</t>
+  </si>
+  <si>
+    <t>0.6149±0.0031</t>
+  </si>
+  <si>
+    <t>0.5242±0.0037</t>
+  </si>
+  <si>
+    <t>0.5374±0.0043</t>
+  </si>
+  <si>
+    <t>0.2987±0.006</t>
+  </si>
+  <si>
+    <t>0.6531±0.0033</t>
+  </si>
+  <si>
+    <t>0.5307±0.004</t>
+  </si>
+  <si>
+    <t>0.5476±0.0043</t>
+  </si>
+  <si>
+    <t>0.4376±0.0049</t>
+  </si>
+  <si>
+    <t>0.4429±0.0053</t>
+  </si>
+  <si>
+    <t>0.1682±0.0072</t>
+  </si>
+  <si>
+    <t>0.5819±0.004</t>
+  </si>
+  <si>
+    <t>0.4402±0.0051</t>
+  </si>
+  <si>
+    <t>0.7137±0.0026</t>
+  </si>
+  <si>
+    <t>0.6556±0.0053</t>
+  </si>
+  <si>
+    <t>0.4057±0.0063</t>
+  </si>
+  <si>
+    <t>0.8123±0.0028</t>
+  </si>
+  <si>
+    <t>0.5989±0.0047</t>
+  </si>
+  <si>
+    <t>0.6808±0.003</t>
+  </si>
+  <si>
+    <t>0.6236±0.0099</t>
+  </si>
+  <si>
+    <t>0.4542±0.004</t>
+  </si>
+  <si>
+    <t>0.298±0.0086</t>
+  </si>
+  <si>
+    <t>0.7634±0.0036</t>
+  </si>
+  <si>
+    <t>0.5256±0.0059</t>
   </si>
 </sst>
 </file>
@@ -4690,7 +5539,9 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23:L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4761,217 +5612,505 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1172</v>
+      </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="I3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1242</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G4" t="s">
+        <v>407</v>
+      </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="I4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1248</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1183</v>
+      </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="I5" t="s">
+        <v>1249</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1250</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1254</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1189</v>
+      </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="I6" t="s">
+        <v>1255</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1257</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1258</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1259</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1260</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1194</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1195</v>
+      </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="I7" t="s">
+        <v>1261</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1262</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1263</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1264</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1265</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1266</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1200</v>
+      </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="I8" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1269</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1271</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1272</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1206</v>
+      </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="I9" t="s">
+        <v>1273</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1274</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1275</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1276</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1212</v>
+      </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="I10" t="s">
+        <v>1279</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1280</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1281</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1282</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1284</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1218</v>
+      </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="I11" t="s">
+        <v>497</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1286</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1287</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1288</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1289</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="B12" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1224</v>
+      </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="I12" t="s">
+        <v>1290</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1291</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1292</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1293</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1295</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="B13" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1230</v>
+      </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="I13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1299</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1301</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1236</v>
+      </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="I14" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1303</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1304</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1305</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1306</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1307</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7009,7 +8148,7 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10929,7 +12068,9 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11000,217 +12141,505 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1313</v>
+      </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="I3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1385</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1317</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1318</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1319</v>
+      </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="I4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1387</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1390</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1324</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1325</v>
+      </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="I5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1395</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1396</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1331</v>
+      </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="I6" t="s">
+        <v>1397</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1401</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1402</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1335</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1337</v>
+      </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="I7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1404</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1407</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1408</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1343</v>
+      </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="I8" t="s">
+        <v>1409</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1410</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1411</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1412</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1413</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1414</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1346</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1348</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1349</v>
+      </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="I9" t="s">
+        <v>1415</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1416</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1417</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1418</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1419</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1420</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1354</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1355</v>
+      </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="I10" t="s">
+        <v>1421</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1422</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1423</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1426</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1360</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1361</v>
+      </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="I11" t="s">
+        <v>1427</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1429</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1430</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1432</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="B12" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1366</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1367</v>
+      </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="I12" t="s">
+        <v>1433</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1435</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1436</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1438</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="B13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1373</v>
+      </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="I13" t="s">
+        <v>1439</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1440</v>
+      </c>
+      <c r="K13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1441</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1442</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1443</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1379</v>
+      </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="I14" t="s">
+        <v>1444</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1445</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1446</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1448</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1449</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>